<commit_message>
added target values to calibration spreadsheet
</commit_message>
<xml_diff>
--- a/projects/office_calibration.xlsx
+++ b/projects/office_calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="821">
   <si>
     <t>type</t>
   </si>
@@ -2171,12 +2171,6 @@
     <t>kWh</t>
   </si>
   <si>
-    <t>Total Electricity Peak Modeled</t>
-  </si>
-  <si>
-    <t>kW</t>
-  </si>
-  <si>
     <t>Electricity Consumption Period 1 Modeled</t>
   </si>
   <si>
@@ -2207,9 +2201,6 @@
     <t>Electricity Consumption Period 10 Modeled</t>
   </si>
   <si>
-    <t>Electricity Consumption Period 11 Modeled</t>
-  </si>
-  <si>
     <t>Gas Consumption Period 1 Modeled</t>
   </si>
   <si>
@@ -2450,9 +2441,6 @@
     <t>calibration_reports.electric_bill_consumption_modeled</t>
   </si>
   <si>
-    <t>calibration_reports.electric_bill_peak_demand_modeled</t>
-  </si>
-  <si>
     <t>calibration_reports.electric_bill_period_1_consumption_modeled</t>
   </si>
   <si>
@@ -2481,9 +2469,6 @@
   </si>
   <si>
     <t>calibration_reports.electric_bill_period_10_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports.electric_bill_period_11_consumption_modeled</t>
   </si>
   <si>
     <t>calibration_reports.gas_bill_consumption_modeled</t>
@@ -6658,8 +6643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6728,7 +6713,7 @@
         <v>470</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>472</v>
@@ -6799,7 +6784,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -6810,10 +6795,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -6821,10 +6806,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -6942,7 +6927,7 @@
         <v>557</v>
       </c>
       <c r="B26" s="29">
-        <v>450360000000000</v>
+        <v>900360000000000</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>575</v>
@@ -6985,13 +6970,13 @@
     </row>
     <row r="30" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="B30" s="30">
         <v>1</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="D30" s="35"/>
     </row>
@@ -7025,7 +7010,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -7052,7 +7037,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -7078,7 +7063,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7093,7 +7078,7 @@
         <v>702</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7281,13 +7266,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>68</v>
@@ -7300,16 +7285,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -7317,16 +7302,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="38" customFormat="1" x14ac:dyDescent="0.3">
@@ -7362,7 +7347,7 @@
         <v>618</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -7455,13 +7440,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="E13" s="38" t="s">
         <v>68</v>
@@ -7483,7 +7468,7 @@
         <v>64</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="H14" s="30">
         <v>10000</v>
@@ -7537,7 +7522,7 @@
         <v>64</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="H17" s="30">
         <v>10</v>
@@ -7548,10 +7533,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="F18" s="30" t="s">
         <v>64</v>
@@ -7566,10 +7551,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>64</v>
@@ -7584,10 +7569,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="F20" s="30" t="s">
         <v>64</v>
@@ -7602,10 +7587,10 @@
         <v>21</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>64</v>
@@ -7620,10 +7605,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>64</v>
@@ -7638,10 +7623,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>64</v>
@@ -7656,10 +7641,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>64</v>
@@ -7674,10 +7659,10 @@
         <v>21</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>64</v>
@@ -7692,10 +7677,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>64</v>
@@ -7710,10 +7695,10 @@
         <v>21</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>64</v>
@@ -7728,10 +7713,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="F28" s="30" t="s">
         <v>64</v>
@@ -7746,10 +7731,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="F29" s="30" t="s">
         <v>64</v>
@@ -7764,10 +7749,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="F30" s="30" t="s">
         <v>64</v>
@@ -7817,13 +7802,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="E33" s="38" t="s">
         <v>68</v>
@@ -7834,10 +7819,10 @@
         <v>21</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="F34" s="30" t="s">
         <v>64</v>
@@ -7851,19 +7836,19 @@
         <v>21</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="F35" s="30" t="s">
         <v>62</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="I35" s="30" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="36" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -7871,10 +7856,10 @@
         <v>21</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="F36" s="30" t="s">
         <v>64</v>
@@ -8398,7 +8383,7 @@
         <v>1</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="C59" s="30" t="s">
         <v>76</v>
@@ -8415,7 +8400,7 @@
         <v>22</v>
       </c>
       <c r="D60" s="43" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="E60" s="43" t="s">
         <v>77</v>
@@ -8443,7 +8428,7 @@
         <v>0.01</v>
       </c>
       <c r="Q60" s="43" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="61" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -8488,7 +8473,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="C63" s="30" t="s">
         <v>76</v>
@@ -8505,7 +8490,7 @@
         <v>22</v>
       </c>
       <c r="D64" s="43" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="E64" s="43" t="s">
         <v>77</v>
@@ -8533,7 +8518,7 @@
         <v>0.01</v>
       </c>
       <c r="Q64" s="43" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="65" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -8578,7 +8563,7 @@
         <v>1</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C67" s="30" t="s">
         <v>76</v>
@@ -8595,7 +8580,7 @@
         <v>22</v>
       </c>
       <c r="D68" s="43" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="E68" s="43" t="s">
         <v>77</v>
@@ -8623,7 +8608,7 @@
         <v>0.01</v>
       </c>
       <c r="Q68" s="43" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -8707,7 +8692,7 @@
         <v>22</v>
       </c>
       <c r="D73" s="44" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="E73" s="43" t="s">
         <v>70</v>
@@ -8735,7 +8720,7 @@
         <v>2.5</v>
       </c>
       <c r="Q73" s="43" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -8854,7 +8839,7 @@
         <v>22</v>
       </c>
       <c r="D79" s="43" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="E79" s="43" t="s">
         <v>46</v>
@@ -9629,11 +9614,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9858,7 +9843,7 @@
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>710</v>
@@ -9875,7 +9860,9 @@
       <c r="H8" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I8" s="30"/>
+      <c r="I8" s="30">
+        <v>39359</v>
+      </c>
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -9886,10 +9873,10 @@
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="30" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>64</v>
@@ -9901,20 +9888,22 @@
         <v>1</v>
       </c>
       <c r="H9" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="30"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="30">
+        <v>4153</v>
+      </c>
       <c r="J9" s="30"/>
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="30" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>710</v>
@@ -9931,18 +9920,20 @@
       <c r="H10" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I10" s="30"/>
+      <c r="I10" s="30">
+        <v>3732</v>
+      </c>
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>710</v>
@@ -9959,18 +9950,20 @@
       <c r="H11" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I11" s="30"/>
+      <c r="I11" s="30">
+        <v>3884</v>
+      </c>
       <c r="J11" s="30"/>
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>710</v>
@@ -9987,18 +9980,20 @@
       <c r="H12" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="30"/>
+      <c r="I12" s="30">
+        <v>3708</v>
+      </c>
       <c r="J12" s="30"/>
       <c r="K12" s="30"/>
       <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>710</v>
@@ -10015,18 +10010,20 @@
       <c r="H13" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="30"/>
+      <c r="I13" s="30">
+        <v>4009</v>
+      </c>
       <c r="J13" s="30"/>
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="30" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>710</v>
@@ -10043,18 +10040,20 @@
       <c r="H14" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="30"/>
+      <c r="I14" s="30">
+        <v>5042</v>
+      </c>
       <c r="J14" s="30"/>
       <c r="K14" s="30"/>
       <c r="L14" s="30"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="30" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>710</v>
@@ -10071,18 +10070,20 @@
       <c r="H15" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I15" s="30"/>
+      <c r="I15" s="30">
+        <v>4616</v>
+      </c>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B16" s="30"/>
       <c r="C16" s="30" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>710</v>
@@ -10099,18 +10100,20 @@
       <c r="H16" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I16" s="30"/>
+      <c r="I16" s="30">
+        <v>3115</v>
+      </c>
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="30" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>710</v>
@@ -10127,18 +10130,20 @@
       <c r="H17" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I17" s="30"/>
+      <c r="I17" s="30">
+        <v>3357</v>
+      </c>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="30" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>710</v>
@@ -10155,7 +10160,9 @@
       <c r="H18" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I18" s="30"/>
+      <c r="I18" s="30">
+        <v>3743</v>
+      </c>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
@@ -10166,10 +10173,10 @@
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="30" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>710</v>
+        <v>723</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>64</v>
@@ -10183,21 +10190,23 @@
       <c r="H19" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I19" s="30"/>
+      <c r="I19" s="30">
+        <v>2659</v>
+      </c>
       <c r="J19" s="30"/>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B20" s="30"/>
       <c r="C20" s="30" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>710</v>
+        <v>723</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>64</v>
@@ -10209,23 +10218,25 @@
         <v>1</v>
       </c>
       <c r="H20" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="30"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="30">
+        <v>1038</v>
+      </c>
       <c r="J20" s="30"/>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="30" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E21" s="30" t="s">
         <v>64</v>
@@ -10239,21 +10250,23 @@
       <c r="H21" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I21" s="30"/>
+      <c r="I21" s="30">
+        <v>724</v>
+      </c>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="30" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E22" s="30" t="s">
         <v>64</v>
@@ -10267,21 +10280,23 @@
       <c r="H22" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I22" s="30"/>
+      <c r="I22" s="30">
+        <v>297</v>
+      </c>
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="30" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E23" s="30" t="s">
         <v>64</v>
@@ -10295,21 +10310,23 @@
       <c r="H23" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I23" s="30"/>
+      <c r="I23" s="30">
+        <v>71</v>
+      </c>
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="30" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E24" s="30" t="s">
         <v>64</v>
@@ -10323,21 +10340,23 @@
       <c r="H24" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I24" s="30"/>
+      <c r="I24" s="30">
+        <v>14</v>
+      </c>
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="30" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E25" s="30" t="s">
         <v>64</v>
@@ -10351,21 +10370,23 @@
       <c r="H25" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I25" s="30"/>
+      <c r="I25" s="30">
+        <v>1</v>
+      </c>
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="30" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>64</v>
@@ -10379,21 +10400,23 @@
       <c r="H26" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I26" s="30"/>
+      <c r="I26" s="30">
+        <v>0</v>
+      </c>
       <c r="J26" s="30"/>
       <c r="K26" s="30"/>
       <c r="L26" s="30"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B27" s="30"/>
       <c r="C27" s="30" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E27" s="30" t="s">
         <v>64</v>
@@ -10407,21 +10430,23 @@
       <c r="H27" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I27" s="30"/>
+      <c r="I27" s="30">
+        <v>22</v>
+      </c>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B28" s="30"/>
       <c r="C28" s="30" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E28" s="30" t="s">
         <v>64</v>
@@ -10435,66 +10460,24 @@
       <c r="H28" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="I28" s="30"/>
+      <c r="I28" s="30">
+        <v>72</v>
+      </c>
       <c r="J28" s="30"/>
       <c r="K28" s="30"/>
       <c r="L28" s="30"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="30" t="s">
-        <v>733</v>
-      </c>
+      <c r="A29" s="30"/>
       <c r="B29" s="30"/>
-      <c r="C29" s="30" t="s">
-        <v>824</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="30" t="s">
-        <v>734</v>
-      </c>
+      <c r="A30" s="30"/>
       <c r="B30" s="30"/>
-      <c r="C30" s="30" t="s">
-        <v>825</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>726</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="30"/>
@@ -10531,18 +10514,6 @@
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
       <c r="D36" s="30"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
changed run period dates
</commit_message>
<xml_diff>
--- a/projects/office_calibration.xlsx
+++ b/projects/office_calibration.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="13180" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2140,12 +2140,6 @@
     <t>End date</t>
   </si>
   <si>
-    <t>2013-12-21</t>
-  </si>
-  <si>
-    <t>2013-01-21</t>
-  </si>
-  <si>
     <t>calibration_data</t>
   </si>
   <si>
@@ -2591,6 +2585,12 @@
   </si>
   <si>
     <t>DOE Ref 1980-2004</t>
+  </si>
+  <si>
+    <t>2013-01-10</t>
+  </si>
+  <si>
+    <t>2013-12-12</t>
   </si>
 </sst>
 </file>
@@ -2600,7 +2600,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4705,10 +4705,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1836">
     <cellStyle name="Comma" xfId="1749" builtinId="3"/>
@@ -6851,17 +6851,17 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="81.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="28">
+    <row r="1" spans="1:1" ht="28.8">
       <c r="A1" s="36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="28">
+    <row r="2" spans="1:1" ht="28.8">
       <c r="A2" s="36" t="s">
         <v>41</v>
       </c>
@@ -6881,16 +6881,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="33.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="61.6640625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.6640625" style="1"/>
   </cols>
@@ -6924,7 +6924,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28">
+    <row r="4" spans="1:5" ht="28.8">
       <c r="A4" s="1" t="s">
         <v>456</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="42">
+    <row r="5" spans="1:5" ht="72">
       <c r="A5" s="1" t="s">
         <v>469</v>
       </c>
@@ -6946,18 +6946,18 @@
         <v>614</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="46.25" customHeight="1">
+    <row r="6" spans="1:5" ht="46.2" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>470</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="28.8">
       <c r="A7" s="1" t="s">
         <v>442</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="1" t="s">
         <v>443</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -7033,10 +7033,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -7044,10 +7044,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -7061,7 +7061,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="1" t="s">
         <v>463</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="57.6">
       <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
@@ -7119,7 +7119,7 @@
       <c r="B22" s="26"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="57.6">
       <c r="A23" s="11" t="s">
         <v>450</v>
       </c>
@@ -7208,13 +7208,13 @@
     </row>
     <row r="30" spans="1:5" s="31" customFormat="1">
       <c r="A30" s="31" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B30" s="30">
         <v>1</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D30" s="35"/>
     </row>
@@ -7243,12 +7243,12 @@
       <c r="C35" s="26"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="43.2">
       <c r="A36" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -7261,10 +7261,10 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="28">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8">
       <c r="A39" s="11" t="s">
         <v>30</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -7293,7 +7293,7 @@
       </c>
       <c r="E40" s="2"/>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="57.6">
       <c r="A42" s="11" t="s">
         <v>35</v>
       </c>
@@ -7301,7 +7301,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7310,13 +7310,13 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="31" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1">
@@ -7349,34 +7349,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y224"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:H30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H57" sqref="H57:H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="31" customWidth="1"/>
     <col min="2" max="2" width="47" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="31" customWidth="1"/>
-    <col min="4" max="4" width="39.1640625" style="31" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" style="31" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" style="31" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="31" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="4" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" style="31" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" style="31" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" style="31" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" style="31" customWidth="1"/>
     <col min="12" max="12" width="6.6640625" style="31" customWidth="1"/>
     <col min="13" max="14" width="7.6640625" style="31" customWidth="1"/>
-    <col min="15" max="15" width="11.5" style="31"/>
-    <col min="16" max="16" width="11.5" style="31" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" style="31"/>
+    <col min="16" max="16" width="11.44140625" style="31" customWidth="1"/>
     <col min="17" max="17" width="23" style="31" customWidth="1"/>
     <col min="18" max="18" width="27.6640625" style="31" customWidth="1"/>
-    <col min="19" max="19" width="46.1640625" style="31" customWidth="1"/>
-    <col min="20" max="22" width="11.5" style="31"/>
+    <col min="19" max="19" width="46.109375" style="31" customWidth="1"/>
+    <col min="20" max="22" width="11.44140625" style="31"/>
     <col min="23" max="23" width="13.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="11.5" style="31"/>
+    <col min="24" max="16384" width="11.44140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18">
@@ -7405,16 +7405,16 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="52" t="s">
+      <c r="T1" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-    </row>
-    <row r="2" spans="1:25" s="8" customFormat="1" ht="15">
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+    </row>
+    <row r="2" spans="1:25" s="8" customFormat="1" ht="15.6">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -7430,7 +7430,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:25" s="14" customFormat="1" ht="45">
+    <row r="3" spans="1:25" s="14" customFormat="1" ht="62.4">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -7509,13 +7509,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>68</v>
@@ -7528,16 +7528,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="30" customFormat="1">
@@ -7545,16 +7545,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="38" customFormat="1">
@@ -7590,7 +7590,7 @@
         <v>618</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -7615,7 +7615,7 @@
         <v>618</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -7683,13 +7683,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E13" s="38" t="s">
         <v>68</v>
@@ -7697,7 +7697,7 @@
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
     </row>
-    <row r="14" spans="1:25" ht="17">
+    <row r="14" spans="1:25" ht="17.399999999999999">
       <c r="A14" s="30"/>
       <c r="B14" s="30" t="s">
         <v>21</v>
@@ -7713,9 +7713,9 @@
         <v>64</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>765</v>
-      </c>
-      <c r="H14" s="53">
+        <v>763</v>
+      </c>
+      <c r="H14" s="52">
         <v>104666</v>
       </c>
       <c r="I14" s="31"/>
@@ -7753,7 +7753,7 @@
         <v>0.1</v>
       </c>
       <c r="Q15" s="51" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="16" spans="1:25" s="30" customFormat="1">
@@ -7787,7 +7787,7 @@
         <v>64</v>
       </c>
       <c r="G17" s="43" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="H17" s="43">
         <v>12</v>
@@ -7809,7 +7809,7 @@
         <v>0.1</v>
       </c>
       <c r="Q17" s="51" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="30" customFormat="1">
@@ -7817,10 +7817,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F18" s="30" t="s">
         <v>64</v>
@@ -7834,10 +7834,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>64</v>
@@ -7851,10 +7851,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F20" s="30" t="s">
         <v>64</v>
@@ -7868,10 +7868,10 @@
         <v>21</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>64</v>
@@ -7885,10 +7885,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>64</v>
@@ -7902,10 +7902,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>64</v>
@@ -7919,10 +7919,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>64</v>
@@ -7936,10 +7936,10 @@
         <v>21</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>64</v>
@@ -7953,10 +7953,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>64</v>
@@ -7970,10 +7970,10 @@
         <v>21</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>64</v>
@@ -7987,10 +7987,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F28" s="30" t="s">
         <v>64</v>
@@ -8004,10 +8004,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="F29" s="30" t="s">
         <v>64</v>
@@ -8021,10 +8021,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="F30" s="30" t="s">
         <v>64</v>
@@ -8073,13 +8073,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="E33" s="38" t="s">
         <v>68</v>
@@ -8092,10 +8092,10 @@
         <v>22</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F34" s="43" t="s">
         <v>64</v>
@@ -8120,7 +8120,7 @@
         <v>0.01</v>
       </c>
       <c r="Q34" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="43" customFormat="1">
@@ -8128,10 +8128,10 @@
         <v>22</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F35" s="43" t="s">
         <v>64</v>
@@ -8156,7 +8156,7 @@
         <v>0.01</v>
       </c>
       <c r="Q35" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="36" spans="1:17" s="38" customFormat="1">
@@ -8164,7 +8164,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C36" s="38" t="s">
         <v>74</v>
@@ -8183,7 +8183,7 @@
         <v>22</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E37" s="43" t="s">
         <v>75</v>
@@ -8192,7 +8192,7 @@
         <v>619</v>
       </c>
       <c r="G37" s="43" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="H37" s="43">
         <v>0</v>
@@ -8214,7 +8214,7 @@
         <v>5</v>
       </c>
       <c r="Q37" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="38" customFormat="1">
@@ -8271,7 +8271,7 @@
       </c>
       <c r="P39" s="40"/>
       <c r="Q39" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -8378,7 +8378,7 @@
       </c>
       <c r="P43" s="40"/>
       <c r="Q43" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -8485,7 +8485,7 @@
       </c>
       <c r="P47" s="40"/>
       <c r="Q47" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -8592,7 +8592,7 @@
       </c>
       <c r="P51" s="40"/>
       <c r="Q51" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -8678,7 +8678,7 @@
         <v>618</v>
       </c>
       <c r="H55" s="31" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="I55" s="31"/>
     </row>
@@ -8696,7 +8696,7 @@
         <v>618</v>
       </c>
       <c r="H56" s="31" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="I56" s="31"/>
     </row>
@@ -8714,7 +8714,7 @@
         <v>618</v>
       </c>
       <c r="H57" s="41" t="s">
-        <v>700</v>
+        <v>848</v>
       </c>
       <c r="I57" s="31"/>
     </row>
@@ -8732,7 +8732,7 @@
         <v>618</v>
       </c>
       <c r="H58" s="41" t="s">
-        <v>699</v>
+        <v>849</v>
       </c>
       <c r="I58" s="31"/>
     </row>
@@ -8741,13 +8741,13 @@
         <v>1</v>
       </c>
       <c r="B59" s="38" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="E59" s="38" t="s">
         <v>233</v>
@@ -8760,7 +8760,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="49" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C60" s="49" t="s">
         <v>76</v>
@@ -8777,7 +8777,7 @@
         <v>22</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E61" s="43" t="s">
         <v>77</v>
@@ -8805,7 +8805,7 @@
         <v>0.01</v>
       </c>
       <c r="Q61" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="30" customFormat="1">
@@ -8850,7 +8850,7 @@
         <v>1</v>
       </c>
       <c r="B64" s="49" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C64" s="49" t="s">
         <v>76</v>
@@ -8867,7 +8867,7 @@
         <v>22</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E65" s="43" t="s">
         <v>77</v>
@@ -8895,7 +8895,7 @@
         <v>0.01</v>
       </c>
       <c r="Q65" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="66" spans="1:17" s="30" customFormat="1">
@@ -8940,7 +8940,7 @@
         <v>1</v>
       </c>
       <c r="B68" s="49" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C68" s="49" t="s">
         <v>76</v>
@@ -8957,7 +8957,7 @@
         <v>22</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E69" s="43" t="s">
         <v>77</v>
@@ -8985,7 +8985,7 @@
         <v>0.01</v>
       </c>
       <c r="Q69" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="30" customFormat="1">
@@ -9068,7 +9068,7 @@
         <v>22</v>
       </c>
       <c r="D74" s="44" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E74" s="43" t="s">
         <v>70</v>
@@ -9096,7 +9096,7 @@
         <v>2.5</v>
       </c>
       <c r="Q74" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="30" customFormat="1">
@@ -9204,7 +9204,7 @@
         <v>22</v>
       </c>
       <c r="D80" s="43" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E80" s="43" t="s">
         <v>46</v>
@@ -9470,7 +9470,7 @@
         <v>22</v>
       </c>
       <c r="D90" s="43" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="E90" s="43" t="s">
         <v>330</v>
@@ -9499,7 +9499,7 @@
         <v>2.5</v>
       </c>
       <c r="Q90" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="91" spans="1:17" s="50" customFormat="1">
@@ -9507,13 +9507,13 @@
         <v>1</v>
       </c>
       <c r="B91" s="50" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C91" s="50" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="D91" s="50" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E91" s="50" t="s">
         <v>68</v>
@@ -9524,7 +9524,7 @@
         <v>22</v>
       </c>
       <c r="D92" s="43" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="E92" s="43" t="s">
         <v>258</v>
@@ -9553,7 +9553,7 @@
         <v>2.5</v>
       </c>
       <c r="Q92" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="93" spans="1:17" s="50" customFormat="1">
@@ -9561,13 +9561,13 @@
         <v>1</v>
       </c>
       <c r="B93" s="50" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C93" s="50" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D93" s="50" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E93" s="50" t="s">
         <v>68</v>
@@ -9578,7 +9578,7 @@
         <v>22</v>
       </c>
       <c r="D94" s="43" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="E94" s="43" t="s">
         <v>258</v>
@@ -9607,7 +9607,7 @@
         <v>2.5</v>
       </c>
       <c r="Q94" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="95" spans="1:17" s="50" customFormat="1">
@@ -9652,7 +9652,7 @@
         <v>22</v>
       </c>
       <c r="D97" s="43" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="E97" s="43" t="s">
         <v>288</v>
@@ -9661,7 +9661,7 @@
         <v>64</v>
       </c>
       <c r="G97" s="43" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="H97" s="43">
         <v>0</v>
@@ -9684,7 +9684,7 @@
         <v>2.5</v>
       </c>
       <c r="Q97" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="98" spans="1:17" s="30" customFormat="1">
@@ -9692,7 +9692,7 @@
         <v>21</v>
       </c>
       <c r="D98" s="30" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="E98" s="30" t="s">
         <v>48</v>
@@ -9701,7 +9701,7 @@
         <v>64</v>
       </c>
       <c r="G98" s="30" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="H98" s="30">
         <v>0</v>
@@ -9712,7 +9712,7 @@
         <v>21</v>
       </c>
       <c r="D99" s="30" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="E99" s="30" t="s">
         <v>50</v>
@@ -9721,7 +9721,7 @@
         <v>64</v>
       </c>
       <c r="G99" s="30" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="H99" s="30">
         <v>0</v>
@@ -9732,7 +9732,7 @@
         <v>21</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="E100" s="30" t="s">
         <v>52</v>
@@ -9741,7 +9741,7 @@
         <v>65</v>
       </c>
       <c r="G100" s="30" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="H100" s="30">
         <v>0</v>
@@ -9752,7 +9752,7 @@
         <v>21</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="E101" s="30" t="s">
         <v>54</v>
@@ -9769,7 +9769,7 @@
         <v>21</v>
       </c>
       <c r="D102" s="30" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="E102" s="30" t="s">
         <v>56</v>
@@ -9778,7 +9778,7 @@
         <v>65</v>
       </c>
       <c r="G102" s="30" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="H102" s="30">
         <v>15</v>
@@ -9789,7 +9789,7 @@
         <v>21</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="E103" s="30" t="s">
         <v>58</v>
@@ -9798,7 +9798,7 @@
         <v>64</v>
       </c>
       <c r="G103" s="30" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="H103" s="30">
         <v>0</v>
@@ -9809,7 +9809,7 @@
         <v>21</v>
       </c>
       <c r="D104" s="30" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E104" s="30" t="s">
         <v>60</v>
@@ -9818,7 +9818,7 @@
         <v>65</v>
       </c>
       <c r="G104" s="30" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="H104" s="30">
         <v>1</v>
@@ -9832,10 +9832,10 @@
         <v>187</v>
       </c>
       <c r="C105" s="38" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="D105" s="38" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="E105" s="38" t="s">
         <v>68</v>
@@ -9848,7 +9848,7 @@
         <v>22</v>
       </c>
       <c r="D106" s="43" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="E106" s="43" t="s">
         <v>190</v>
@@ -9857,7 +9857,7 @@
         <v>64</v>
       </c>
       <c r="G106" s="43" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="H106" s="43">
         <v>1</v>
@@ -9880,7 +9880,7 @@
         <v>1</v>
       </c>
       <c r="Q106" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="107" spans="1:17" s="43" customFormat="1">
@@ -9888,7 +9888,7 @@
         <v>22</v>
       </c>
       <c r="D107" s="43" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="E107" s="43" t="s">
         <v>192</v>
@@ -9897,7 +9897,7 @@
         <v>64</v>
       </c>
       <c r="G107" s="43" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="H107" s="43">
         <v>-1</v>
@@ -9920,7 +9920,7 @@
         <v>1</v>
       </c>
       <c r="Q107" s="43" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="108" spans="1:17">
@@ -9928,7 +9928,7 @@
         <v>21</v>
       </c>
       <c r="D108" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E108" s="31" t="s">
         <v>194</v>
@@ -10433,17 +10433,17 @@
       <selection pane="bottomLeft" activeCell="A29" sqref="A29:A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="29.5" style="31" customWidth="1"/>
+    <col min="1" max="2" width="29.44140625" style="31" customWidth="1"/>
     <col min="3" max="3" width="71" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="31" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="31" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5" style="31" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="31" customWidth="1"/>
+    <col min="6" max="7" width="10.44140625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="31" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" style="31" customWidth="1"/>
     <col min="10" max="10" width="9.6640625" style="31" customWidth="1"/>
-    <col min="11" max="16384" width="11.5" style="31"/>
+    <col min="11" max="16384" width="11.44140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18">
@@ -10461,7 +10461,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="15">
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="15.6">
       <c r="A2" s="8" t="s">
         <v>459</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="30">
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="46.8">
       <c r="A3" s="14" t="s">
         <v>628</v>
       </c>
@@ -10651,14 +10651,14 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="30" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>64</v>
@@ -10682,14 +10682,14 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="30" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="30" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E9" s="30" t="s">
         <v>64</v>
@@ -10712,14 +10712,14 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="30" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="30" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E10" s="30" t="s">
         <v>64</v>
@@ -10742,14 +10742,14 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="30" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E11" s="30" t="s">
         <v>64</v>
@@ -10772,14 +10772,14 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="30" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>64</v>
@@ -10802,14 +10802,14 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="30" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>64</v>
@@ -10832,14 +10832,14 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="30" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="30" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>64</v>
@@ -10862,14 +10862,14 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="30" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="30" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>64</v>
@@ -10892,14 +10892,14 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="30" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B16" s="30"/>
       <c r="C16" s="30" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>64</v>
@@ -10922,14 +10922,14 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="30" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="30" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E17" s="30" t="s">
         <v>64</v>
@@ -10952,14 +10952,14 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="30" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="30" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>64</v>
@@ -10982,14 +10982,14 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="30" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="30" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E19" s="30" t="s">
         <v>64</v>
@@ -11013,14 +11013,14 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="30" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B20" s="30"/>
       <c r="C20" s="30" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>64</v>
@@ -11043,14 +11043,14 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="30" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="30" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E21" s="30" t="s">
         <v>64</v>
@@ -11073,14 +11073,14 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="30" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="30" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E22" s="30" t="s">
         <v>64</v>
@@ -11103,14 +11103,14 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="30" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="30" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E23" s="30" t="s">
         <v>64</v>
@@ -11133,14 +11133,14 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="30" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="30" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E24" s="30" t="s">
         <v>64</v>
@@ -11163,14 +11163,14 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="30" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="30" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E25" s="30" t="s">
         <v>64</v>
@@ -11193,14 +11193,14 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="30" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="30" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>64</v>
@@ -11223,14 +11223,14 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="30" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B27" s="30"/>
       <c r="C27" s="30" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E27" s="30" t="s">
         <v>64</v>
@@ -11253,14 +11253,14 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="30" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B28" s="30"/>
       <c r="C28" s="30" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E28" s="30" t="s">
         <v>64</v>
@@ -11283,14 +11283,14 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="30" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="30" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E29" s="31" t="s">
         <v>64</v>
@@ -11307,14 +11307,14 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="30" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B30" s="30"/>
       <c r="C30" s="30" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>64</v>
@@ -11331,14 +11331,14 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="30" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B31" s="30"/>
       <c r="C31" s="30" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E31" s="31" t="s">
         <v>64</v>
@@ -11355,14 +11355,14 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="30" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B32" s="30"/>
       <c r="C32" s="30" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E32" s="31" t="s">
         <v>64</v>
@@ -11420,19 +11420,19 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.6">
       <c r="A1" s="17" t="b">
         <v>0</v>
       </c>
@@ -11451,7 +11451,7 @@
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="17"/>
       <c r="B2" s="17" t="s">
         <v>21</v>
@@ -11472,7 +11472,7 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="15.6">
       <c r="A3" s="17"/>
       <c r="B3" s="17" t="s">
         <v>21</v>
@@ -11495,7 +11495,7 @@
       </c>
       <c r="I3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="15.6">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>21</v>
@@ -11518,7 +11518,7 @@
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:9" ht="15.6">
       <c r="A5" s="17"/>
       <c r="B5" s="17" t="s">
         <v>21</v>
@@ -11541,7 +11541,7 @@
       </c>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:9" ht="15.6">
       <c r="A6" s="17"/>
       <c r="B6" s="17" t="s">
         <v>21</v>
@@ -11564,7 +11564,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:9" ht="15.6">
       <c r="A7" s="17"/>
       <c r="B7" s="17" t="s">
         <v>21</v>
@@ -11587,7 +11587,7 @@
       </c>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" ht="15">
+    <row r="8" spans="1:9" ht="15.6">
       <c r="A8" s="17"/>
       <c r="B8" s="17" t="s">
         <v>21</v>
@@ -11610,7 +11610,7 @@
       </c>
       <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:9" ht="15.6">
       <c r="A9" s="17"/>
       <c r="B9" s="17" t="s">
         <v>21</v>
@@ -11633,7 +11633,7 @@
       </c>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="15.6">
       <c r="A10" s="17"/>
       <c r="B10" s="17" t="s">
         <v>21</v>
@@ -11656,7 +11656,7 @@
       </c>
       <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="1:9" ht="15">
+    <row r="11" spans="1:9" ht="15.6">
       <c r="A11" s="17" t="b">
         <v>0</v>
       </c>
@@ -11675,7 +11675,7 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="15">
+    <row r="12" spans="1:9" ht="15.6">
       <c r="A12" s="17"/>
       <c r="B12" s="17" t="s">
         <v>21</v>
@@ -11696,7 +11696,7 @@
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:9" ht="15.6">
       <c r="A13" s="17"/>
       <c r="B13" s="17" t="s">
         <v>21</v>
@@ -11719,7 +11719,7 @@
       </c>
       <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:9" ht="15.6">
       <c r="A14" s="17"/>
       <c r="B14" s="17" t="s">
         <v>21</v>
@@ -11742,7 +11742,7 @@
       </c>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:9" ht="15">
+    <row r="15" spans="1:9" ht="15.6">
       <c r="A15" s="17"/>
       <c r="B15" s="17" t="s">
         <v>21</v>
@@ -11765,7 +11765,7 @@
       </c>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="15">
+    <row r="16" spans="1:9" ht="15.6">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
         <v>21</v>
@@ -11788,7 +11788,7 @@
       </c>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" ht="15">
+    <row r="17" spans="1:9" ht="15.6">
       <c r="A17" s="17"/>
       <c r="B17" s="17" t="s">
         <v>21</v>
@@ -11811,7 +11811,7 @@
       </c>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" ht="15">
+    <row r="18" spans="1:9" ht="15.6">
       <c r="A18" s="17"/>
       <c r="B18" s="17" t="s">
         <v>21</v>
@@ -11834,7 +11834,7 @@
       </c>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="15">
+    <row r="19" spans="1:9" ht="15.6">
       <c r="A19" s="17"/>
       <c r="B19" s="17" t="s">
         <v>21</v>
@@ -11857,7 +11857,7 @@
       </c>
       <c r="I19" s="17"/>
     </row>
-    <row r="20" spans="1:9" ht="15">
+    <row r="20" spans="1:9" ht="15.6">
       <c r="A20" s="17"/>
       <c r="B20" s="17" t="s">
         <v>21</v>
@@ -11880,7 +11880,7 @@
       </c>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" ht="15">
+    <row r="21" spans="1:9" ht="15.6">
       <c r="A21" s="17" t="b">
         <v>0</v>
       </c>
@@ -11899,7 +11899,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" ht="15">
+    <row r="22" spans="1:9" ht="15.6">
       <c r="A22" s="17"/>
       <c r="B22" s="17" t="s">
         <v>21</v>
@@ -11922,7 +11922,7 @@
       </c>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" ht="15">
+    <row r="23" spans="1:9" ht="15.6">
       <c r="A23" s="17"/>
       <c r="B23" s="17" t="s">
         <v>21</v>
@@ -11945,7 +11945,7 @@
       </c>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" ht="15">
+    <row r="24" spans="1:9" ht="15.6">
       <c r="A24" s="17"/>
       <c r="B24" s="17" t="s">
         <v>21</v>
@@ -11968,7 +11968,7 @@
       </c>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="15">
+    <row r="25" spans="1:9" ht="15.6">
       <c r="A25" s="17"/>
       <c r="B25" s="17" t="s">
         <v>21</v>
@@ -11991,7 +11991,7 @@
       </c>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="1:9" ht="15">
+    <row r="26" spans="1:9" ht="15.6">
       <c r="A26" s="17"/>
       <c r="B26" s="17" t="s">
         <v>21</v>
@@ -12014,7 +12014,7 @@
       </c>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" ht="15">
+    <row r="27" spans="1:9" ht="15.6">
       <c r="A27" s="17"/>
       <c r="B27" s="17" t="s">
         <v>21</v>
@@ -12037,7 +12037,7 @@
       </c>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="15">
+    <row r="28" spans="1:9" ht="15.6">
       <c r="A28" s="17"/>
       <c r="B28" s="17" t="s">
         <v>21</v>
@@ -12060,7 +12060,7 @@
       </c>
       <c r="I28" s="17"/>
     </row>
-    <row r="29" spans="1:9" ht="15">
+    <row r="29" spans="1:9" ht="15.6">
       <c r="A29" s="17"/>
       <c r="B29" s="17" t="s">
         <v>21</v>
@@ -12083,7 +12083,7 @@
       </c>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="1:9" ht="15">
+    <row r="30" spans="1:9" ht="15.6">
       <c r="A30" s="17"/>
       <c r="B30" s="17" t="s">
         <v>21</v>
@@ -12106,7 +12106,7 @@
       </c>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" spans="1:9" ht="15">
+    <row r="31" spans="1:9" ht="15.6">
       <c r="A31" s="17" t="b">
         <v>0</v>
       </c>
@@ -12125,7 +12125,7 @@
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
     </row>
-    <row r="32" spans="1:9" ht="15">
+    <row r="32" spans="1:9" ht="15.6">
       <c r="A32" s="17"/>
       <c r="B32" s="17" t="s">
         <v>21</v>
@@ -12146,7 +12146,7 @@
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
     </row>
-    <row r="33" spans="1:9" ht="15">
+    <row r="33" spans="1:9" ht="15.6">
       <c r="A33" s="17"/>
       <c r="B33" s="17" t="s">
         <v>21</v>
@@ -12169,7 +12169,7 @@
       </c>
       <c r="I33" s="17"/>
     </row>
-    <row r="34" spans="1:9" ht="15">
+    <row r="34" spans="1:9" ht="15.6">
       <c r="A34" s="17"/>
       <c r="B34" s="17" t="s">
         <v>21</v>
@@ -12192,7 +12192,7 @@
       </c>
       <c r="I34" s="17"/>
     </row>
-    <row r="35" spans="1:9" ht="15">
+    <row r="35" spans="1:9" ht="15.6">
       <c r="A35" s="17"/>
       <c r="B35" s="17" t="s">
         <v>21</v>
@@ -12215,7 +12215,7 @@
       </c>
       <c r="I35" s="17"/>
     </row>
-    <row r="36" spans="1:9" ht="15">
+    <row r="36" spans="1:9" ht="15.6">
       <c r="A36" s="17"/>
       <c r="B36" s="17" t="s">
         <v>21</v>
@@ -12238,7 +12238,7 @@
       </c>
       <c r="I36" s="17"/>
     </row>
-    <row r="37" spans="1:9" ht="15">
+    <row r="37" spans="1:9" ht="15.6">
       <c r="A37" s="17"/>
       <c r="B37" s="17" t="s">
         <v>21</v>
@@ -12261,7 +12261,7 @@
       </c>
       <c r="I37" s="17"/>
     </row>
-    <row r="38" spans="1:9" ht="15">
+    <row r="38" spans="1:9" ht="15.6">
       <c r="A38" s="17"/>
       <c r="B38" s="17" t="s">
         <v>21</v>
@@ -12284,7 +12284,7 @@
       </c>
       <c r="I38" s="17"/>
     </row>
-    <row r="39" spans="1:9" ht="15">
+    <row r="39" spans="1:9" ht="15.6">
       <c r="A39" s="17"/>
       <c r="B39" s="17" t="s">
         <v>21</v>
@@ -12307,7 +12307,7 @@
       </c>
       <c r="I39" s="17"/>
     </row>
-    <row r="40" spans="1:9" ht="15">
+    <row r="40" spans="1:9" ht="15.6">
       <c r="A40" s="17"/>
       <c r="B40" s="17" t="s">
         <v>21</v>
@@ -12330,7 +12330,7 @@
       </c>
       <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="1:9" ht="15">
+    <row r="41" spans="1:9" ht="15.6">
       <c r="A41" s="17" t="b">
         <v>0</v>
       </c>
@@ -12349,7 +12349,7 @@
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="1:9" ht="15">
+    <row r="42" spans="1:9" ht="15.6">
       <c r="A42" s="17"/>
       <c r="B42" s="17" t="s">
         <v>21</v>
@@ -12370,7 +12370,7 @@
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" ht="15">
+    <row r="43" spans="1:9" ht="15.6">
       <c r="A43" s="17"/>
       <c r="B43" s="17" t="s">
         <v>21</v>
@@ -12393,7 +12393,7 @@
       </c>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" ht="15">
+    <row r="44" spans="1:9" ht="15.6">
       <c r="A44" s="17"/>
       <c r="B44" s="17" t="s">
         <v>21</v>
@@ -12416,7 +12416,7 @@
       </c>
       <c r="I44" s="17"/>
     </row>
-    <row r="45" spans="1:9" ht="15">
+    <row r="45" spans="1:9" ht="15.6">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>21</v>
@@ -12439,7 +12439,7 @@
       </c>
       <c r="I45" s="17"/>
     </row>
-    <row r="46" spans="1:9" ht="15">
+    <row r="46" spans="1:9" ht="15.6">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
         <v>21</v>
@@ -12462,7 +12462,7 @@
       </c>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="1:9" ht="15">
+    <row r="47" spans="1:9" ht="15.6">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
         <v>21</v>
@@ -12485,7 +12485,7 @@
       </c>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="1:9" ht="15">
+    <row r="48" spans="1:9" ht="15.6">
       <c r="A48" s="17"/>
       <c r="B48" s="17" t="s">
         <v>21</v>
@@ -12508,7 +12508,7 @@
       </c>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" ht="15">
+    <row r="49" spans="1:9" ht="15.6">
       <c r="A49" s="17"/>
       <c r="B49" s="17" t="s">
         <v>21</v>
@@ -12531,7 +12531,7 @@
       </c>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="1:9" ht="15">
+    <row r="50" spans="1:9" ht="15.6">
       <c r="A50" s="17"/>
       <c r="B50" s="17" t="s">
         <v>21</v>
@@ -12554,7 +12554,7 @@
       </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="15">
+    <row r="51" spans="1:9" ht="15.6">
       <c r="A51" s="17" t="b">
         <v>0</v>
       </c>
@@ -12573,7 +12573,7 @@
       <c r="H51" s="17"/>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="15">
+    <row r="52" spans="1:9" ht="15.6">
       <c r="A52" s="17"/>
       <c r="B52" s="17" t="s">
         <v>21</v>
@@ -12594,7 +12594,7 @@
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="15">
+    <row r="53" spans="1:9" ht="15.6">
       <c r="A53" s="17"/>
       <c r="B53" s="17" t="s">
         <v>21</v>
@@ -12617,7 +12617,7 @@
       </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="15">
+    <row r="54" spans="1:9" ht="15.6">
       <c r="A54" s="17"/>
       <c r="B54" s="17" t="s">
         <v>21</v>
@@ -12640,7 +12640,7 @@
       </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="15">
+    <row r="55" spans="1:9" ht="15.6">
       <c r="A55" s="17"/>
       <c r="B55" s="17" t="s">
         <v>21</v>
@@ -12663,7 +12663,7 @@
       </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="15">
+    <row r="56" spans="1:9" ht="15.6">
       <c r="A56" s="17"/>
       <c r="B56" s="17" t="s">
         <v>21</v>
@@ -12686,7 +12686,7 @@
       </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="15">
+    <row r="57" spans="1:9" ht="15.6">
       <c r="A57" s="17"/>
       <c r="B57" s="17" t="s">
         <v>21</v>
@@ -12709,7 +12709,7 @@
       </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="15">
+    <row r="58" spans="1:9" ht="15.6">
       <c r="A58" s="17"/>
       <c r="B58" s="17" t="s">
         <v>21</v>
@@ -12732,7 +12732,7 @@
       </c>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="15">
+    <row r="59" spans="1:9" ht="15.6">
       <c r="A59" s="17"/>
       <c r="B59" s="17" t="s">
         <v>21</v>
@@ -12755,7 +12755,7 @@
       </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="15">
+    <row r="60" spans="1:9" ht="15.6">
       <c r="A60" s="17"/>
       <c r="B60" s="17" t="s">
         <v>21</v>
@@ -12778,7 +12778,7 @@
       </c>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="15">
+    <row r="61" spans="1:9" ht="15.6">
       <c r="A61" s="17" t="b">
         <v>0</v>
       </c>
@@ -12797,7 +12797,7 @@
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="15">
+    <row r="62" spans="1:9" ht="15.6">
       <c r="A62" s="17"/>
       <c r="B62" s="17" t="s">
         <v>21</v>
@@ -12818,7 +12818,7 @@
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="15">
+    <row r="63" spans="1:9" ht="15.6">
       <c r="A63" s="17"/>
       <c r="B63" s="17" t="s">
         <v>21</v>
@@ -12843,7 +12843,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15">
+    <row r="64" spans="1:9" ht="15.6">
       <c r="A64" s="17"/>
       <c r="B64" s="17" t="s">
         <v>21</v>
@@ -12866,7 +12866,7 @@
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" ht="15">
+    <row r="65" spans="1:9" ht="15.6">
       <c r="A65" s="17"/>
       <c r="B65" s="17" t="s">
         <v>21</v>
@@ -12889,7 +12889,7 @@
       </c>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" ht="15">
+    <row r="66" spans="1:9" ht="15.6">
       <c r="A66" s="17"/>
       <c r="B66" s="17" t="s">
         <v>21</v>
@@ -12912,7 +12912,7 @@
       </c>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" ht="15">
+    <row r="67" spans="1:9" ht="15.6">
       <c r="A67" s="17"/>
       <c r="B67" s="17" t="s">
         <v>21</v>
@@ -12935,7 +12935,7 @@
       </c>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" ht="15">
+    <row r="68" spans="1:9" ht="15.6">
       <c r="A68" s="17"/>
       <c r="B68" s="17" t="s">
         <v>21</v>
@@ -12958,7 +12958,7 @@
       </c>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" ht="15">
+    <row r="69" spans="1:9" ht="15.6">
       <c r="A69" s="17"/>
       <c r="B69" s="17" t="s">
         <v>21</v>
@@ -12981,7 +12981,7 @@
       </c>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" ht="15">
+    <row r="70" spans="1:9" ht="15.6">
       <c r="A70" s="17"/>
       <c r="B70" s="17" t="s">
         <v>21</v>
@@ -13004,7 +13004,7 @@
       </c>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" ht="15">
+    <row r="71" spans="1:9" ht="15.6">
       <c r="A71" s="17"/>
       <c r="B71" s="17" t="s">
         <v>21</v>
@@ -13027,7 +13027,7 @@
       </c>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" ht="15">
+    <row r="72" spans="1:9" ht="15.6">
       <c r="A72" s="17" t="b">
         <v>0</v>
       </c>
@@ -13046,7 +13046,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" ht="15">
+    <row r="73" spans="1:9" ht="15.6">
       <c r="A73" s="17"/>
       <c r="B73" s="17" t="s">
         <v>21</v>
@@ -13067,7 +13067,7 @@
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" ht="15">
+    <row r="74" spans="1:9" ht="15.6">
       <c r="A74" s="17"/>
       <c r="B74" s="17" t="s">
         <v>21</v>
@@ -13090,7 +13090,7 @@
       </c>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" ht="15">
+    <row r="75" spans="1:9" ht="15.6">
       <c r="A75" s="17"/>
       <c r="B75" s="17" t="s">
         <v>21</v>
@@ -13115,7 +13115,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15">
+    <row r="76" spans="1:9" ht="15.6">
       <c r="A76" s="17"/>
       <c r="B76" s="17" t="s">
         <v>21</v>
@@ -13138,7 +13138,7 @@
       </c>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" ht="15">
+    <row r="77" spans="1:9" ht="15.6">
       <c r="A77" s="17"/>
       <c r="B77" s="17" t="s">
         <v>21</v>
@@ -13161,7 +13161,7 @@
       </c>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" ht="15">
+    <row r="78" spans="1:9" ht="15.6">
       <c r="A78" s="17"/>
       <c r="B78" s="17" t="s">
         <v>21</v>
@@ -13184,7 +13184,7 @@
       </c>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" ht="15">
+    <row r="79" spans="1:9" ht="15.6">
       <c r="A79" s="17"/>
       <c r="B79" s="17" t="s">
         <v>21</v>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" ht="15">
+    <row r="80" spans="1:9" ht="15.6">
       <c r="A80" s="17"/>
       <c r="B80" s="17" t="s">
         <v>21</v>
@@ -13230,7 +13230,7 @@
       </c>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" ht="15">
+    <row r="81" spans="1:9" ht="15.6">
       <c r="A81" s="17"/>
       <c r="B81" s="17" t="s">
         <v>21</v>
@@ -13253,7 +13253,7 @@
       </c>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" ht="15">
+    <row r="82" spans="1:9" ht="15.6">
       <c r="A82" s="17"/>
       <c r="B82" s="17" t="s">
         <v>21</v>
@@ -13276,7 +13276,7 @@
       </c>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" ht="15">
+    <row r="83" spans="1:9" ht="15.6">
       <c r="A83" s="17"/>
       <c r="B83" s="17" t="s">
         <v>21</v>
@@ -13299,7 +13299,7 @@
       </c>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" ht="15">
+    <row r="84" spans="1:9" ht="15.6">
       <c r="A84" s="17"/>
       <c r="B84" s="17" t="s">
         <v>21</v>
@@ -13322,7 +13322,7 @@
       </c>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" ht="15">
+    <row r="85" spans="1:9" ht="15.6">
       <c r="A85" s="17"/>
       <c r="B85" s="17" t="s">
         <v>21</v>
@@ -13345,7 +13345,7 @@
       </c>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" ht="15">
+    <row r="86" spans="1:9" ht="15.6">
       <c r="A86" s="17" t="b">
         <v>0</v>
       </c>
@@ -13364,7 +13364,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" ht="15">
+    <row r="87" spans="1:9" ht="15.6">
       <c r="A87" s="17"/>
       <c r="B87" s="17" t="s">
         <v>21</v>
@@ -13387,7 +13387,7 @@
       </c>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" ht="15">
+    <row r="88" spans="1:9" ht="15.6">
       <c r="A88" s="17"/>
       <c r="B88" s="17" t="s">
         <v>21</v>
@@ -13410,7 +13410,7 @@
       </c>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" ht="15">
+    <row r="89" spans="1:9" ht="15.6">
       <c r="A89" s="17"/>
       <c r="B89" s="17" t="s">
         <v>21</v>
@@ -13433,7 +13433,7 @@
       </c>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" ht="15">
+    <row r="90" spans="1:9" ht="15.6">
       <c r="A90" s="17"/>
       <c r="B90" s="17" t="s">
         <v>21</v>
@@ -13456,7 +13456,7 @@
       </c>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" ht="15">
+    <row r="91" spans="1:9" ht="15.6">
       <c r="A91" s="17"/>
       <c r="B91" s="17" t="s">
         <v>21</v>
@@ -13479,7 +13479,7 @@
       </c>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" ht="15">
+    <row r="92" spans="1:9" ht="15.6">
       <c r="A92" s="17"/>
       <c r="B92" s="17" t="s">
         <v>21</v>
@@ -13502,7 +13502,7 @@
       </c>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" ht="15">
+    <row r="93" spans="1:9" ht="15.6">
       <c r="A93" s="17"/>
       <c r="B93" s="17" t="s">
         <v>21</v>
@@ -13525,7 +13525,7 @@
       </c>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" ht="15">
+    <row r="94" spans="1:9" ht="15.6">
       <c r="A94" s="17"/>
       <c r="B94" s="17" t="s">
         <v>21</v>
@@ -13548,7 +13548,7 @@
       </c>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" ht="15">
+    <row r="95" spans="1:9" ht="15.6">
       <c r="A95" s="17"/>
       <c r="B95" s="17" t="s">
         <v>21</v>
@@ -13571,7 +13571,7 @@
       </c>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" ht="15">
+    <row r="96" spans="1:9" ht="15.6">
       <c r="A96" s="17"/>
       <c r="B96" s="17" t="s">
         <v>21</v>
@@ -13594,7 +13594,7 @@
       </c>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" ht="15">
+    <row r="97" spans="1:9" ht="15.6">
       <c r="A97" s="17" t="b">
         <v>0</v>
       </c>
@@ -13613,7 +13613,7 @@
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" ht="15">
+    <row r="98" spans="1:9" ht="15.6">
       <c r="A98" s="17"/>
       <c r="B98" s="17" t="s">
         <v>21</v>
@@ -13638,7 +13638,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15">
+    <row r="99" spans="1:9" ht="15.6">
       <c r="A99" s="17" t="b">
         <v>0</v>
       </c>
@@ -13657,7 +13657,7 @@
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="1:9" ht="15">
+    <row r="100" spans="1:9" ht="15.6">
       <c r="A100" s="17"/>
       <c r="B100" s="17" t="s">
         <v>21</v>
@@ -13678,7 +13678,7 @@
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="1:9" ht="15">
+    <row r="101" spans="1:9" ht="15.6">
       <c r="A101" s="17"/>
       <c r="B101" s="17" t="s">
         <v>21</v>
@@ -13703,7 +13703,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15">
+    <row r="102" spans="1:9" ht="15.6">
       <c r="A102" s="17" t="b">
         <v>0</v>
       </c>
@@ -13722,7 +13722,7 @@
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="1:9" ht="15">
+    <row r="103" spans="1:9" ht="15.6">
       <c r="A103" s="17"/>
       <c r="B103" s="17" t="s">
         <v>21</v>
@@ -13745,7 +13745,7 @@
       </c>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="1:9" ht="15">
+    <row r="104" spans="1:9" ht="15.6">
       <c r="A104" s="17"/>
       <c r="B104" s="17" t="s">
         <v>21</v>
@@ -13770,7 +13770,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15">
+    <row r="105" spans="1:9" ht="15.6">
       <c r="A105" s="17"/>
       <c r="B105" s="17" t="s">
         <v>21</v>
@@ -13793,7 +13793,7 @@
       </c>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="1:9" ht="15">
+    <row r="106" spans="1:9" ht="15.6">
       <c r="A106" s="17"/>
       <c r="B106" s="17" t="s">
         <v>21</v>
@@ -13814,7 +13814,7 @@
       <c r="H106" s="17"/>
       <c r="I106" s="17"/>
     </row>
-    <row r="107" spans="1:9" ht="15">
+    <row r="107" spans="1:9" ht="15.6">
       <c r="A107" s="17" t="b">
         <v>0</v>
       </c>
@@ -13833,7 +13833,7 @@
       <c r="H107" s="17"/>
       <c r="I107" s="17"/>
     </row>
-    <row r="108" spans="1:9" ht="15">
+    <row r="108" spans="1:9" ht="15.6">
       <c r="A108" s="17"/>
       <c r="B108" s="17" t="s">
         <v>21</v>
@@ -13858,7 +13858,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15">
+    <row r="109" spans="1:9" ht="15.6">
       <c r="A109" s="17"/>
       <c r="B109" s="17" t="s">
         <v>21</v>
@@ -13881,7 +13881,7 @@
       </c>
       <c r="I109" s="17"/>
     </row>
-    <row r="110" spans="1:9" ht="15">
+    <row r="110" spans="1:9" ht="15.6">
       <c r="A110" s="17"/>
       <c r="B110" s="17" t="s">
         <v>21</v>
@@ -13904,7 +13904,7 @@
       </c>
       <c r="I110" s="17"/>
     </row>
-    <row r="111" spans="1:9" ht="15">
+    <row r="111" spans="1:9" ht="15.6">
       <c r="A111" s="17"/>
       <c r="B111" s="17" t="s">
         <v>21</v>
@@ -13927,7 +13927,7 @@
       </c>
       <c r="I111" s="17"/>
     </row>
-    <row r="112" spans="1:9" ht="15">
+    <row r="112" spans="1:9" ht="15.6">
       <c r="A112" s="17"/>
       <c r="B112" s="17" t="s">
         <v>21</v>
@@ -13950,7 +13950,7 @@
       </c>
       <c r="I112" s="17"/>
     </row>
-    <row r="113" spans="1:9" ht="15">
+    <row r="113" spans="1:9" ht="15.6">
       <c r="A113" s="17"/>
       <c r="B113" s="17" t="s">
         <v>21</v>
@@ -13973,7 +13973,7 @@
       </c>
       <c r="I113" s="17"/>
     </row>
-    <row r="114" spans="1:9" ht="15">
+    <row r="114" spans="1:9" ht="15.6">
       <c r="A114" s="17"/>
       <c r="B114" s="17" t="s">
         <v>21</v>
@@ -13996,7 +13996,7 @@
       </c>
       <c r="I114" s="17"/>
     </row>
-    <row r="115" spans="1:9" ht="15">
+    <row r="115" spans="1:9" ht="15.6">
       <c r="A115" s="17" t="b">
         <v>0</v>
       </c>
@@ -14015,7 +14015,7 @@
       <c r="H115" s="17"/>
       <c r="I115" s="17"/>
     </row>
-    <row r="116" spans="1:9" ht="15">
+    <row r="116" spans="1:9" ht="15.6">
       <c r="A116" s="17"/>
       <c r="B116" s="17" t="s">
         <v>21</v>
@@ -14038,7 +14038,7 @@
       </c>
       <c r="I116" s="17"/>
     </row>
-    <row r="117" spans="1:9" ht="15">
+    <row r="117" spans="1:9" ht="15.6">
       <c r="A117" s="17"/>
       <c r="B117" s="17" t="s">
         <v>21</v>
@@ -14061,7 +14061,7 @@
       </c>
       <c r="I117" s="17"/>
     </row>
-    <row r="118" spans="1:9" ht="15">
+    <row r="118" spans="1:9" ht="15.6">
       <c r="A118" s="17"/>
       <c r="B118" s="17" t="s">
         <v>21</v>
@@ -14084,7 +14084,7 @@
       </c>
       <c r="I118" s="17"/>
     </row>
-    <row r="119" spans="1:9" ht="15">
+    <row r="119" spans="1:9" ht="15.6">
       <c r="A119" s="17" t="b">
         <v>0</v>
       </c>
@@ -14103,7 +14103,7 @@
       <c r="H119" s="17"/>
       <c r="I119" s="17"/>
     </row>
-    <row r="120" spans="1:9" ht="15">
+    <row r="120" spans="1:9" ht="15.6">
       <c r="A120" s="17"/>
       <c r="B120" s="17" t="s">
         <v>21</v>
@@ -14126,7 +14126,7 @@
       </c>
       <c r="I120" s="17"/>
     </row>
-    <row r="121" spans="1:9" ht="15">
+    <row r="121" spans="1:9" ht="15.6">
       <c r="A121" s="17"/>
       <c r="B121" s="17" t="s">
         <v>21</v>
@@ -14149,7 +14149,7 @@
       </c>
       <c r="I121" s="17"/>
     </row>
-    <row r="122" spans="1:9" ht="15">
+    <row r="122" spans="1:9" ht="15.6">
       <c r="A122" s="17"/>
       <c r="B122" s="17" t="s">
         <v>21</v>
@@ -14172,7 +14172,7 @@
       </c>
       <c r="I122" s="17"/>
     </row>
-    <row r="123" spans="1:9" ht="15">
+    <row r="123" spans="1:9" ht="15.6">
       <c r="A123" s="17"/>
       <c r="B123" s="17" t="s">
         <v>21</v>
@@ -14195,7 +14195,7 @@
       </c>
       <c r="I123" s="17"/>
     </row>
-    <row r="124" spans="1:9" ht="15">
+    <row r="124" spans="1:9" ht="15.6">
       <c r="A124" s="17"/>
       <c r="B124" s="17" t="s">
         <v>21</v>
@@ -14218,7 +14218,7 @@
       </c>
       <c r="I124" s="17"/>
     </row>
-    <row r="125" spans="1:9" ht="15">
+    <row r="125" spans="1:9" ht="15.6">
       <c r="A125" s="17"/>
       <c r="B125" s="17" t="s">
         <v>21</v>
@@ -14241,7 +14241,7 @@
       </c>
       <c r="I125" s="17"/>
     </row>
-    <row r="126" spans="1:9" ht="15">
+    <row r="126" spans="1:9" ht="15.6">
       <c r="A126" s="17" t="b">
         <v>0</v>
       </c>
@@ -14260,7 +14260,7 @@
       <c r="H126" s="17"/>
       <c r="I126" s="17"/>
     </row>
-    <row r="127" spans="1:9" ht="15">
+    <row r="127" spans="1:9" ht="15.6">
       <c r="A127" s="17"/>
       <c r="B127" s="17" t="s">
         <v>21</v>
@@ -14285,7 +14285,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15">
+    <row r="128" spans="1:9" ht="15.6">
       <c r="A128" s="17"/>
       <c r="B128" s="17" t="s">
         <v>21</v>
@@ -14308,7 +14308,7 @@
       </c>
       <c r="I128" s="17"/>
     </row>
-    <row r="129" spans="1:9" ht="15">
+    <row r="129" spans="1:9" ht="15.6">
       <c r="A129" s="17"/>
       <c r="B129" s="17" t="s">
         <v>21</v>
@@ -14331,7 +14331,7 @@
       </c>
       <c r="I129" s="17"/>
     </row>
-    <row r="130" spans="1:9" ht="15">
+    <row r="130" spans="1:9" ht="15.6">
       <c r="A130" s="17"/>
       <c r="B130" s="17" t="s">
         <v>21</v>
@@ -14354,7 +14354,7 @@
       </c>
       <c r="I130" s="17"/>
     </row>
-    <row r="131" spans="1:9" ht="15">
+    <row r="131" spans="1:9" ht="15.6">
       <c r="A131" s="17"/>
       <c r="B131" s="17" t="s">
         <v>21</v>
@@ -14377,7 +14377,7 @@
       </c>
       <c r="I131" s="17"/>
     </row>
-    <row r="132" spans="1:9" ht="15">
+    <row r="132" spans="1:9" ht="15.6">
       <c r="A132" s="17"/>
       <c r="B132" s="17" t="s">
         <v>21</v>
@@ -14400,7 +14400,7 @@
       </c>
       <c r="I132" s="17"/>
     </row>
-    <row r="133" spans="1:9" ht="15">
+    <row r="133" spans="1:9" ht="15.6">
       <c r="A133" s="17"/>
       <c r="B133" s="17" t="s">
         <v>21</v>
@@ -14423,7 +14423,7 @@
       </c>
       <c r="I133" s="17"/>
     </row>
-    <row r="134" spans="1:9" ht="15">
+    <row r="134" spans="1:9" ht="15.6">
       <c r="A134" s="17"/>
       <c r="B134" s="17" t="s">
         <v>21</v>
@@ -14446,7 +14446,7 @@
       </c>
       <c r="I134" s="17"/>
     </row>
-    <row r="135" spans="1:9" ht="15">
+    <row r="135" spans="1:9" ht="15.6">
       <c r="A135" s="17"/>
       <c r="B135" s="17" t="s">
         <v>21</v>
@@ -14469,7 +14469,7 @@
       </c>
       <c r="I135" s="17"/>
     </row>
-    <row r="136" spans="1:9" ht="15">
+    <row r="136" spans="1:9" ht="15.6">
       <c r="A136" s="17" t="b">
         <v>0</v>
       </c>
@@ -14488,7 +14488,7 @@
       <c r="H136" s="17"/>
       <c r="I136" s="17"/>
     </row>
-    <row r="137" spans="1:9" ht="15">
+    <row r="137" spans="1:9" ht="15.6">
       <c r="A137" s="17"/>
       <c r="B137" s="17" t="s">
         <v>21</v>
@@ -14513,7 +14513,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15">
+    <row r="138" spans="1:9" ht="15.6">
       <c r="A138" s="17"/>
       <c r="B138" s="17" t="s">
         <v>21</v>
@@ -14534,7 +14534,7 @@
       <c r="H138" s="17"/>
       <c r="I138" s="17"/>
     </row>
-    <row r="139" spans="1:9" ht="15">
+    <row r="139" spans="1:9" ht="15.6">
       <c r="A139" s="17"/>
       <c r="B139" s="17" t="s">
         <v>21</v>
@@ -14557,7 +14557,7 @@
       </c>
       <c r="I139" s="17"/>
     </row>
-    <row r="140" spans="1:9" ht="15">
+    <row r="140" spans="1:9" ht="15.6">
       <c r="A140" s="17"/>
       <c r="B140" s="17" t="s">
         <v>21</v>
@@ -14580,7 +14580,7 @@
       </c>
       <c r="I140" s="17"/>
     </row>
-    <row r="141" spans="1:9" ht="15">
+    <row r="141" spans="1:9" ht="15.6">
       <c r="A141" s="17"/>
       <c r="B141" s="17" t="s">
         <v>21</v>
@@ -14603,7 +14603,7 @@
       </c>
       <c r="I141" s="17"/>
     </row>
-    <row r="142" spans="1:9" ht="15">
+    <row r="142" spans="1:9" ht="15.6">
       <c r="A142" s="17"/>
       <c r="B142" s="17" t="s">
         <v>21</v>
@@ -14626,7 +14626,7 @@
       </c>
       <c r="I142" s="17"/>
     </row>
-    <row r="143" spans="1:9" ht="15">
+    <row r="143" spans="1:9" ht="15.6">
       <c r="A143" s="17"/>
       <c r="B143" s="17" t="s">
         <v>21</v>
@@ -14649,7 +14649,7 @@
       </c>
       <c r="I143" s="17"/>
     </row>
-    <row r="144" spans="1:9" ht="15">
+    <row r="144" spans="1:9" ht="15.6">
       <c r="A144" s="17"/>
       <c r="B144" s="17" t="s">
         <v>21</v>
@@ -14672,7 +14672,7 @@
       </c>
       <c r="I144" s="17"/>
     </row>
-    <row r="145" spans="1:9" ht="15">
+    <row r="145" spans="1:9" ht="15.6">
       <c r="A145" s="17"/>
       <c r="B145" s="17" t="s">
         <v>21</v>
@@ -14695,7 +14695,7 @@
       </c>
       <c r="I145" s="17"/>
     </row>
-    <row r="146" spans="1:9" ht="15">
+    <row r="146" spans="1:9" ht="15.6">
       <c r="A146" s="17"/>
       <c r="B146" s="17" t="s">
         <v>21</v>
@@ -14718,7 +14718,7 @@
       </c>
       <c r="I146" s="17"/>
     </row>
-    <row r="147" spans="1:9" ht="15">
+    <row r="147" spans="1:9" ht="15.6">
       <c r="A147" s="17"/>
       <c r="B147" s="17" t="s">
         <v>21</v>
@@ -14741,7 +14741,7 @@
       </c>
       <c r="I147" s="17"/>
     </row>
-    <row r="148" spans="1:9" ht="15">
+    <row r="148" spans="1:9" ht="15.6">
       <c r="A148" s="17"/>
       <c r="B148" s="17" t="s">
         <v>21</v>
@@ -14764,7 +14764,7 @@
       </c>
       <c r="I148" s="17"/>
     </row>
-    <row r="149" spans="1:9" ht="15">
+    <row r="149" spans="1:9" ht="15.6">
       <c r="A149" s="17"/>
       <c r="B149" s="17" t="s">
         <v>21</v>
@@ -14787,7 +14787,7 @@
       </c>
       <c r="I149" s="17"/>
     </row>
-    <row r="150" spans="1:9" ht="15">
+    <row r="150" spans="1:9" ht="15.6">
       <c r="A150" s="17"/>
       <c r="B150" s="17" t="s">
         <v>21</v>
@@ -14810,7 +14810,7 @@
       </c>
       <c r="I150" s="17"/>
     </row>
-    <row r="151" spans="1:9" ht="15">
+    <row r="151" spans="1:9" ht="15.6">
       <c r="A151" s="17" t="b">
         <v>0</v>
       </c>
@@ -14829,7 +14829,7 @@
       <c r="H151" s="17"/>
       <c r="I151" s="17"/>
     </row>
-    <row r="152" spans="1:9" ht="15">
+    <row r="152" spans="1:9" ht="15.6">
       <c r="A152" s="17"/>
       <c r="B152" s="17" t="s">
         <v>21</v>
@@ -14852,7 +14852,7 @@
       </c>
       <c r="I152" s="17"/>
     </row>
-    <row r="153" spans="1:9" ht="15">
+    <row r="153" spans="1:9" ht="15.6">
       <c r="A153" s="17" t="b">
         <v>0</v>
       </c>
@@ -14871,7 +14871,7 @@
       <c r="H153" s="17"/>
       <c r="I153" s="17"/>
     </row>
-    <row r="154" spans="1:9" ht="15">
+    <row r="154" spans="1:9" ht="15.6">
       <c r="A154" s="17"/>
       <c r="B154" s="17" t="s">
         <v>21</v>
@@ -14894,7 +14894,7 @@
       </c>
       <c r="I154" s="17"/>
     </row>
-    <row r="155" spans="1:9" ht="15">
+    <row r="155" spans="1:9" ht="15.6">
       <c r="A155" s="17"/>
       <c r="B155" s="17" t="s">
         <v>21</v>
@@ -14917,7 +14917,7 @@
       </c>
       <c r="I155" s="17"/>
     </row>
-    <row r="156" spans="1:9" ht="15">
+    <row r="156" spans="1:9" ht="15.6">
       <c r="A156" s="17" t="b">
         <v>0</v>
       </c>
@@ -14936,7 +14936,7 @@
       <c r="H156" s="17"/>
       <c r="I156" s="17"/>
     </row>
-    <row r="157" spans="1:9" ht="15">
+    <row r="157" spans="1:9" ht="15.6">
       <c r="A157" s="17"/>
       <c r="B157" s="17" t="s">
         <v>21</v>
@@ -14961,7 +14961,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15">
+    <row r="158" spans="1:9" ht="15.6">
       <c r="A158" s="17"/>
       <c r="B158" s="17" t="s">
         <v>21</v>
@@ -14984,7 +14984,7 @@
       </c>
       <c r="I158" s="17"/>
     </row>
-    <row r="159" spans="1:9" ht="15">
+    <row r="159" spans="1:9" ht="15.6">
       <c r="A159" s="17"/>
       <c r="B159" s="17" t="s">
         <v>21</v>
@@ -15007,7 +15007,7 @@
       </c>
       <c r="I159" s="17"/>
     </row>
-    <row r="160" spans="1:9" ht="15">
+    <row r="160" spans="1:9" ht="15.6">
       <c r="A160" s="17"/>
       <c r="B160" s="17" t="s">
         <v>21</v>
@@ -15030,7 +15030,7 @@
       </c>
       <c r="I160" s="17"/>
     </row>
-    <row r="161" spans="1:9" ht="15">
+    <row r="161" spans="1:9" ht="15.6">
       <c r="A161" s="17"/>
       <c r="B161" s="17" t="s">
         <v>21</v>
@@ -15053,7 +15053,7 @@
       </c>
       <c r="I161" s="17"/>
     </row>
-    <row r="162" spans="1:9" ht="15">
+    <row r="162" spans="1:9" ht="15.6">
       <c r="A162" s="17"/>
       <c r="B162" s="17" t="s">
         <v>21</v>
@@ -15076,7 +15076,7 @@
       </c>
       <c r="I162" s="17"/>
     </row>
-    <row r="163" spans="1:9" ht="15">
+    <row r="163" spans="1:9" ht="15.6">
       <c r="A163" s="17"/>
       <c r="B163" s="17" t="s">
         <v>21</v>
@@ -15099,7 +15099,7 @@
       </c>
       <c r="I163" s="17"/>
     </row>
-    <row r="164" spans="1:9" ht="15">
+    <row r="164" spans="1:9" ht="15.6">
       <c r="A164" s="17"/>
       <c r="B164" s="17" t="s">
         <v>21</v>
@@ -15122,7 +15122,7 @@
       </c>
       <c r="I164" s="17"/>
     </row>
-    <row r="165" spans="1:9" ht="15">
+    <row r="165" spans="1:9" ht="15.6">
       <c r="A165" s="17"/>
       <c r="B165" s="17" t="s">
         <v>21</v>
@@ -15145,7 +15145,7 @@
       </c>
       <c r="I165" s="17"/>
     </row>
-    <row r="166" spans="1:9" ht="15">
+    <row r="166" spans="1:9" ht="15.6">
       <c r="A166" s="17"/>
       <c r="B166" s="17" t="s">
         <v>21</v>
@@ -15168,7 +15168,7 @@
       </c>
       <c r="I166" s="17"/>
     </row>
-    <row r="167" spans="1:9" ht="15">
+    <row r="167" spans="1:9" ht="15.6">
       <c r="A167" s="17" t="b">
         <v>0</v>
       </c>
@@ -15187,7 +15187,7 @@
       <c r="H167" s="17"/>
       <c r="I167" s="17"/>
     </row>
-    <row r="168" spans="1:9" ht="15">
+    <row r="168" spans="1:9" ht="15.6">
       <c r="A168" s="17"/>
       <c r="B168" s="17" t="s">
         <v>21</v>
@@ -15212,7 +15212,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15">
+    <row r="169" spans="1:9" ht="15.6">
       <c r="A169" s="17"/>
       <c r="B169" s="17" t="s">
         <v>21</v>
@@ -15235,7 +15235,7 @@
       </c>
       <c r="I169" s="17"/>
     </row>
-    <row r="170" spans="1:9" ht="15">
+    <row r="170" spans="1:9" ht="15.6">
       <c r="A170" s="17"/>
       <c r="B170" s="17" t="s">
         <v>21</v>
@@ -15258,7 +15258,7 @@
       </c>
       <c r="I170" s="17"/>
     </row>
-    <row r="171" spans="1:9" ht="15">
+    <row r="171" spans="1:9" ht="15.6">
       <c r="A171" s="17"/>
       <c r="B171" s="17" t="s">
         <v>21</v>
@@ -15281,7 +15281,7 @@
       </c>
       <c r="I171" s="17"/>
     </row>
-    <row r="172" spans="1:9" ht="15">
+    <row r="172" spans="1:9" ht="15.6">
       <c r="A172" s="17"/>
       <c r="B172" s="17" t="s">
         <v>21</v>
@@ -15304,7 +15304,7 @@
       </c>
       <c r="I172" s="17"/>
     </row>
-    <row r="173" spans="1:9" ht="15">
+    <row r="173" spans="1:9" ht="15.6">
       <c r="A173" s="17"/>
       <c r="B173" s="17" t="s">
         <v>21</v>
@@ -15327,7 +15327,7 @@
       </c>
       <c r="I173" s="17"/>
     </row>
-    <row r="174" spans="1:9" ht="15">
+    <row r="174" spans="1:9" ht="15.6">
       <c r="A174" s="17"/>
       <c r="B174" s="17" t="s">
         <v>21</v>
@@ -15350,7 +15350,7 @@
       </c>
       <c r="I174" s="17"/>
     </row>
-    <row r="175" spans="1:9" ht="15">
+    <row r="175" spans="1:9" ht="15.6">
       <c r="A175" s="17"/>
       <c r="B175" s="17" t="s">
         <v>21</v>
@@ -15373,7 +15373,7 @@
       </c>
       <c r="I175" s="17"/>
     </row>
-    <row r="176" spans="1:9" ht="15">
+    <row r="176" spans="1:9" ht="15.6">
       <c r="A176" s="17"/>
       <c r="B176" s="17" t="s">
         <v>21</v>
@@ -15396,7 +15396,7 @@
       </c>
       <c r="I176" s="17"/>
     </row>
-    <row r="177" spans="1:9" ht="15">
+    <row r="177" spans="1:9" ht="15.6">
       <c r="A177" s="17"/>
       <c r="B177" s="17" t="s">
         <v>21</v>
@@ -15419,7 +15419,7 @@
       </c>
       <c r="I177" s="17"/>
     </row>
-    <row r="178" spans="1:9" ht="15">
+    <row r="178" spans="1:9" ht="15.6">
       <c r="A178" s="17" t="b">
         <v>0</v>
       </c>
@@ -15438,7 +15438,7 @@
       <c r="H178" s="17"/>
       <c r="I178" s="17"/>
     </row>
-    <row r="179" spans="1:9" ht="15">
+    <row r="179" spans="1:9" ht="15.6">
       <c r="A179" s="17"/>
       <c r="B179" s="17" t="s">
         <v>21</v>
@@ -15461,7 +15461,7 @@
       </c>
       <c r="I179" s="17"/>
     </row>
-    <row r="180" spans="1:9" ht="15">
+    <row r="180" spans="1:9" ht="15.6">
       <c r="A180" s="17"/>
       <c r="B180" s="17" t="s">
         <v>21</v>
@@ -15484,7 +15484,7 @@
       </c>
       <c r="I180" s="17"/>
     </row>
-    <row r="181" spans="1:9" ht="15">
+    <row r="181" spans="1:9" ht="15.6">
       <c r="A181" s="17"/>
       <c r="B181" s="17" t="s">
         <v>21</v>
@@ -15507,7 +15507,7 @@
       </c>
       <c r="I181" s="17"/>
     </row>
-    <row r="182" spans="1:9" ht="15">
+    <row r="182" spans="1:9" ht="15.6">
       <c r="A182" s="17"/>
       <c r="B182" s="17" t="s">
         <v>21</v>
@@ -15530,7 +15530,7 @@
       </c>
       <c r="I182" s="17"/>
     </row>
-    <row r="183" spans="1:9" ht="15">
+    <row r="183" spans="1:9" ht="15.6">
       <c r="A183" s="17" t="b">
         <v>0</v>
       </c>
@@ -15549,7 +15549,7 @@
       <c r="H183" s="17"/>
       <c r="I183" s="17"/>
     </row>
-    <row r="184" spans="1:9" ht="15">
+    <row r="184" spans="1:9" ht="15.6">
       <c r="A184" s="17"/>
       <c r="B184" s="17" t="s">
         <v>21</v>
@@ -15572,7 +15572,7 @@
       </c>
       <c r="I184" s="17"/>
     </row>
-    <row r="185" spans="1:9" ht="15">
+    <row r="185" spans="1:9" ht="15.6">
       <c r="A185" s="17"/>
       <c r="B185" s="17" t="s">
         <v>21</v>
@@ -15595,7 +15595,7 @@
       </c>
       <c r="I185" s="17"/>
     </row>
-    <row r="186" spans="1:9" ht="15">
+    <row r="186" spans="1:9" ht="15.6">
       <c r="A186" s="17"/>
       <c r="B186" s="17" t="s">
         <v>21</v>
@@ -15618,7 +15618,7 @@
       </c>
       <c r="I186" s="17"/>
     </row>
-    <row r="187" spans="1:9" ht="15">
+    <row r="187" spans="1:9" ht="15.6">
       <c r="A187" s="17"/>
       <c r="B187" s="17" t="s">
         <v>21</v>
@@ -15641,7 +15641,7 @@
       </c>
       <c r="I187" s="17"/>
     </row>
-    <row r="188" spans="1:9" ht="15">
+    <row r="188" spans="1:9" ht="15.6">
       <c r="A188" s="17" t="b">
         <v>0</v>
       </c>
@@ -15660,7 +15660,7 @@
       <c r="H188" s="17"/>
       <c r="I188" s="17"/>
     </row>
-    <row r="189" spans="1:9" ht="15">
+    <row r="189" spans="1:9" ht="15.6">
       <c r="A189" s="17"/>
       <c r="B189" s="17" t="s">
         <v>21</v>
@@ -15681,7 +15681,7 @@
       <c r="H189" s="17"/>
       <c r="I189" s="17"/>
     </row>
-    <row r="190" spans="1:9" ht="15">
+    <row r="190" spans="1:9" ht="15.6">
       <c r="A190" s="17"/>
       <c r="B190" s="17" t="s">
         <v>21</v>
@@ -15704,7 +15704,7 @@
       </c>
       <c r="I190" s="17"/>
     </row>
-    <row r="191" spans="1:9" ht="15">
+    <row r="191" spans="1:9" ht="15.6">
       <c r="A191" s="17" t="b">
         <v>0</v>
       </c>
@@ -15723,7 +15723,7 @@
       <c r="H191" s="17"/>
       <c r="I191" s="17"/>
     </row>
-    <row r="192" spans="1:9" ht="15">
+    <row r="192" spans="1:9" ht="15.6">
       <c r="A192" s="17"/>
       <c r="B192" s="17" t="s">
         <v>21</v>
@@ -15746,7 +15746,7 @@
       </c>
       <c r="I192" s="17"/>
     </row>
-    <row r="193" spans="1:9" ht="15">
+    <row r="193" spans="1:9" ht="15.6">
       <c r="A193" s="17"/>
       <c r="B193" s="17" t="s">
         <v>21</v>
@@ -15771,7 +15771,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15">
+    <row r="194" spans="1:9" ht="15.6">
       <c r="A194" s="17"/>
       <c r="B194" s="17" t="s">
         <v>21</v>
@@ -15792,7 +15792,7 @@
       <c r="H194" s="17"/>
       <c r="I194" s="17"/>
     </row>
-    <row r="195" spans="1:9" ht="15">
+    <row r="195" spans="1:9" ht="15.6">
       <c r="A195" s="17"/>
       <c r="B195" s="17" t="s">
         <v>21</v>
@@ -15817,7 +15817,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15">
+    <row r="196" spans="1:9" ht="15.6">
       <c r="A196" s="17"/>
       <c r="B196" s="17" t="s">
         <v>21</v>
@@ -15842,7 +15842,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15">
+    <row r="197" spans="1:9" ht="15.6">
       <c r="A197" s="17" t="b">
         <v>0</v>
       </c>
@@ -15861,7 +15861,7 @@
       <c r="H197" s="17"/>
       <c r="I197" s="17"/>
     </row>
-    <row r="198" spans="1:9" ht="15">
+    <row r="198" spans="1:9" ht="15.6">
       <c r="A198" s="17"/>
       <c r="B198" s="17" t="s">
         <v>21</v>
@@ -15886,7 +15886,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15">
+    <row r="199" spans="1:9" ht="15.6">
       <c r="A199" s="17"/>
       <c r="B199" s="17" t="s">
         <v>21</v>
@@ -15909,7 +15909,7 @@
       </c>
       <c r="I199" s="17"/>
     </row>
-    <row r="200" spans="1:9" ht="15">
+    <row r="200" spans="1:9" ht="15.6">
       <c r="A200" s="17"/>
       <c r="B200" s="17" t="s">
         <v>21</v>
@@ -15932,7 +15932,7 @@
       </c>
       <c r="I200" s="17"/>
     </row>
-    <row r="201" spans="1:9" ht="15">
+    <row r="201" spans="1:9" ht="15.6">
       <c r="A201" s="17"/>
       <c r="B201" s="17" t="s">
         <v>21</v>
@@ -15955,7 +15955,7 @@
       </c>
       <c r="I201" s="17"/>
     </row>
-    <row r="202" spans="1:9" ht="15">
+    <row r="202" spans="1:9" ht="15.6">
       <c r="A202" s="17"/>
       <c r="B202" s="17" t="s">
         <v>21</v>
@@ -15978,7 +15978,7 @@
       </c>
       <c r="I202" s="17"/>
     </row>
-    <row r="203" spans="1:9" ht="15">
+    <row r="203" spans="1:9" ht="15.6">
       <c r="A203" s="17"/>
       <c r="B203" s="17" t="s">
         <v>21</v>
@@ -16001,7 +16001,7 @@
       </c>
       <c r="I203" s="17"/>
     </row>
-    <row r="204" spans="1:9" ht="15">
+    <row r="204" spans="1:9" ht="15.6">
       <c r="A204" s="17"/>
       <c r="B204" s="17" t="s">
         <v>21</v>
@@ -16024,7 +16024,7 @@
       </c>
       <c r="I204" s="17"/>
     </row>
-    <row r="205" spans="1:9" ht="15">
+    <row r="205" spans="1:9" ht="15.6">
       <c r="A205" s="17"/>
       <c r="B205" s="17" t="s">
         <v>21</v>
@@ -16047,7 +16047,7 @@
       </c>
       <c r="I205" s="17"/>
     </row>
-    <row r="206" spans="1:9" ht="15">
+    <row r="206" spans="1:9" ht="15.6">
       <c r="A206" s="17"/>
       <c r="B206" s="17" t="s">
         <v>21</v>
@@ -16070,7 +16070,7 @@
       </c>
       <c r="I206" s="17"/>
     </row>
-    <row r="207" spans="1:9" ht="15">
+    <row r="207" spans="1:9" ht="15.6">
       <c r="A207" s="17" t="b">
         <v>0</v>
       </c>
@@ -16089,7 +16089,7 @@
       <c r="H207" s="17"/>
       <c r="I207" s="17"/>
     </row>
-    <row r="208" spans="1:9" ht="15">
+    <row r="208" spans="1:9" ht="15.6">
       <c r="A208" s="17"/>
       <c r="B208" s="17" t="s">
         <v>21</v>
@@ -16114,7 +16114,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15">
+    <row r="209" spans="1:9" ht="15.6">
       <c r="A209" s="17"/>
       <c r="B209" s="17" t="s">
         <v>21</v>
@@ -16137,7 +16137,7 @@
       </c>
       <c r="I209" s="17"/>
     </row>
-    <row r="210" spans="1:9" ht="15">
+    <row r="210" spans="1:9" ht="15.6">
       <c r="A210" s="17"/>
       <c r="B210" s="17" t="s">
         <v>21</v>
@@ -16160,7 +16160,7 @@
       </c>
       <c r="I210" s="17"/>
     </row>
-    <row r="211" spans="1:9" ht="15">
+    <row r="211" spans="1:9" ht="15.6">
       <c r="A211" s="17"/>
       <c r="B211" s="17" t="s">
         <v>21</v>
@@ -16183,7 +16183,7 @@
       </c>
       <c r="I211" s="17"/>
     </row>
-    <row r="212" spans="1:9" ht="15">
+    <row r="212" spans="1:9" ht="15.6">
       <c r="A212" s="17"/>
       <c r="B212" s="17" t="s">
         <v>21</v>
@@ -16206,7 +16206,7 @@
       </c>
       <c r="I212" s="17"/>
     </row>
-    <row r="213" spans="1:9" ht="15">
+    <row r="213" spans="1:9" ht="15.6">
       <c r="A213" s="17"/>
       <c r="B213" s="17" t="s">
         <v>21</v>
@@ -16229,7 +16229,7 @@
       </c>
       <c r="I213" s="17"/>
     </row>
-    <row r="214" spans="1:9" ht="15">
+    <row r="214" spans="1:9" ht="15.6">
       <c r="A214" s="17"/>
       <c r="B214" s="17" t="s">
         <v>21</v>
@@ -16252,7 +16252,7 @@
       </c>
       <c r="I214" s="17"/>
     </row>
-    <row r="215" spans="1:9" ht="15">
+    <row r="215" spans="1:9" ht="15.6">
       <c r="A215" s="17"/>
       <c r="B215" s="17" t="s">
         <v>21</v>
@@ -16275,7 +16275,7 @@
       </c>
       <c r="I215" s="17"/>
     </row>
-    <row r="216" spans="1:9" ht="15">
+    <row r="216" spans="1:9" ht="15.6">
       <c r="A216" s="17"/>
       <c r="B216" s="17" t="s">
         <v>21</v>
@@ -16298,7 +16298,7 @@
       </c>
       <c r="I216" s="17"/>
     </row>
-    <row r="217" spans="1:9" ht="15">
+    <row r="217" spans="1:9" ht="15.6">
       <c r="A217" s="17" t="b">
         <v>0</v>
       </c>
@@ -16317,7 +16317,7 @@
       <c r="H217" s="17"/>
       <c r="I217" s="17"/>
     </row>
-    <row r="218" spans="1:9" ht="15">
+    <row r="218" spans="1:9" ht="15.6">
       <c r="A218" s="17"/>
       <c r="B218" s="17" t="s">
         <v>21</v>
@@ -16338,7 +16338,7 @@
       <c r="H218" s="17"/>
       <c r="I218" s="17"/>
     </row>
-    <row r="219" spans="1:9" ht="15">
+    <row r="219" spans="1:9" ht="15.6">
       <c r="A219" s="17"/>
       <c r="B219" s="17" t="s">
         <v>21</v>
@@ -16361,7 +16361,7 @@
       </c>
       <c r="I219" s="17"/>
     </row>
-    <row r="220" spans="1:9" ht="15">
+    <row r="220" spans="1:9" ht="15.6">
       <c r="A220" s="17"/>
       <c r="B220" s="17" t="s">
         <v>21</v>
@@ -16384,7 +16384,7 @@
       </c>
       <c r="I220" s="17"/>
     </row>
-    <row r="221" spans="1:9" ht="15">
+    <row r="221" spans="1:9" ht="15.6">
       <c r="A221" s="17"/>
       <c r="B221" s="17" t="s">
         <v>21</v>
@@ -16407,7 +16407,7 @@
       </c>
       <c r="I221" s="17"/>
     </row>
-    <row r="222" spans="1:9" ht="15">
+    <row r="222" spans="1:9" ht="15.6">
       <c r="A222" s="17"/>
       <c r="B222" s="17" t="s">
         <v>21</v>
@@ -16430,7 +16430,7 @@
       </c>
       <c r="I222" s="17"/>
     </row>
-    <row r="223" spans="1:9" ht="15">
+    <row r="223" spans="1:9" ht="15.6">
       <c r="A223" s="17"/>
       <c r="B223" s="17" t="s">
         <v>21</v>
@@ -16453,7 +16453,7 @@
       </c>
       <c r="I223" s="17"/>
     </row>
-    <row r="224" spans="1:9" ht="15">
+    <row r="224" spans="1:9" ht="15.6">
       <c r="A224" s="17"/>
       <c r="B224" s="17" t="s">
         <v>21</v>
@@ -16476,7 +16476,7 @@
       </c>
       <c r="I224" s="17"/>
     </row>
-    <row r="225" spans="1:9" ht="15">
+    <row r="225" spans="1:9" ht="15.6">
       <c r="A225" s="17"/>
       <c r="B225" s="17" t="s">
         <v>21</v>
@@ -16499,7 +16499,7 @@
       </c>
       <c r="I225" s="17"/>
     </row>
-    <row r="226" spans="1:9" ht="15">
+    <row r="226" spans="1:9" ht="15.6">
       <c r="A226" s="17"/>
       <c r="B226" s="17" t="s">
         <v>21</v>
@@ -16522,7 +16522,7 @@
       </c>
       <c r="I226" s="17"/>
     </row>
-    <row r="227" spans="1:9" ht="15">
+    <row r="227" spans="1:9" ht="15.6">
       <c r="A227" s="17"/>
       <c r="B227" s="17" t="s">
         <v>21</v>
@@ -16545,7 +16545,7 @@
       </c>
       <c r="I227" s="17"/>
     </row>
-    <row r="228" spans="1:9" ht="15">
+    <row r="228" spans="1:9" ht="15.6">
       <c r="A228" s="17"/>
       <c r="B228" s="17" t="s">
         <v>21</v>
@@ -16568,7 +16568,7 @@
       </c>
       <c r="I228" s="17"/>
     </row>
-    <row r="229" spans="1:9" ht="15">
+    <row r="229" spans="1:9" ht="15.6">
       <c r="A229" s="17"/>
       <c r="B229" s="17" t="s">
         <v>21</v>
@@ -16591,7 +16591,7 @@
       </c>
       <c r="I229" s="17"/>
     </row>
-    <row r="230" spans="1:9" ht="15">
+    <row r="230" spans="1:9" ht="15.6">
       <c r="A230" s="17"/>
       <c r="B230" s="17" t="s">
         <v>21</v>
@@ -16614,7 +16614,7 @@
       </c>
       <c r="I230" s="17"/>
     </row>
-    <row r="231" spans="1:9" ht="15">
+    <row r="231" spans="1:9" ht="15.6">
       <c r="A231" s="17"/>
       <c r="B231" s="17" t="s">
         <v>21</v>
@@ -16637,7 +16637,7 @@
       </c>
       <c r="I231" s="17"/>
     </row>
-    <row r="232" spans="1:9" ht="15">
+    <row r="232" spans="1:9" ht="15.6">
       <c r="A232" s="17"/>
       <c r="B232" s="17" t="s">
         <v>21</v>
@@ -16660,7 +16660,7 @@
       </c>
       <c r="I232" s="17"/>
     </row>
-    <row r="233" spans="1:9" ht="15">
+    <row r="233" spans="1:9" ht="15.6">
       <c r="A233" s="17"/>
       <c r="B233" s="17" t="s">
         <v>21</v>
@@ -16683,7 +16683,7 @@
       </c>
       <c r="I233" s="17"/>
     </row>
-    <row r="234" spans="1:9" ht="15">
+    <row r="234" spans="1:9" ht="15.6">
       <c r="A234" s="17" t="b">
         <v>0</v>
       </c>
@@ -16702,7 +16702,7 @@
       <c r="H234" s="17"/>
       <c r="I234" s="17"/>
     </row>
-    <row r="235" spans="1:9" ht="15">
+    <row r="235" spans="1:9" ht="15.6">
       <c r="A235" s="17"/>
       <c r="B235" s="17" t="s">
         <v>21</v>
@@ -16723,7 +16723,7 @@
       <c r="H235" s="17"/>
       <c r="I235" s="17"/>
     </row>
-    <row r="236" spans="1:9" ht="15">
+    <row r="236" spans="1:9" ht="15.6">
       <c r="A236" s="17"/>
       <c r="B236" s="17" t="s">
         <v>21</v>
@@ -16746,7 +16746,7 @@
       </c>
       <c r="I236" s="17"/>
     </row>
-    <row r="237" spans="1:9" ht="15">
+    <row r="237" spans="1:9" ht="15.6">
       <c r="A237" s="17"/>
       <c r="B237" s="17" t="s">
         <v>21</v>
@@ -16769,7 +16769,7 @@
       </c>
       <c r="I237" s="17"/>
     </row>
-    <row r="238" spans="1:9" ht="15">
+    <row r="238" spans="1:9" ht="15.6">
       <c r="A238" s="17"/>
       <c r="B238" s="17" t="s">
         <v>21</v>
@@ -16792,7 +16792,7 @@
       </c>
       <c r="I238" s="17"/>
     </row>
-    <row r="239" spans="1:9" ht="15">
+    <row r="239" spans="1:9" ht="15.6">
       <c r="A239" s="17"/>
       <c r="B239" s="17" t="s">
         <v>21</v>
@@ -16815,7 +16815,7 @@
       </c>
       <c r="I239" s="17"/>
     </row>
-    <row r="240" spans="1:9" ht="15">
+    <row r="240" spans="1:9" ht="15.6">
       <c r="A240" s="17"/>
       <c r="B240" s="17" t="s">
         <v>21</v>
@@ -16838,7 +16838,7 @@
       </c>
       <c r="I240" s="17"/>
     </row>
-    <row r="241" spans="1:9" ht="15">
+    <row r="241" spans="1:9" ht="15.6">
       <c r="A241" s="17"/>
       <c r="B241" s="17" t="s">
         <v>21</v>
@@ -16861,7 +16861,7 @@
       </c>
       <c r="I241" s="17"/>
     </row>
-    <row r="242" spans="1:9" ht="15">
+    <row r="242" spans="1:9" ht="15.6">
       <c r="A242" s="17"/>
       <c r="B242" s="17" t="s">
         <v>21</v>
@@ -16884,7 +16884,7 @@
       </c>
       <c r="I242" s="17"/>
     </row>
-    <row r="243" spans="1:9" ht="15">
+    <row r="243" spans="1:9" ht="15.6">
       <c r="A243" s="17"/>
       <c r="B243" s="17" t="s">
         <v>21</v>
@@ -16907,7 +16907,7 @@
       </c>
       <c r="I243" s="17"/>
     </row>
-    <row r="244" spans="1:9" ht="15">
+    <row r="244" spans="1:9" ht="15.6">
       <c r="A244" s="17"/>
       <c r="B244" s="17" t="s">
         <v>21</v>
@@ -16930,7 +16930,7 @@
       </c>
       <c r="I244" s="17"/>
     </row>
-    <row r="245" spans="1:9" ht="15">
+    <row r="245" spans="1:9" ht="15.6">
       <c r="A245" s="17"/>
       <c r="B245" s="17" t="s">
         <v>21</v>
@@ -16953,7 +16953,7 @@
       </c>
       <c r="I245" s="17"/>
     </row>
-    <row r="246" spans="1:9" ht="15">
+    <row r="246" spans="1:9" ht="15.6">
       <c r="A246" s="17"/>
       <c r="B246" s="17" t="s">
         <v>21</v>
@@ -16976,7 +16976,7 @@
       </c>
       <c r="I246" s="17"/>
     </row>
-    <row r="247" spans="1:9" ht="15">
+    <row r="247" spans="1:9" ht="15.6">
       <c r="A247" s="17"/>
       <c r="B247" s="17" t="s">
         <v>21</v>
@@ -16999,7 +16999,7 @@
       </c>
       <c r="I247" s="17"/>
     </row>
-    <row r="248" spans="1:9" ht="15">
+    <row r="248" spans="1:9" ht="15.6">
       <c r="A248" s="17"/>
       <c r="B248" s="17" t="s">
         <v>21</v>
@@ -17022,7 +17022,7 @@
       </c>
       <c r="I248" s="17"/>
     </row>
-    <row r="249" spans="1:9" ht="15">
+    <row r="249" spans="1:9" ht="15.6">
       <c r="A249" s="17"/>
       <c r="B249" s="17" t="s">
         <v>21</v>
@@ -17045,7 +17045,7 @@
       </c>
       <c r="I249" s="17"/>
     </row>
-    <row r="250" spans="1:9" ht="15">
+    <row r="250" spans="1:9" ht="15.6">
       <c r="A250" s="17"/>
       <c r="B250" s="17" t="s">
         <v>21</v>
@@ -17068,7 +17068,7 @@
       </c>
       <c r="I250" s="17"/>
     </row>
-    <row r="251" spans="1:9" ht="15">
+    <row r="251" spans="1:9" ht="15.6">
       <c r="A251" s="17" t="b">
         <v>0</v>
       </c>
@@ -17087,7 +17087,7 @@
       <c r="H251" s="17"/>
       <c r="I251" s="17"/>
     </row>
-    <row r="252" spans="1:9" ht="15">
+    <row r="252" spans="1:9" ht="15.6">
       <c r="A252" s="17"/>
       <c r="B252" s="17" t="s">
         <v>21</v>
@@ -17112,7 +17112,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15">
+    <row r="253" spans="1:9" ht="15.6">
       <c r="A253" s="17"/>
       <c r="B253" s="17" t="s">
         <v>21</v>
@@ -17135,7 +17135,7 @@
       </c>
       <c r="I253" s="17"/>
     </row>
-    <row r="254" spans="1:9" ht="15">
+    <row r="254" spans="1:9" ht="15.6">
       <c r="A254" s="17"/>
       <c r="B254" s="17" t="s">
         <v>21</v>
@@ -17158,7 +17158,7 @@
       </c>
       <c r="I254" s="17"/>
     </row>
-    <row r="255" spans="1:9" ht="15">
+    <row r="255" spans="1:9" ht="15.6">
       <c r="A255" s="17"/>
       <c r="B255" s="17" t="s">
         <v>21</v>
@@ -17181,7 +17181,7 @@
       </c>
       <c r="I255" s="17"/>
     </row>
-    <row r="256" spans="1:9" ht="15">
+    <row r="256" spans="1:9" ht="15.6">
       <c r="A256" s="17"/>
       <c r="B256" s="17" t="s">
         <v>21</v>
@@ -17204,7 +17204,7 @@
       </c>
       <c r="I256" s="17"/>
     </row>
-    <row r="257" spans="1:9" ht="15">
+    <row r="257" spans="1:9" ht="15.6">
       <c r="A257" s="17" t="b">
         <v>0</v>
       </c>
@@ -17223,7 +17223,7 @@
       <c r="H257" s="17"/>
       <c r="I257" s="17"/>
     </row>
-    <row r="258" spans="1:9" ht="15">
+    <row r="258" spans="1:9" ht="15.6">
       <c r="A258" s="17"/>
       <c r="B258" s="17" t="s">
         <v>21</v>
@@ -17248,7 +17248,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15">
+    <row r="259" spans="1:9" ht="15.6">
       <c r="A259" s="17"/>
       <c r="B259" s="17" t="s">
         <v>21</v>
@@ -17271,7 +17271,7 @@
       </c>
       <c r="I259" s="17"/>
     </row>
-    <row r="260" spans="1:9" ht="15">
+    <row r="260" spans="1:9" ht="15.6">
       <c r="A260" s="17" t="b">
         <v>0</v>
       </c>
@@ -17290,7 +17290,7 @@
       <c r="H260" s="17"/>
       <c r="I260" s="17"/>
     </row>
-    <row r="261" spans="1:9" ht="15">
+    <row r="261" spans="1:9" ht="15.6">
       <c r="A261" s="17" t="b">
         <v>0</v>
       </c>
@@ -17309,7 +17309,7 @@
       <c r="H261" s="17"/>
       <c r="I261" s="17"/>
     </row>
-    <row r="262" spans="1:9" ht="15">
+    <row r="262" spans="1:9" ht="15.6">
       <c r="A262" s="17" t="b">
         <v>0</v>
       </c>
@@ -17328,7 +17328,7 @@
       <c r="H262" s="17"/>
       <c r="I262" s="17"/>
     </row>
-    <row r="263" spans="1:9" ht="15">
+    <row r="263" spans="1:9" ht="15.6">
       <c r="A263" s="17"/>
       <c r="B263" s="17" t="s">
         <v>21</v>
@@ -17349,7 +17349,7 @@
       <c r="H263" s="17"/>
       <c r="I263" s="17"/>
     </row>
-    <row r="264" spans="1:9" ht="15">
+    <row r="264" spans="1:9" ht="15.6">
       <c r="A264" s="17"/>
       <c r="B264" s="17" t="s">
         <v>21</v>
@@ -17372,7 +17372,7 @@
       </c>
       <c r="I264" s="17"/>
     </row>
-    <row r="265" spans="1:9" ht="15">
+    <row r="265" spans="1:9" ht="15.6">
       <c r="A265" s="17"/>
       <c r="B265" s="17" t="s">
         <v>21</v>
@@ -17395,7 +17395,7 @@
       </c>
       <c r="I265" s="17"/>
     </row>
-    <row r="266" spans="1:9" ht="15">
+    <row r="266" spans="1:9" ht="15.6">
       <c r="A266" s="17"/>
       <c r="B266" s="17" t="s">
         <v>21</v>
@@ -17418,7 +17418,7 @@
       </c>
       <c r="I266" s="17"/>
     </row>
-    <row r="267" spans="1:9" ht="15">
+    <row r="267" spans="1:9" ht="15.6">
       <c r="A267" s="17"/>
       <c r="B267" s="17" t="s">
         <v>21</v>
@@ -17441,7 +17441,7 @@
       </c>
       <c r="I267" s="17"/>
     </row>
-    <row r="268" spans="1:9" ht="15">
+    <row r="268" spans="1:9" ht="15.6">
       <c r="A268" s="17"/>
       <c r="B268" s="17" t="s">
         <v>21</v>
@@ -17464,7 +17464,7 @@
       </c>
       <c r="I268" s="17"/>
     </row>
-    <row r="269" spans="1:9" ht="15">
+    <row r="269" spans="1:9" ht="15.6">
       <c r="A269" s="17"/>
       <c r="B269" s="17" t="s">
         <v>21</v>
@@ -17487,7 +17487,7 @@
       </c>
       <c r="I269" s="17"/>
     </row>
-    <row r="270" spans="1:9" ht="15">
+    <row r="270" spans="1:9" ht="15.6">
       <c r="A270" s="17"/>
       <c r="B270" s="17" t="s">
         <v>21</v>
@@ -17510,7 +17510,7 @@
       </c>
       <c r="I270" s="17"/>
     </row>
-    <row r="271" spans="1:9" ht="15">
+    <row r="271" spans="1:9" ht="15.6">
       <c r="A271" s="17"/>
       <c r="B271" s="17" t="s">
         <v>21</v>
@@ -17533,7 +17533,7 @@
       </c>
       <c r="I271" s="17"/>
     </row>
-    <row r="272" spans="1:9" ht="15">
+    <row r="272" spans="1:9" ht="15.6">
       <c r="A272" s="17"/>
       <c r="B272" s="17" t="s">
         <v>21</v>
@@ -17556,7 +17556,7 @@
       </c>
       <c r="I272" s="17"/>
     </row>
-    <row r="273" spans="1:9" ht="15">
+    <row r="273" spans="1:9" ht="15.6">
       <c r="A273" s="17"/>
       <c r="B273" s="17" t="s">
         <v>21</v>
@@ -17579,7 +17579,7 @@
       </c>
       <c r="I273" s="17"/>
     </row>
-    <row r="274" spans="1:9" ht="15">
+    <row r="274" spans="1:9" ht="15.6">
       <c r="A274" s="17" t="b">
         <v>0</v>
       </c>
@@ -17598,7 +17598,7 @@
       <c r="H274" s="17"/>
       <c r="I274" s="17"/>
     </row>
-    <row r="275" spans="1:9" ht="15">
+    <row r="275" spans="1:9" ht="15.6">
       <c r="A275" s="17"/>
       <c r="B275" s="17" t="s">
         <v>21</v>
@@ -17621,7 +17621,7 @@
       </c>
       <c r="I275" s="17"/>
     </row>
-    <row r="276" spans="1:9" ht="15">
+    <row r="276" spans="1:9" ht="15.6">
       <c r="A276" s="17" t="b">
         <v>0</v>
       </c>
@@ -17640,7 +17640,7 @@
       <c r="H276" s="17"/>
       <c r="I276" s="17"/>
     </row>
-    <row r="277" spans="1:9" ht="15">
+    <row r="277" spans="1:9" ht="15.6">
       <c r="A277" s="17"/>
       <c r="B277" s="17" t="s">
         <v>21</v>
@@ -17665,7 +17665,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15">
+    <row r="278" spans="1:9" ht="15.6">
       <c r="A278" s="17"/>
       <c r="B278" s="17" t="s">
         <v>21</v>
@@ -17688,7 +17688,7 @@
       </c>
       <c r="I278" s="17"/>
     </row>
-    <row r="279" spans="1:9" ht="15">
+    <row r="279" spans="1:9" ht="15.6">
       <c r="A279" s="17"/>
       <c r="B279" s="17" t="s">
         <v>21</v>
@@ -17711,7 +17711,7 @@
       </c>
       <c r="I279" s="17"/>
     </row>
-    <row r="280" spans="1:9" ht="15">
+    <row r="280" spans="1:9" ht="15.6">
       <c r="A280" s="17"/>
       <c r="B280" s="17" t="s">
         <v>21</v>
@@ -17734,7 +17734,7 @@
       </c>
       <c r="I280" s="17"/>
     </row>
-    <row r="281" spans="1:9" ht="15">
+    <row r="281" spans="1:9" ht="15.6">
       <c r="A281" s="17"/>
       <c r="B281" s="17" t="s">
         <v>21</v>
@@ -17757,7 +17757,7 @@
       </c>
       <c r="I281" s="17"/>
     </row>
-    <row r="282" spans="1:9" ht="15">
+    <row r="282" spans="1:9" ht="15.6">
       <c r="A282" s="17"/>
       <c r="B282" s="17" t="s">
         <v>21</v>
@@ -17780,7 +17780,7 @@
       </c>
       <c r="I282" s="17"/>
     </row>
-    <row r="283" spans="1:9" ht="15">
+    <row r="283" spans="1:9" ht="15.6">
       <c r="A283" s="17"/>
       <c r="B283" s="17" t="s">
         <v>21</v>
@@ -17803,7 +17803,7 @@
       </c>
       <c r="I283" s="17"/>
     </row>
-    <row r="284" spans="1:9" ht="15">
+    <row r="284" spans="1:9" ht="15.6">
       <c r="A284" s="17"/>
       <c r="B284" s="17" t="s">
         <v>21</v>
@@ -17826,7 +17826,7 @@
       </c>
       <c r="I284" s="17"/>
     </row>
-    <row r="285" spans="1:9" ht="15">
+    <row r="285" spans="1:9" ht="15.6">
       <c r="A285" s="17"/>
       <c r="B285" s="17" t="s">
         <v>21</v>
@@ -17849,7 +17849,7 @@
       </c>
       <c r="I285" s="17"/>
     </row>
-    <row r="286" spans="1:9" ht="15">
+    <row r="286" spans="1:9" ht="15.6">
       <c r="A286" s="17"/>
       <c r="B286" s="17" t="s">
         <v>21</v>
@@ -17872,7 +17872,7 @@
       </c>
       <c r="I286" s="17"/>
     </row>
-    <row r="287" spans="1:9" ht="15">
+    <row r="287" spans="1:9" ht="15.6">
       <c r="A287" s="17"/>
       <c r="B287" s="17" t="s">
         <v>21</v>
@@ -17895,7 +17895,7 @@
       </c>
       <c r="I287" s="17"/>
     </row>
-    <row r="288" spans="1:9" ht="15">
+    <row r="288" spans="1:9" ht="15.6">
       <c r="A288" s="17" t="b">
         <v>0</v>
       </c>
@@ -17914,7 +17914,7 @@
       <c r="H288" s="17"/>
       <c r="I288" s="17"/>
     </row>
-    <row r="289" spans="1:9" ht="15">
+    <row r="289" spans="1:9" ht="15.6">
       <c r="A289" s="17"/>
       <c r="B289" s="17" t="s">
         <v>21</v>
@@ -17937,7 +17937,7 @@
       </c>
       <c r="I289" s="17"/>
     </row>
-    <row r="290" spans="1:9" ht="15">
+    <row r="290" spans="1:9" ht="15.6">
       <c r="A290" s="17" t="b">
         <v>0</v>
       </c>
@@ -17956,7 +17956,7 @@
       <c r="H290" s="17"/>
       <c r="I290" s="17"/>
     </row>
-    <row r="291" spans="1:9" ht="15">
+    <row r="291" spans="1:9" ht="15.6">
       <c r="A291" s="17"/>
       <c r="B291" s="17" t="s">
         <v>21</v>
@@ -17977,7 +17977,7 @@
       <c r="H291" s="17"/>
       <c r="I291" s="17"/>
     </row>
-    <row r="292" spans="1:9" ht="15">
+    <row r="292" spans="1:9" ht="15.6">
       <c r="A292" s="17" t="b">
         <v>0</v>
       </c>
@@ -17996,7 +17996,7 @@
       <c r="H292" s="17"/>
       <c r="I292" s="17"/>
     </row>
-    <row r="293" spans="1:9" ht="15">
+    <row r="293" spans="1:9" ht="15.6">
       <c r="A293" s="17"/>
       <c r="B293" s="17" t="s">
         <v>21</v>
@@ -18017,7 +18017,7 @@
       <c r="H293" s="17"/>
       <c r="I293" s="17"/>
     </row>
-    <row r="294" spans="1:9" ht="15">
+    <row r="294" spans="1:9" ht="15.6">
       <c r="A294" s="17" t="b">
         <v>0</v>
       </c>
@@ -18036,7 +18036,7 @@
       <c r="H294" s="17"/>
       <c r="I294" s="17"/>
     </row>
-    <row r="295" spans="1:9" ht="15">
+    <row r="295" spans="1:9" ht="15.6">
       <c r="A295" s="17"/>
       <c r="B295" s="17" t="s">
         <v>21</v>
@@ -18057,7 +18057,7 @@
       <c r="H295" s="17"/>
       <c r="I295" s="17"/>
     </row>
-    <row r="296" spans="1:9" ht="15">
+    <row r="296" spans="1:9" ht="15.6">
       <c r="A296" s="17" t="b">
         <v>0</v>
       </c>
@@ -18076,7 +18076,7 @@
       <c r="H296" s="17"/>
       <c r="I296" s="17"/>
     </row>
-    <row r="297" spans="1:9" ht="15">
+    <row r="297" spans="1:9" ht="15.6">
       <c r="A297" s="17"/>
       <c r="B297" s="17" t="s">
         <v>21</v>
@@ -18099,7 +18099,7 @@
       </c>
       <c r="I297" s="17"/>
     </row>
-    <row r="298" spans="1:9" ht="15">
+    <row r="298" spans="1:9" ht="15.6">
       <c r="A298" s="17" t="b">
         <v>0</v>
       </c>
@@ -18118,7 +18118,7 @@
       <c r="H298" s="17"/>
       <c r="I298" s="17"/>
     </row>
-    <row r="299" spans="1:9" ht="15">
+    <row r="299" spans="1:9" ht="15.6">
       <c r="A299" s="17"/>
       <c r="B299" s="17" t="s">
         <v>21</v>
@@ -18143,7 +18143,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15">
+    <row r="300" spans="1:9" ht="15.6">
       <c r="A300" s="17"/>
       <c r="B300" s="17" t="s">
         <v>21</v>
@@ -18166,7 +18166,7 @@
       </c>
       <c r="I300" s="17"/>
     </row>
-    <row r="301" spans="1:9" ht="15">
+    <row r="301" spans="1:9" ht="15.6">
       <c r="A301" s="17"/>
       <c r="B301" s="17" t="s">
         <v>21</v>
@@ -18189,7 +18189,7 @@
       </c>
       <c r="I301" s="17"/>
     </row>
-    <row r="302" spans="1:9" ht="15">
+    <row r="302" spans="1:9" ht="15.6">
       <c r="A302" s="17"/>
       <c r="B302" s="17" t="s">
         <v>21</v>
@@ -18212,7 +18212,7 @@
       </c>
       <c r="I302" s="17"/>
     </row>
-    <row r="303" spans="1:9" ht="15">
+    <row r="303" spans="1:9" ht="15.6">
       <c r="A303" s="17"/>
       <c r="B303" s="17" t="s">
         <v>21</v>
@@ -18235,7 +18235,7 @@
       </c>
       <c r="I303" s="17"/>
     </row>
-    <row r="304" spans="1:9" ht="15">
+    <row r="304" spans="1:9" ht="15.6">
       <c r="A304" s="17"/>
       <c r="B304" s="17" t="s">
         <v>21</v>
@@ -18258,7 +18258,7 @@
       </c>
       <c r="I304" s="17"/>
     </row>
-    <row r="305" spans="1:9" ht="15">
+    <row r="305" spans="1:9" ht="15.6">
       <c r="A305" s="17"/>
       <c r="B305" s="17" t="s">
         <v>21</v>
@@ -18281,7 +18281,7 @@
       </c>
       <c r="I305" s="17"/>
     </row>
-    <row r="306" spans="1:9" ht="15">
+    <row r="306" spans="1:9" ht="15.6">
       <c r="A306" s="17"/>
       <c r="B306" s="17" t="s">
         <v>21</v>
@@ -18304,7 +18304,7 @@
       </c>
       <c r="I306" s="17"/>
     </row>
-    <row r="307" spans="1:9" ht="15">
+    <row r="307" spans="1:9" ht="15.6">
       <c r="A307" s="17"/>
       <c r="B307" s="17" t="s">
         <v>21</v>
@@ -18327,7 +18327,7 @@
       </c>
       <c r="I307" s="17"/>
     </row>
-    <row r="308" spans="1:9" ht="15">
+    <row r="308" spans="1:9" ht="15.6">
       <c r="A308" s="17" t="b">
         <v>0</v>
       </c>
@@ -18346,7 +18346,7 @@
       <c r="H308" s="17"/>
       <c r="I308" s="17"/>
     </row>
-    <row r="309" spans="1:9" ht="15">
+    <row r="309" spans="1:9" ht="15.6">
       <c r="A309" s="17"/>
       <c r="B309" s="17" t="s">
         <v>21</v>
@@ -18369,7 +18369,7 @@
       </c>
       <c r="I309" s="17"/>
     </row>
-    <row r="310" spans="1:9" ht="15">
+    <row r="310" spans="1:9" ht="15.6">
       <c r="A310" s="17"/>
       <c r="B310" s="17" t="s">
         <v>21</v>
@@ -18392,7 +18392,7 @@
       </c>
       <c r="I310" s="17"/>
     </row>
-    <row r="311" spans="1:9" ht="15">
+    <row r="311" spans="1:9" ht="15.6">
       <c r="A311" s="17"/>
       <c r="B311" s="17" t="s">
         <v>21</v>
@@ -18415,7 +18415,7 @@
       </c>
       <c r="I311" s="17"/>
     </row>
-    <row r="312" spans="1:9" ht="15">
+    <row r="312" spans="1:9" ht="15.6">
       <c r="A312" s="17"/>
       <c r="B312" s="17" t="s">
         <v>21</v>
@@ -18438,7 +18438,7 @@
       </c>
       <c r="I312" s="17"/>
     </row>
-    <row r="313" spans="1:9" ht="15">
+    <row r="313" spans="1:9" ht="15.6">
       <c r="A313" s="17" t="b">
         <v>0</v>
       </c>
@@ -18457,7 +18457,7 @@
       <c r="H313" s="17"/>
       <c r="I313" s="17"/>
     </row>
-    <row r="314" spans="1:9" ht="15">
+    <row r="314" spans="1:9" ht="15.6">
       <c r="A314" s="17"/>
       <c r="B314" s="17" t="s">
         <v>21</v>
@@ -18480,7 +18480,7 @@
       </c>
       <c r="I314" s="17"/>
     </row>
-    <row r="315" spans="1:9" ht="15">
+    <row r="315" spans="1:9" ht="15.6">
       <c r="A315" s="17"/>
       <c r="B315" s="17" t="s">
         <v>21</v>
@@ -18503,7 +18503,7 @@
       </c>
       <c r="I315" s="17"/>
     </row>
-    <row r="316" spans="1:9" ht="15">
+    <row r="316" spans="1:9" ht="15.6">
       <c r="A316" s="17"/>
       <c r="B316" s="17" t="s">
         <v>21</v>
@@ -18528,7 +18528,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15">
+    <row r="317" spans="1:9" ht="15.6">
       <c r="A317" s="17" t="b">
         <v>0</v>
       </c>
@@ -18547,7 +18547,7 @@
       <c r="H317" s="17"/>
       <c r="I317" s="17"/>
     </row>
-    <row r="318" spans="1:9" ht="15">
+    <row r="318" spans="1:9" ht="15.6">
       <c r="A318" s="17"/>
       <c r="B318" s="17" t="s">
         <v>21</v>
@@ -18572,7 +18572,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15">
+    <row r="319" spans="1:9" ht="15.6">
       <c r="A319" s="17"/>
       <c r="B319" s="17" t="s">
         <v>21</v>
@@ -18595,7 +18595,7 @@
       </c>
       <c r="I319" s="17"/>
     </row>
-    <row r="320" spans="1:9" ht="15">
+    <row r="320" spans="1:9" ht="15.6">
       <c r="A320" s="17" t="b">
         <v>0</v>
       </c>
@@ -18614,7 +18614,7 @@
       <c r="H320" s="17"/>
       <c r="I320" s="17"/>
     </row>
-    <row r="321" spans="1:9" ht="15">
+    <row r="321" spans="1:9" ht="15.6">
       <c r="A321" s="17"/>
       <c r="B321" s="17" t="s">
         <v>21</v>
@@ -18635,7 +18635,7 @@
       <c r="H321" s="17"/>
       <c r="I321" s="17"/>
     </row>
-    <row r="322" spans="1:9" ht="15">
+    <row r="322" spans="1:9" ht="15.6">
       <c r="A322" s="17"/>
       <c r="B322" s="17" t="s">
         <v>21</v>
@@ -18656,7 +18656,7 @@
       <c r="H322" s="17"/>
       <c r="I322" s="17"/>
     </row>
-    <row r="323" spans="1:9" ht="15">
+    <row r="323" spans="1:9" ht="15.6">
       <c r="A323" s="17"/>
       <c r="B323" s="17" t="s">
         <v>21</v>
@@ -18679,7 +18679,7 @@
       </c>
       <c r="I323" s="17"/>
     </row>
-    <row r="324" spans="1:9" ht="15">
+    <row r="324" spans="1:9" ht="15.6">
       <c r="A324" s="17" t="b">
         <v>0</v>
       </c>
@@ -18698,7 +18698,7 @@
       <c r="H324" s="17"/>
       <c r="I324" s="17"/>
     </row>
-    <row r="325" spans="1:9" ht="15">
+    <row r="325" spans="1:9" ht="15.6">
       <c r="A325" s="17" t="b">
         <v>0</v>
       </c>
@@ -18717,7 +18717,7 @@
       <c r="H325" s="17"/>
       <c r="I325" s="17"/>
     </row>
-    <row r="326" spans="1:9" ht="15">
+    <row r="326" spans="1:9" ht="15.6">
       <c r="A326" s="17"/>
       <c r="B326" s="17" t="s">
         <v>21</v>
@@ -18742,7 +18742,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15">
+    <row r="327" spans="1:9" ht="15.6">
       <c r="A327" s="17"/>
       <c r="B327" s="17" t="s">
         <v>21</v>
@@ -19099,7 +19099,7 @@
       <c r="O343" s="1"/>
       <c r="P343" s="1"/>
     </row>
-    <row r="344" spans="1:16" ht="15">
+    <row r="344" spans="1:16" ht="15.6">
       <c r="A344" s="17"/>
       <c r="B344" t="s">
         <v>21</v>
@@ -19462,7 +19462,7 @@
       <c r="J361"/>
       <c r="K361"/>
     </row>
-    <row r="362" spans="1:18" s="1" customFormat="1" ht="15">
+    <row r="362" spans="1:18" s="1" customFormat="1" ht="15.6">
       <c r="A362" s="17"/>
       <c r="B362" t="s">
         <v>22</v>
@@ -19590,14 +19590,14 @@
       <selection activeCell="A17" sqref="A17:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
-    <col min="17" max="17" width="24.5" customWidth="1"/>
+    <col min="17" max="17" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">

</xml_diff>

<commit_message>
updated algorithm params and delta_x
</commit_message>
<xml_diff>
--- a/projects/office_calibration.xlsx
+++ b/projects/office_calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="13170" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -6893,17 +6893,17 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="81.7109375" customWidth="1"/>
+    <col min="1" max="1" width="81.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="45">
+    <row r="1" spans="1:1" ht="28.8">
       <c r="A1" s="36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="30">
+    <row r="2" spans="1:1" ht="28.8">
       <c r="A2" s="36" t="s">
         <v>41</v>
       </c>
@@ -6923,18 +6923,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="1"/>
+    <col min="4" max="4" width="33.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="61.6640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6966,7 +6966,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
+    <row r="4" spans="1:5" ht="28.8">
       <c r="A4" s="1" t="s">
         <v>456</v>
       </c>
@@ -6977,7 +6977,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="75">
+    <row r="5" spans="1:5" ht="72">
       <c r="A5" s="1" t="s">
         <v>469</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="46.15" customHeight="1">
+    <row r="6" spans="1:5" ht="46.2" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>470</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5" ht="28.8">
       <c r="A7" s="1" t="s">
         <v>442</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="1" t="s">
         <v>443</v>
       </c>
@@ -7103,7 +7103,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="1" t="s">
         <v>463</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="60">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="57.6">
       <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
@@ -7161,7 +7161,7 @@
       <c r="B22" s="26"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="60">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="57.6">
       <c r="A23" s="11" t="s">
         <v>450</v>
       </c>
@@ -7207,7 +7207,7 @@
         <v>557</v>
       </c>
       <c r="B26" s="29">
-        <v>900360000000000</v>
+        <v>450360000000000</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>575</v>
@@ -7219,7 +7219,7 @@
         <v>558</v>
       </c>
       <c r="B27" s="30">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>574</v>
@@ -7285,7 +7285,7 @@
       <c r="C35" s="26"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="45">
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="43.2">
       <c r="A36" s="11" t="s">
         <v>33</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="30">
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8">
       <c r="A39" s="11" t="s">
         <v>30</v>
       </c>
@@ -7335,7 +7335,7 @@
       </c>
       <c r="E40" s="2"/>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="60">
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="57.6">
       <c r="A42" s="11" t="s">
         <v>35</v>
       </c>
@@ -7391,37 +7391,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N72" sqref="N72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="31" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="31" customWidth="1"/>
     <col min="2" max="2" width="47" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="31" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="31" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="31" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="31" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" style="31" customWidth="1"/>
-    <col min="13" max="14" width="7.7109375" style="31" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="31"/>
-    <col min="16" max="16" width="11.42578125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" style="31" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" style="31" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" style="31" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" style="31" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" style="31" customWidth="1"/>
+    <col min="13" max="14" width="7.6640625" style="31" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" style="31"/>
+    <col min="16" max="16" width="11.44140625" style="31" customWidth="1"/>
     <col min="17" max="17" width="23" style="31" customWidth="1"/>
-    <col min="18" max="18" width="27.7109375" style="31" customWidth="1"/>
-    <col min="19" max="19" width="46.140625" style="31" customWidth="1"/>
-    <col min="20" max="22" width="11.42578125" style="31"/>
-    <col min="23" max="23" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="11.42578125" style="31"/>
+    <col min="18" max="18" width="27.6640625" style="31" customWidth="1"/>
+    <col min="19" max="19" width="46.109375" style="31" customWidth="1"/>
+    <col min="20" max="22" width="11.44140625" style="31"/>
+    <col min="23" max="23" width="13.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="11.44140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18.75">
+    <row r="1" spans="1:25" ht="18">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7456,7 +7456,7 @@
       <c r="X1" s="53"/>
       <c r="Y1" s="53"/>
     </row>
-    <row r="2" spans="1:25" s="8" customFormat="1" ht="15.75">
+    <row r="2" spans="1:25" s="8" customFormat="1" ht="15.6">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -7472,7 +7472,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:25" s="14" customFormat="1" ht="63">
+    <row r="3" spans="1:25" s="14" customFormat="1" ht="62.4">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -7739,7 +7739,7 @@
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
     </row>
-    <row r="14" spans="1:25" ht="18">
+    <row r="14" spans="1:25" ht="17.399999999999999">
       <c r="A14" s="30"/>
       <c r="B14" s="30" t="s">
         <v>21</v>
@@ -8921,7 +8921,7 @@
         <v>0.14166666666666669</v>
       </c>
       <c r="N64" s="43">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="Q64" s="43" t="s">
         <v>773</v>
@@ -9011,7 +9011,7 @@
         <v>0.14166666666666669</v>
       </c>
       <c r="N68" s="43">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="Q68" s="43" t="s">
         <v>773</v>
@@ -9101,7 +9101,7 @@
         <v>0.14166666666666669</v>
       </c>
       <c r="N72" s="43">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="Q72" s="43" t="s">
         <v>773</v>
@@ -10552,20 +10552,20 @@
       <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="29.42578125" style="31" customWidth="1"/>
+    <col min="1" max="2" width="29.44140625" style="31" customWidth="1"/>
     <col min="3" max="3" width="71" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="31" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.42578125" style="31" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="31" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="31" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="31" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="31"/>
+    <col min="4" max="4" width="10.44140625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.44140625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="31" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="31" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="31" customWidth="1"/>
+    <col min="11" max="16384" width="11.44140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75">
+    <row r="1" spans="1:12" ht="18">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -10580,7 +10580,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="15.75">
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="15.6">
       <c r="A2" s="8" t="s">
         <v>459</v>
       </c>
@@ -10615,7 +10615,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="47.25">
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="46.8">
       <c r="A3" s="14" t="s">
         <v>628</v>
       </c>
@@ -11629,19 +11629,19 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:9" ht="15.6">
       <c r="A1" s="17" t="b">
         <v>0</v>
       </c>
@@ -11660,7 +11660,7 @@
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75">
+    <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="17"/>
       <c r="B2" s="17" t="s">
         <v>21</v>
@@ -11681,7 +11681,7 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75">
+    <row r="3" spans="1:9" ht="15.6">
       <c r="A3" s="17"/>
       <c r="B3" s="17" t="s">
         <v>21</v>
@@ -11704,7 +11704,7 @@
       </c>
       <c r="I3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75">
+    <row r="4" spans="1:9" ht="15.6">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>21</v>
@@ -11727,7 +11727,7 @@
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.6">
       <c r="A5" s="17"/>
       <c r="B5" s="17" t="s">
         <v>21</v>
@@ -11750,7 +11750,7 @@
       </c>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:9" ht="15.6">
       <c r="A6" s="17"/>
       <c r="B6" s="17" t="s">
         <v>21</v>
@@ -11773,7 +11773,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:9" ht="15.6">
       <c r="A7" s="17"/>
       <c r="B7" s="17" t="s">
         <v>21</v>
@@ -11796,7 +11796,7 @@
       </c>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:9" ht="15.6">
       <c r="A8" s="17"/>
       <c r="B8" s="17" t="s">
         <v>21</v>
@@ -11819,7 +11819,7 @@
       </c>
       <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75">
+    <row r="9" spans="1:9" ht="15.6">
       <c r="A9" s="17"/>
       <c r="B9" s="17" t="s">
         <v>21</v>
@@ -11842,7 +11842,7 @@
       </c>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75">
+    <row r="10" spans="1:9" ht="15.6">
       <c r="A10" s="17"/>
       <c r="B10" s="17" t="s">
         <v>21</v>
@@ -11865,7 +11865,7 @@
       </c>
       <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75">
+    <row r="11" spans="1:9" ht="15.6">
       <c r="A11" s="17" t="b">
         <v>0</v>
       </c>
@@ -11884,7 +11884,7 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75">
+    <row r="12" spans="1:9" ht="15.6">
       <c r="A12" s="17"/>
       <c r="B12" s="17" t="s">
         <v>21</v>
@@ -11905,7 +11905,7 @@
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75">
+    <row r="13" spans="1:9" ht="15.6">
       <c r="A13" s="17"/>
       <c r="B13" s="17" t="s">
         <v>21</v>
@@ -11928,7 +11928,7 @@
       </c>
       <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75">
+    <row r="14" spans="1:9" ht="15.6">
       <c r="A14" s="17"/>
       <c r="B14" s="17" t="s">
         <v>21</v>
@@ -11951,7 +11951,7 @@
       </c>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75">
+    <row r="15" spans="1:9" ht="15.6">
       <c r="A15" s="17"/>
       <c r="B15" s="17" t="s">
         <v>21</v>
@@ -11974,7 +11974,7 @@
       </c>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75">
+    <row r="16" spans="1:9" ht="15.6">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
         <v>21</v>
@@ -11997,7 +11997,7 @@
       </c>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75">
+    <row r="17" spans="1:9" ht="15.6">
       <c r="A17" s="17"/>
       <c r="B17" s="17" t="s">
         <v>21</v>
@@ -12020,7 +12020,7 @@
       </c>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75">
+    <row r="18" spans="1:9" ht="15.6">
       <c r="A18" s="17"/>
       <c r="B18" s="17" t="s">
         <v>21</v>
@@ -12043,7 +12043,7 @@
       </c>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75">
+    <row r="19" spans="1:9" ht="15.6">
       <c r="A19" s="17"/>
       <c r="B19" s="17" t="s">
         <v>21</v>
@@ -12066,7 +12066,7 @@
       </c>
       <c r="I19" s="17"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75">
+    <row r="20" spans="1:9" ht="15.6">
       <c r="A20" s="17"/>
       <c r="B20" s="17" t="s">
         <v>21</v>
@@ -12089,7 +12089,7 @@
       </c>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75">
+    <row r="21" spans="1:9" ht="15.6">
       <c r="A21" s="17" t="b">
         <v>0</v>
       </c>
@@ -12108,7 +12108,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75">
+    <row r="22" spans="1:9" ht="15.6">
       <c r="A22" s="17"/>
       <c r="B22" s="17" t="s">
         <v>21</v>
@@ -12131,7 +12131,7 @@
       </c>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75">
+    <row r="23" spans="1:9" ht="15.6">
       <c r="A23" s="17"/>
       <c r="B23" s="17" t="s">
         <v>21</v>
@@ -12154,7 +12154,7 @@
       </c>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75">
+    <row r="24" spans="1:9" ht="15.6">
       <c r="A24" s="17"/>
       <c r="B24" s="17" t="s">
         <v>21</v>
@@ -12177,7 +12177,7 @@
       </c>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75">
+    <row r="25" spans="1:9" ht="15.6">
       <c r="A25" s="17"/>
       <c r="B25" s="17" t="s">
         <v>21</v>
@@ -12200,7 +12200,7 @@
       </c>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75">
+    <row r="26" spans="1:9" ht="15.6">
       <c r="A26" s="17"/>
       <c r="B26" s="17" t="s">
         <v>21</v>
@@ -12223,7 +12223,7 @@
       </c>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75">
+    <row r="27" spans="1:9" ht="15.6">
       <c r="A27" s="17"/>
       <c r="B27" s="17" t="s">
         <v>21</v>
@@ -12246,7 +12246,7 @@
       </c>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75">
+    <row r="28" spans="1:9" ht="15.6">
       <c r="A28" s="17"/>
       <c r="B28" s="17" t="s">
         <v>21</v>
@@ -12269,7 +12269,7 @@
       </c>
       <c r="I28" s="17"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75">
+    <row r="29" spans="1:9" ht="15.6">
       <c r="A29" s="17"/>
       <c r="B29" s="17" t="s">
         <v>21</v>
@@ -12292,7 +12292,7 @@
       </c>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75">
+    <row r="30" spans="1:9" ht="15.6">
       <c r="A30" s="17"/>
       <c r="B30" s="17" t="s">
         <v>21</v>
@@ -12315,7 +12315,7 @@
       </c>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75">
+    <row r="31" spans="1:9" ht="15.6">
       <c r="A31" s="17" t="b">
         <v>0</v>
       </c>
@@ -12334,7 +12334,7 @@
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75">
+    <row r="32" spans="1:9" ht="15.6">
       <c r="A32" s="17"/>
       <c r="B32" s="17" t="s">
         <v>21</v>
@@ -12355,7 +12355,7 @@
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75">
+    <row r="33" spans="1:9" ht="15.6">
       <c r="A33" s="17"/>
       <c r="B33" s="17" t="s">
         <v>21</v>
@@ -12378,7 +12378,7 @@
       </c>
       <c r="I33" s="17"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75">
+    <row r="34" spans="1:9" ht="15.6">
       <c r="A34" s="17"/>
       <c r="B34" s="17" t="s">
         <v>21</v>
@@ -12401,7 +12401,7 @@
       </c>
       <c r="I34" s="17"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75">
+    <row r="35" spans="1:9" ht="15.6">
       <c r="A35" s="17"/>
       <c r="B35" s="17" t="s">
         <v>21</v>
@@ -12424,7 +12424,7 @@
       </c>
       <c r="I35" s="17"/>
     </row>
-    <row r="36" spans="1:9" ht="15.75">
+    <row r="36" spans="1:9" ht="15.6">
       <c r="A36" s="17"/>
       <c r="B36" s="17" t="s">
         <v>21</v>
@@ -12447,7 +12447,7 @@
       </c>
       <c r="I36" s="17"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75">
+    <row r="37" spans="1:9" ht="15.6">
       <c r="A37" s="17"/>
       <c r="B37" s="17" t="s">
         <v>21</v>
@@ -12470,7 +12470,7 @@
       </c>
       <c r="I37" s="17"/>
     </row>
-    <row r="38" spans="1:9" ht="15.75">
+    <row r="38" spans="1:9" ht="15.6">
       <c r="A38" s="17"/>
       <c r="B38" s="17" t="s">
         <v>21</v>
@@ -12493,7 +12493,7 @@
       </c>
       <c r="I38" s="17"/>
     </row>
-    <row r="39" spans="1:9" ht="15.75">
+    <row r="39" spans="1:9" ht="15.6">
       <c r="A39" s="17"/>
       <c r="B39" s="17" t="s">
         <v>21</v>
@@ -12516,7 +12516,7 @@
       </c>
       <c r="I39" s="17"/>
     </row>
-    <row r="40" spans="1:9" ht="15.75">
+    <row r="40" spans="1:9" ht="15.6">
       <c r="A40" s="17"/>
       <c r="B40" s="17" t="s">
         <v>21</v>
@@ -12539,7 +12539,7 @@
       </c>
       <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75">
+    <row r="41" spans="1:9" ht="15.6">
       <c r="A41" s="17" t="b">
         <v>0</v>
       </c>
@@ -12558,7 +12558,7 @@
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="1:9" ht="15.75">
+    <row r="42" spans="1:9" ht="15.6">
       <c r="A42" s="17"/>
       <c r="B42" s="17" t="s">
         <v>21</v>
@@ -12579,7 +12579,7 @@
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" ht="15.75">
+    <row r="43" spans="1:9" ht="15.6">
       <c r="A43" s="17"/>
       <c r="B43" s="17" t="s">
         <v>21</v>
@@ -12602,7 +12602,7 @@
       </c>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" ht="15.75">
+    <row r="44" spans="1:9" ht="15.6">
       <c r="A44" s="17"/>
       <c r="B44" s="17" t="s">
         <v>21</v>
@@ -12625,7 +12625,7 @@
       </c>
       <c r="I44" s="17"/>
     </row>
-    <row r="45" spans="1:9" ht="15.75">
+    <row r="45" spans="1:9" ht="15.6">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>21</v>
@@ -12648,7 +12648,7 @@
       </c>
       <c r="I45" s="17"/>
     </row>
-    <row r="46" spans="1:9" ht="15.75">
+    <row r="46" spans="1:9" ht="15.6">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
         <v>21</v>
@@ -12671,7 +12671,7 @@
       </c>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="1:9" ht="15.75">
+    <row r="47" spans="1:9" ht="15.6">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
         <v>21</v>
@@ -12694,7 +12694,7 @@
       </c>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="1:9" ht="15.75">
+    <row r="48" spans="1:9" ht="15.6">
       <c r="A48" s="17"/>
       <c r="B48" s="17" t="s">
         <v>21</v>
@@ -12717,7 +12717,7 @@
       </c>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75">
+    <row r="49" spans="1:9" ht="15.6">
       <c r="A49" s="17"/>
       <c r="B49" s="17" t="s">
         <v>21</v>
@@ -12740,7 +12740,7 @@
       </c>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75">
+    <row r="50" spans="1:9" ht="15.6">
       <c r="A50" s="17"/>
       <c r="B50" s="17" t="s">
         <v>21</v>
@@ -12763,7 +12763,7 @@
       </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75">
+    <row r="51" spans="1:9" ht="15.6">
       <c r="A51" s="17" t="b">
         <v>0</v>
       </c>
@@ -12782,7 +12782,7 @@
       <c r="H51" s="17"/>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75">
+    <row r="52" spans="1:9" ht="15.6">
       <c r="A52" s="17"/>
       <c r="B52" s="17" t="s">
         <v>21</v>
@@ -12803,7 +12803,7 @@
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75">
+    <row r="53" spans="1:9" ht="15.6">
       <c r="A53" s="17"/>
       <c r="B53" s="17" t="s">
         <v>21</v>
@@ -12826,7 +12826,7 @@
       </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75">
+    <row r="54" spans="1:9" ht="15.6">
       <c r="A54" s="17"/>
       <c r="B54" s="17" t="s">
         <v>21</v>
@@ -12849,7 +12849,7 @@
       </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="15.75">
+    <row r="55" spans="1:9" ht="15.6">
       <c r="A55" s="17"/>
       <c r="B55" s="17" t="s">
         <v>21</v>
@@ -12872,7 +12872,7 @@
       </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="15.75">
+    <row r="56" spans="1:9" ht="15.6">
       <c r="A56" s="17"/>
       <c r="B56" s="17" t="s">
         <v>21</v>
@@ -12895,7 +12895,7 @@
       </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="15.75">
+    <row r="57" spans="1:9" ht="15.6">
       <c r="A57" s="17"/>
       <c r="B57" s="17" t="s">
         <v>21</v>
@@ -12918,7 +12918,7 @@
       </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75">
+    <row r="58" spans="1:9" ht="15.6">
       <c r="A58" s="17"/>
       <c r="B58" s="17" t="s">
         <v>21</v>
@@ -12941,7 +12941,7 @@
       </c>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="15.75">
+    <row r="59" spans="1:9" ht="15.6">
       <c r="A59" s="17"/>
       <c r="B59" s="17" t="s">
         <v>21</v>
@@ -12964,7 +12964,7 @@
       </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="15.75">
+    <row r="60" spans="1:9" ht="15.6">
       <c r="A60" s="17"/>
       <c r="B60" s="17" t="s">
         <v>21</v>
@@ -12987,7 +12987,7 @@
       </c>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="15.75">
+    <row r="61" spans="1:9" ht="15.6">
       <c r="A61" s="17" t="b">
         <v>0</v>
       </c>
@@ -13006,7 +13006,7 @@
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="15.75">
+    <row r="62" spans="1:9" ht="15.6">
       <c r="A62" s="17"/>
       <c r="B62" s="17" t="s">
         <v>21</v>
@@ -13027,7 +13027,7 @@
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75">
+    <row r="63" spans="1:9" ht="15.6">
       <c r="A63" s="17"/>
       <c r="B63" s="17" t="s">
         <v>21</v>
@@ -13052,7 +13052,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.75">
+    <row r="64" spans="1:9" ht="15.6">
       <c r="A64" s="17"/>
       <c r="B64" s="17" t="s">
         <v>21</v>
@@ -13075,7 +13075,7 @@
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" ht="15.75">
+    <row r="65" spans="1:9" ht="15.6">
       <c r="A65" s="17"/>
       <c r="B65" s="17" t="s">
         <v>21</v>
@@ -13098,7 +13098,7 @@
       </c>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" ht="15.75">
+    <row r="66" spans="1:9" ht="15.6">
       <c r="A66" s="17"/>
       <c r="B66" s="17" t="s">
         <v>21</v>
@@ -13121,7 +13121,7 @@
       </c>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" ht="15.75">
+    <row r="67" spans="1:9" ht="15.6">
       <c r="A67" s="17"/>
       <c r="B67" s="17" t="s">
         <v>21</v>
@@ -13144,7 +13144,7 @@
       </c>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" ht="15.75">
+    <row r="68" spans="1:9" ht="15.6">
       <c r="A68" s="17"/>
       <c r="B68" s="17" t="s">
         <v>21</v>
@@ -13167,7 +13167,7 @@
       </c>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" ht="15.75">
+    <row r="69" spans="1:9" ht="15.6">
       <c r="A69" s="17"/>
       <c r="B69" s="17" t="s">
         <v>21</v>
@@ -13190,7 +13190,7 @@
       </c>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" ht="15.75">
+    <row r="70" spans="1:9" ht="15.6">
       <c r="A70" s="17"/>
       <c r="B70" s="17" t="s">
         <v>21</v>
@@ -13213,7 +13213,7 @@
       </c>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" ht="15.75">
+    <row r="71" spans="1:9" ht="15.6">
       <c r="A71" s="17"/>
       <c r="B71" s="17" t="s">
         <v>21</v>
@@ -13236,7 +13236,7 @@
       </c>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" ht="15.75">
+    <row r="72" spans="1:9" ht="15.6">
       <c r="A72" s="17" t="b">
         <v>0</v>
       </c>
@@ -13255,7 +13255,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" ht="15.75">
+    <row r="73" spans="1:9" ht="15.6">
       <c r="A73" s="17"/>
       <c r="B73" s="17" t="s">
         <v>21</v>
@@ -13276,7 +13276,7 @@
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" ht="15.75">
+    <row r="74" spans="1:9" ht="15.6">
       <c r="A74" s="17"/>
       <c r="B74" s="17" t="s">
         <v>21</v>
@@ -13299,7 +13299,7 @@
       </c>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" ht="15.75">
+    <row r="75" spans="1:9" ht="15.6">
       <c r="A75" s="17"/>
       <c r="B75" s="17" t="s">
         <v>21</v>
@@ -13324,7 +13324,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.75">
+    <row r="76" spans="1:9" ht="15.6">
       <c r="A76" s="17"/>
       <c r="B76" s="17" t="s">
         <v>21</v>
@@ -13347,7 +13347,7 @@
       </c>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" ht="15.75">
+    <row r="77" spans="1:9" ht="15.6">
       <c r="A77" s="17"/>
       <c r="B77" s="17" t="s">
         <v>21</v>
@@ -13370,7 +13370,7 @@
       </c>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" ht="15.75">
+    <row r="78" spans="1:9" ht="15.6">
       <c r="A78" s="17"/>
       <c r="B78" s="17" t="s">
         <v>21</v>
@@ -13393,7 +13393,7 @@
       </c>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" ht="15.75">
+    <row r="79" spans="1:9" ht="15.6">
       <c r="A79" s="17"/>
       <c r="B79" s="17" t="s">
         <v>21</v>
@@ -13416,7 +13416,7 @@
       </c>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" ht="15.75">
+    <row r="80" spans="1:9" ht="15.6">
       <c r="A80" s="17"/>
       <c r="B80" s="17" t="s">
         <v>21</v>
@@ -13439,7 +13439,7 @@
       </c>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" ht="15.75">
+    <row r="81" spans="1:9" ht="15.6">
       <c r="A81" s="17"/>
       <c r="B81" s="17" t="s">
         <v>21</v>
@@ -13462,7 +13462,7 @@
       </c>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" ht="15.75">
+    <row r="82" spans="1:9" ht="15.6">
       <c r="A82" s="17"/>
       <c r="B82" s="17" t="s">
         <v>21</v>
@@ -13485,7 +13485,7 @@
       </c>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" ht="15.75">
+    <row r="83" spans="1:9" ht="15.6">
       <c r="A83" s="17"/>
       <c r="B83" s="17" t="s">
         <v>21</v>
@@ -13508,7 +13508,7 @@
       </c>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" ht="15.75">
+    <row r="84" spans="1:9" ht="15.6">
       <c r="A84" s="17"/>
       <c r="B84" s="17" t="s">
         <v>21</v>
@@ -13531,7 +13531,7 @@
       </c>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" ht="15.75">
+    <row r="85" spans="1:9" ht="15.6">
       <c r="A85" s="17"/>
       <c r="B85" s="17" t="s">
         <v>21</v>
@@ -13554,7 +13554,7 @@
       </c>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" ht="15.75">
+    <row r="86" spans="1:9" ht="15.6">
       <c r="A86" s="17" t="b">
         <v>0</v>
       </c>
@@ -13573,7 +13573,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" ht="15.75">
+    <row r="87" spans="1:9" ht="15.6">
       <c r="A87" s="17"/>
       <c r="B87" s="17" t="s">
         <v>21</v>
@@ -13596,7 +13596,7 @@
       </c>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" ht="15.75">
+    <row r="88" spans="1:9" ht="15.6">
       <c r="A88" s="17"/>
       <c r="B88" s="17" t="s">
         <v>21</v>
@@ -13619,7 +13619,7 @@
       </c>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" ht="15.75">
+    <row r="89" spans="1:9" ht="15.6">
       <c r="A89" s="17"/>
       <c r="B89" s="17" t="s">
         <v>21</v>
@@ -13642,7 +13642,7 @@
       </c>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" ht="15.75">
+    <row r="90" spans="1:9" ht="15.6">
       <c r="A90" s="17"/>
       <c r="B90" s="17" t="s">
         <v>21</v>
@@ -13665,7 +13665,7 @@
       </c>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" ht="15.75">
+    <row r="91" spans="1:9" ht="15.6">
       <c r="A91" s="17"/>
       <c r="B91" s="17" t="s">
         <v>21</v>
@@ -13688,7 +13688,7 @@
       </c>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" ht="15.75">
+    <row r="92" spans="1:9" ht="15.6">
       <c r="A92" s="17"/>
       <c r="B92" s="17" t="s">
         <v>21</v>
@@ -13711,7 +13711,7 @@
       </c>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" ht="15.75">
+    <row r="93" spans="1:9" ht="15.6">
       <c r="A93" s="17"/>
       <c r="B93" s="17" t="s">
         <v>21</v>
@@ -13734,7 +13734,7 @@
       </c>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" ht="15.75">
+    <row r="94" spans="1:9" ht="15.6">
       <c r="A94" s="17"/>
       <c r="B94" s="17" t="s">
         <v>21</v>
@@ -13757,7 +13757,7 @@
       </c>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" ht="15.75">
+    <row r="95" spans="1:9" ht="15.6">
       <c r="A95" s="17"/>
       <c r="B95" s="17" t="s">
         <v>21</v>
@@ -13780,7 +13780,7 @@
       </c>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" ht="15.75">
+    <row r="96" spans="1:9" ht="15.6">
       <c r="A96" s="17"/>
       <c r="B96" s="17" t="s">
         <v>21</v>
@@ -13803,7 +13803,7 @@
       </c>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" ht="15.75">
+    <row r="97" spans="1:9" ht="15.6">
       <c r="A97" s="17" t="b">
         <v>0</v>
       </c>
@@ -13822,7 +13822,7 @@
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" ht="15.75">
+    <row r="98" spans="1:9" ht="15.6">
       <c r="A98" s="17"/>
       <c r="B98" s="17" t="s">
         <v>21</v>
@@ -13847,7 +13847,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.75">
+    <row r="99" spans="1:9" ht="15.6">
       <c r="A99" s="17" t="b">
         <v>0</v>
       </c>
@@ -13866,7 +13866,7 @@
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="1:9" ht="15.75">
+    <row r="100" spans="1:9" ht="15.6">
       <c r="A100" s="17"/>
       <c r="B100" s="17" t="s">
         <v>21</v>
@@ -13887,7 +13887,7 @@
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="1:9" ht="15.75">
+    <row r="101" spans="1:9" ht="15.6">
       <c r="A101" s="17"/>
       <c r="B101" s="17" t="s">
         <v>21</v>
@@ -13912,7 +13912,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.75">
+    <row r="102" spans="1:9" ht="15.6">
       <c r="A102" s="17" t="b">
         <v>0</v>
       </c>
@@ -13931,7 +13931,7 @@
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="1:9" ht="15.75">
+    <row r="103" spans="1:9" ht="15.6">
       <c r="A103" s="17"/>
       <c r="B103" s="17" t="s">
         <v>21</v>
@@ -13954,7 +13954,7 @@
       </c>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="1:9" ht="15.75">
+    <row r="104" spans="1:9" ht="15.6">
       <c r="A104" s="17"/>
       <c r="B104" s="17" t="s">
         <v>21</v>
@@ -13979,7 +13979,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.75">
+    <row r="105" spans="1:9" ht="15.6">
       <c r="A105" s="17"/>
       <c r="B105" s="17" t="s">
         <v>21</v>
@@ -14002,7 +14002,7 @@
       </c>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="1:9" ht="15.75">
+    <row r="106" spans="1:9" ht="15.6">
       <c r="A106" s="17"/>
       <c r="B106" s="17" t="s">
         <v>21</v>
@@ -14023,7 +14023,7 @@
       <c r="H106" s="17"/>
       <c r="I106" s="17"/>
     </row>
-    <row r="107" spans="1:9" ht="15.75">
+    <row r="107" spans="1:9" ht="15.6">
       <c r="A107" s="17" t="b">
         <v>0</v>
       </c>
@@ -14042,7 +14042,7 @@
       <c r="H107" s="17"/>
       <c r="I107" s="17"/>
     </row>
-    <row r="108" spans="1:9" ht="15.75">
+    <row r="108" spans="1:9" ht="15.6">
       <c r="A108" s="17"/>
       <c r="B108" s="17" t="s">
         <v>21</v>
@@ -14067,7 +14067,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.75">
+    <row r="109" spans="1:9" ht="15.6">
       <c r="A109" s="17"/>
       <c r="B109" s="17" t="s">
         <v>21</v>
@@ -14090,7 +14090,7 @@
       </c>
       <c r="I109" s="17"/>
     </row>
-    <row r="110" spans="1:9" ht="15.75">
+    <row r="110" spans="1:9" ht="15.6">
       <c r="A110" s="17"/>
       <c r="B110" s="17" t="s">
         <v>21</v>
@@ -14113,7 +14113,7 @@
       </c>
       <c r="I110" s="17"/>
     </row>
-    <row r="111" spans="1:9" ht="15.75">
+    <row r="111" spans="1:9" ht="15.6">
       <c r="A111" s="17"/>
       <c r="B111" s="17" t="s">
         <v>21</v>
@@ -14136,7 +14136,7 @@
       </c>
       <c r="I111" s="17"/>
     </row>
-    <row r="112" spans="1:9" ht="15.75">
+    <row r="112" spans="1:9" ht="15.6">
       <c r="A112" s="17"/>
       <c r="B112" s="17" t="s">
         <v>21</v>
@@ -14159,7 +14159,7 @@
       </c>
       <c r="I112" s="17"/>
     </row>
-    <row r="113" spans="1:9" ht="15.75">
+    <row r="113" spans="1:9" ht="15.6">
       <c r="A113" s="17"/>
       <c r="B113" s="17" t="s">
         <v>21</v>
@@ -14182,7 +14182,7 @@
       </c>
       <c r="I113" s="17"/>
     </row>
-    <row r="114" spans="1:9" ht="15.75">
+    <row r="114" spans="1:9" ht="15.6">
       <c r="A114" s="17"/>
       <c r="B114" s="17" t="s">
         <v>21</v>
@@ -14205,7 +14205,7 @@
       </c>
       <c r="I114" s="17"/>
     </row>
-    <row r="115" spans="1:9" ht="15.75">
+    <row r="115" spans="1:9" ht="15.6">
       <c r="A115" s="17" t="b">
         <v>0</v>
       </c>
@@ -14224,7 +14224,7 @@
       <c r="H115" s="17"/>
       <c r="I115" s="17"/>
     </row>
-    <row r="116" spans="1:9" ht="15.75">
+    <row r="116" spans="1:9" ht="15.6">
       <c r="A116" s="17"/>
       <c r="B116" s="17" t="s">
         <v>21</v>
@@ -14247,7 +14247,7 @@
       </c>
       <c r="I116" s="17"/>
     </row>
-    <row r="117" spans="1:9" ht="15.75">
+    <row r="117" spans="1:9" ht="15.6">
       <c r="A117" s="17"/>
       <c r="B117" s="17" t="s">
         <v>21</v>
@@ -14270,7 +14270,7 @@
       </c>
       <c r="I117" s="17"/>
     </row>
-    <row r="118" spans="1:9" ht="15.75">
+    <row r="118" spans="1:9" ht="15.6">
       <c r="A118" s="17"/>
       <c r="B118" s="17" t="s">
         <v>21</v>
@@ -14293,7 +14293,7 @@
       </c>
       <c r="I118" s="17"/>
     </row>
-    <row r="119" spans="1:9" ht="15.75">
+    <row r="119" spans="1:9" ht="15.6">
       <c r="A119" s="17" t="b">
         <v>0</v>
       </c>
@@ -14312,7 +14312,7 @@
       <c r="H119" s="17"/>
       <c r="I119" s="17"/>
     </row>
-    <row r="120" spans="1:9" ht="15.75">
+    <row r="120" spans="1:9" ht="15.6">
       <c r="A120" s="17"/>
       <c r="B120" s="17" t="s">
         <v>21</v>
@@ -14335,7 +14335,7 @@
       </c>
       <c r="I120" s="17"/>
     </row>
-    <row r="121" spans="1:9" ht="15.75">
+    <row r="121" spans="1:9" ht="15.6">
       <c r="A121" s="17"/>
       <c r="B121" s="17" t="s">
         <v>21</v>
@@ -14358,7 +14358,7 @@
       </c>
       <c r="I121" s="17"/>
     </row>
-    <row r="122" spans="1:9" ht="15.75">
+    <row r="122" spans="1:9" ht="15.6">
       <c r="A122" s="17"/>
       <c r="B122" s="17" t="s">
         <v>21</v>
@@ -14381,7 +14381,7 @@
       </c>
       <c r="I122" s="17"/>
     </row>
-    <row r="123" spans="1:9" ht="15.75">
+    <row r="123" spans="1:9" ht="15.6">
       <c r="A123" s="17"/>
       <c r="B123" s="17" t="s">
         <v>21</v>
@@ -14404,7 +14404,7 @@
       </c>
       <c r="I123" s="17"/>
     </row>
-    <row r="124" spans="1:9" ht="15.75">
+    <row r="124" spans="1:9" ht="15.6">
       <c r="A124" s="17"/>
       <c r="B124" s="17" t="s">
         <v>21</v>
@@ -14427,7 +14427,7 @@
       </c>
       <c r="I124" s="17"/>
     </row>
-    <row r="125" spans="1:9" ht="15.75">
+    <row r="125" spans="1:9" ht="15.6">
       <c r="A125" s="17"/>
       <c r="B125" s="17" t="s">
         <v>21</v>
@@ -14450,7 +14450,7 @@
       </c>
       <c r="I125" s="17"/>
     </row>
-    <row r="126" spans="1:9" ht="15.75">
+    <row r="126" spans="1:9" ht="15.6">
       <c r="A126" s="17" t="b">
         <v>0</v>
       </c>
@@ -14469,7 +14469,7 @@
       <c r="H126" s="17"/>
       <c r="I126" s="17"/>
     </row>
-    <row r="127" spans="1:9" ht="15.75">
+    <row r="127" spans="1:9" ht="15.6">
       <c r="A127" s="17"/>
       <c r="B127" s="17" t="s">
         <v>21</v>
@@ -14494,7 +14494,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.75">
+    <row r="128" spans="1:9" ht="15.6">
       <c r="A128" s="17"/>
       <c r="B128" s="17" t="s">
         <v>21</v>
@@ -14517,7 +14517,7 @@
       </c>
       <c r="I128" s="17"/>
     </row>
-    <row r="129" spans="1:9" ht="15.75">
+    <row r="129" spans="1:9" ht="15.6">
       <c r="A129" s="17"/>
       <c r="B129" s="17" t="s">
         <v>21</v>
@@ -14540,7 +14540,7 @@
       </c>
       <c r="I129" s="17"/>
     </row>
-    <row r="130" spans="1:9" ht="15.75">
+    <row r="130" spans="1:9" ht="15.6">
       <c r="A130" s="17"/>
       <c r="B130" s="17" t="s">
         <v>21</v>
@@ -14563,7 +14563,7 @@
       </c>
       <c r="I130" s="17"/>
     </row>
-    <row r="131" spans="1:9" ht="15.75">
+    <row r="131" spans="1:9" ht="15.6">
       <c r="A131" s="17"/>
       <c r="B131" s="17" t="s">
         <v>21</v>
@@ -14586,7 +14586,7 @@
       </c>
       <c r="I131" s="17"/>
     </row>
-    <row r="132" spans="1:9" ht="15.75">
+    <row r="132" spans="1:9" ht="15.6">
       <c r="A132" s="17"/>
       <c r="B132" s="17" t="s">
         <v>21</v>
@@ -14609,7 +14609,7 @@
       </c>
       <c r="I132" s="17"/>
     </row>
-    <row r="133" spans="1:9" ht="15.75">
+    <row r="133" spans="1:9" ht="15.6">
       <c r="A133" s="17"/>
       <c r="B133" s="17" t="s">
         <v>21</v>
@@ -14632,7 +14632,7 @@
       </c>
       <c r="I133" s="17"/>
     </row>
-    <row r="134" spans="1:9" ht="15.75">
+    <row r="134" spans="1:9" ht="15.6">
       <c r="A134" s="17"/>
       <c r="B134" s="17" t="s">
         <v>21</v>
@@ -14655,7 +14655,7 @@
       </c>
       <c r="I134" s="17"/>
     </row>
-    <row r="135" spans="1:9" ht="15.75">
+    <row r="135" spans="1:9" ht="15.6">
       <c r="A135" s="17"/>
       <c r="B135" s="17" t="s">
         <v>21</v>
@@ -14678,7 +14678,7 @@
       </c>
       <c r="I135" s="17"/>
     </row>
-    <row r="136" spans="1:9" ht="15.75">
+    <row r="136" spans="1:9" ht="15.6">
       <c r="A136" s="17" t="b">
         <v>0</v>
       </c>
@@ -14697,7 +14697,7 @@
       <c r="H136" s="17"/>
       <c r="I136" s="17"/>
     </row>
-    <row r="137" spans="1:9" ht="15.75">
+    <row r="137" spans="1:9" ht="15.6">
       <c r="A137" s="17"/>
       <c r="B137" s="17" t="s">
         <v>21</v>
@@ -14722,7 +14722,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.75">
+    <row r="138" spans="1:9" ht="15.6">
       <c r="A138" s="17"/>
       <c r="B138" s="17" t="s">
         <v>21</v>
@@ -14743,7 +14743,7 @@
       <c r="H138" s="17"/>
       <c r="I138" s="17"/>
     </row>
-    <row r="139" spans="1:9" ht="15.75">
+    <row r="139" spans="1:9" ht="15.6">
       <c r="A139" s="17"/>
       <c r="B139" s="17" t="s">
         <v>21</v>
@@ -14766,7 +14766,7 @@
       </c>
       <c r="I139" s="17"/>
     </row>
-    <row r="140" spans="1:9" ht="15.75">
+    <row r="140" spans="1:9" ht="15.6">
       <c r="A140" s="17"/>
       <c r="B140" s="17" t="s">
         <v>21</v>
@@ -14789,7 +14789,7 @@
       </c>
       <c r="I140" s="17"/>
     </row>
-    <row r="141" spans="1:9" ht="15.75">
+    <row r="141" spans="1:9" ht="15.6">
       <c r="A141" s="17"/>
       <c r="B141" s="17" t="s">
         <v>21</v>
@@ -14812,7 +14812,7 @@
       </c>
       <c r="I141" s="17"/>
     </row>
-    <row r="142" spans="1:9" ht="15.75">
+    <row r="142" spans="1:9" ht="15.6">
       <c r="A142" s="17"/>
       <c r="B142" s="17" t="s">
         <v>21</v>
@@ -14835,7 +14835,7 @@
       </c>
       <c r="I142" s="17"/>
     </row>
-    <row r="143" spans="1:9" ht="15.75">
+    <row r="143" spans="1:9" ht="15.6">
       <c r="A143" s="17"/>
       <c r="B143" s="17" t="s">
         <v>21</v>
@@ -14858,7 +14858,7 @@
       </c>
       <c r="I143" s="17"/>
     </row>
-    <row r="144" spans="1:9" ht="15.75">
+    <row r="144" spans="1:9" ht="15.6">
       <c r="A144" s="17"/>
       <c r="B144" s="17" t="s">
         <v>21</v>
@@ -14881,7 +14881,7 @@
       </c>
       <c r="I144" s="17"/>
     </row>
-    <row r="145" spans="1:9" ht="15.75">
+    <row r="145" spans="1:9" ht="15.6">
       <c r="A145" s="17"/>
       <c r="B145" s="17" t="s">
         <v>21</v>
@@ -14904,7 +14904,7 @@
       </c>
       <c r="I145" s="17"/>
     </row>
-    <row r="146" spans="1:9" ht="15.75">
+    <row r="146" spans="1:9" ht="15.6">
       <c r="A146" s="17"/>
       <c r="B146" s="17" t="s">
         <v>21</v>
@@ -14927,7 +14927,7 @@
       </c>
       <c r="I146" s="17"/>
     </row>
-    <row r="147" spans="1:9" ht="15.75">
+    <row r="147" spans="1:9" ht="15.6">
       <c r="A147" s="17"/>
       <c r="B147" s="17" t="s">
         <v>21</v>
@@ -14950,7 +14950,7 @@
       </c>
       <c r="I147" s="17"/>
     </row>
-    <row r="148" spans="1:9" ht="15.75">
+    <row r="148" spans="1:9" ht="15.6">
       <c r="A148" s="17"/>
       <c r="B148" s="17" t="s">
         <v>21</v>
@@ -14973,7 +14973,7 @@
       </c>
       <c r="I148" s="17"/>
     </row>
-    <row r="149" spans="1:9" ht="15.75">
+    <row r="149" spans="1:9" ht="15.6">
       <c r="A149" s="17"/>
       <c r="B149" s="17" t="s">
         <v>21</v>
@@ -14996,7 +14996,7 @@
       </c>
       <c r="I149" s="17"/>
     </row>
-    <row r="150" spans="1:9" ht="15.75">
+    <row r="150" spans="1:9" ht="15.6">
       <c r="A150" s="17"/>
       <c r="B150" s="17" t="s">
         <v>21</v>
@@ -15019,7 +15019,7 @@
       </c>
       <c r="I150" s="17"/>
     </row>
-    <row r="151" spans="1:9" ht="15.75">
+    <row r="151" spans="1:9" ht="15.6">
       <c r="A151" s="17" t="b">
         <v>0</v>
       </c>
@@ -15038,7 +15038,7 @@
       <c r="H151" s="17"/>
       <c r="I151" s="17"/>
     </row>
-    <row r="152" spans="1:9" ht="15.75">
+    <row r="152" spans="1:9" ht="15.6">
       <c r="A152" s="17"/>
       <c r="B152" s="17" t="s">
         <v>21</v>
@@ -15061,7 +15061,7 @@
       </c>
       <c r="I152" s="17"/>
     </row>
-    <row r="153" spans="1:9" ht="15.75">
+    <row r="153" spans="1:9" ht="15.6">
       <c r="A153" s="17" t="b">
         <v>0</v>
       </c>
@@ -15080,7 +15080,7 @@
       <c r="H153" s="17"/>
       <c r="I153" s="17"/>
     </row>
-    <row r="154" spans="1:9" ht="15.75">
+    <row r="154" spans="1:9" ht="15.6">
       <c r="A154" s="17"/>
       <c r="B154" s="17" t="s">
         <v>21</v>
@@ -15103,7 +15103,7 @@
       </c>
       <c r="I154" s="17"/>
     </row>
-    <row r="155" spans="1:9" ht="15.75">
+    <row r="155" spans="1:9" ht="15.6">
       <c r="A155" s="17"/>
       <c r="B155" s="17" t="s">
         <v>21</v>
@@ -15126,7 +15126,7 @@
       </c>
       <c r="I155" s="17"/>
     </row>
-    <row r="156" spans="1:9" ht="15.75">
+    <row r="156" spans="1:9" ht="15.6">
       <c r="A156" s="17" t="b">
         <v>0</v>
       </c>
@@ -15145,7 +15145,7 @@
       <c r="H156" s="17"/>
       <c r="I156" s="17"/>
     </row>
-    <row r="157" spans="1:9" ht="15.75">
+    <row r="157" spans="1:9" ht="15.6">
       <c r="A157" s="17"/>
       <c r="B157" s="17" t="s">
         <v>21</v>
@@ -15170,7 +15170,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.75">
+    <row r="158" spans="1:9" ht="15.6">
       <c r="A158" s="17"/>
       <c r="B158" s="17" t="s">
         <v>21</v>
@@ -15193,7 +15193,7 @@
       </c>
       <c r="I158" s="17"/>
     </row>
-    <row r="159" spans="1:9" ht="15.75">
+    <row r="159" spans="1:9" ht="15.6">
       <c r="A159" s="17"/>
       <c r="B159" s="17" t="s">
         <v>21</v>
@@ -15216,7 +15216,7 @@
       </c>
       <c r="I159" s="17"/>
     </row>
-    <row r="160" spans="1:9" ht="15.75">
+    <row r="160" spans="1:9" ht="15.6">
       <c r="A160" s="17"/>
       <c r="B160" s="17" t="s">
         <v>21</v>
@@ -15239,7 +15239,7 @@
       </c>
       <c r="I160" s="17"/>
     </row>
-    <row r="161" spans="1:9" ht="15.75">
+    <row r="161" spans="1:9" ht="15.6">
       <c r="A161" s="17"/>
       <c r="B161" s="17" t="s">
         <v>21</v>
@@ -15262,7 +15262,7 @@
       </c>
       <c r="I161" s="17"/>
     </row>
-    <row r="162" spans="1:9" ht="15.75">
+    <row r="162" spans="1:9" ht="15.6">
       <c r="A162" s="17"/>
       <c r="B162" s="17" t="s">
         <v>21</v>
@@ -15285,7 +15285,7 @@
       </c>
       <c r="I162" s="17"/>
     </row>
-    <row r="163" spans="1:9" ht="15.75">
+    <row r="163" spans="1:9" ht="15.6">
       <c r="A163" s="17"/>
       <c r="B163" s="17" t="s">
         <v>21</v>
@@ -15308,7 +15308,7 @@
       </c>
       <c r="I163" s="17"/>
     </row>
-    <row r="164" spans="1:9" ht="15.75">
+    <row r="164" spans="1:9" ht="15.6">
       <c r="A164" s="17"/>
       <c r="B164" s="17" t="s">
         <v>21</v>
@@ -15331,7 +15331,7 @@
       </c>
       <c r="I164" s="17"/>
     </row>
-    <row r="165" spans="1:9" ht="15.75">
+    <row r="165" spans="1:9" ht="15.6">
       <c r="A165" s="17"/>
       <c r="B165" s="17" t="s">
         <v>21</v>
@@ -15354,7 +15354,7 @@
       </c>
       <c r="I165" s="17"/>
     </row>
-    <row r="166" spans="1:9" ht="15.75">
+    <row r="166" spans="1:9" ht="15.6">
       <c r="A166" s="17"/>
       <c r="B166" s="17" t="s">
         <v>21</v>
@@ -15377,7 +15377,7 @@
       </c>
       <c r="I166" s="17"/>
     </row>
-    <row r="167" spans="1:9" ht="15.75">
+    <row r="167" spans="1:9" ht="15.6">
       <c r="A167" s="17" t="b">
         <v>0</v>
       </c>
@@ -15396,7 +15396,7 @@
       <c r="H167" s="17"/>
       <c r="I167" s="17"/>
     </row>
-    <row r="168" spans="1:9" ht="15.75">
+    <row r="168" spans="1:9" ht="15.6">
       <c r="A168" s="17"/>
       <c r="B168" s="17" t="s">
         <v>21</v>
@@ -15421,7 +15421,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.75">
+    <row r="169" spans="1:9" ht="15.6">
       <c r="A169" s="17"/>
       <c r="B169" s="17" t="s">
         <v>21</v>
@@ -15444,7 +15444,7 @@
       </c>
       <c r="I169" s="17"/>
     </row>
-    <row r="170" spans="1:9" ht="15.75">
+    <row r="170" spans="1:9" ht="15.6">
       <c r="A170" s="17"/>
       <c r="B170" s="17" t="s">
         <v>21</v>
@@ -15467,7 +15467,7 @@
       </c>
       <c r="I170" s="17"/>
     </row>
-    <row r="171" spans="1:9" ht="15.75">
+    <row r="171" spans="1:9" ht="15.6">
       <c r="A171" s="17"/>
       <c r="B171" s="17" t="s">
         <v>21</v>
@@ -15490,7 +15490,7 @@
       </c>
       <c r="I171" s="17"/>
     </row>
-    <row r="172" spans="1:9" ht="15.75">
+    <row r="172" spans="1:9" ht="15.6">
       <c r="A172" s="17"/>
       <c r="B172" s="17" t="s">
         <v>21</v>
@@ -15513,7 +15513,7 @@
       </c>
       <c r="I172" s="17"/>
     </row>
-    <row r="173" spans="1:9" ht="15.75">
+    <row r="173" spans="1:9" ht="15.6">
       <c r="A173" s="17"/>
       <c r="B173" s="17" t="s">
         <v>21</v>
@@ -15536,7 +15536,7 @@
       </c>
       <c r="I173" s="17"/>
     </row>
-    <row r="174" spans="1:9" ht="15.75">
+    <row r="174" spans="1:9" ht="15.6">
       <c r="A174" s="17"/>
       <c r="B174" s="17" t="s">
         <v>21</v>
@@ -15559,7 +15559,7 @@
       </c>
       <c r="I174" s="17"/>
     </row>
-    <row r="175" spans="1:9" ht="15.75">
+    <row r="175" spans="1:9" ht="15.6">
       <c r="A175" s="17"/>
       <c r="B175" s="17" t="s">
         <v>21</v>
@@ -15582,7 +15582,7 @@
       </c>
       <c r="I175" s="17"/>
     </row>
-    <row r="176" spans="1:9" ht="15.75">
+    <row r="176" spans="1:9" ht="15.6">
       <c r="A176" s="17"/>
       <c r="B176" s="17" t="s">
         <v>21</v>
@@ -15605,7 +15605,7 @@
       </c>
       <c r="I176" s="17"/>
     </row>
-    <row r="177" spans="1:9" ht="15.75">
+    <row r="177" spans="1:9" ht="15.6">
       <c r="A177" s="17"/>
       <c r="B177" s="17" t="s">
         <v>21</v>
@@ -15628,7 +15628,7 @@
       </c>
       <c r="I177" s="17"/>
     </row>
-    <row r="178" spans="1:9" ht="15.75">
+    <row r="178" spans="1:9" ht="15.6">
       <c r="A178" s="17" t="b">
         <v>0</v>
       </c>
@@ -15647,7 +15647,7 @@
       <c r="H178" s="17"/>
       <c r="I178" s="17"/>
     </row>
-    <row r="179" spans="1:9" ht="15.75">
+    <row r="179" spans="1:9" ht="15.6">
       <c r="A179" s="17"/>
       <c r="B179" s="17" t="s">
         <v>21</v>
@@ -15670,7 +15670,7 @@
       </c>
       <c r="I179" s="17"/>
     </row>
-    <row r="180" spans="1:9" ht="15.75">
+    <row r="180" spans="1:9" ht="15.6">
       <c r="A180" s="17"/>
       <c r="B180" s="17" t="s">
         <v>21</v>
@@ -15693,7 +15693,7 @@
       </c>
       <c r="I180" s="17"/>
     </row>
-    <row r="181" spans="1:9" ht="15.75">
+    <row r="181" spans="1:9" ht="15.6">
       <c r="A181" s="17"/>
       <c r="B181" s="17" t="s">
         <v>21</v>
@@ -15716,7 +15716,7 @@
       </c>
       <c r="I181" s="17"/>
     </row>
-    <row r="182" spans="1:9" ht="15.75">
+    <row r="182" spans="1:9" ht="15.6">
       <c r="A182" s="17"/>
       <c r="B182" s="17" t="s">
         <v>21</v>
@@ -15739,7 +15739,7 @@
       </c>
       <c r="I182" s="17"/>
     </row>
-    <row r="183" spans="1:9" ht="15.75">
+    <row r="183" spans="1:9" ht="15.6">
       <c r="A183" s="17" t="b">
         <v>0</v>
       </c>
@@ -15758,7 +15758,7 @@
       <c r="H183" s="17"/>
       <c r="I183" s="17"/>
     </row>
-    <row r="184" spans="1:9" ht="15.75">
+    <row r="184" spans="1:9" ht="15.6">
       <c r="A184" s="17"/>
       <c r="B184" s="17" t="s">
         <v>21</v>
@@ -15781,7 +15781,7 @@
       </c>
       <c r="I184" s="17"/>
     </row>
-    <row r="185" spans="1:9" ht="15.75">
+    <row r="185" spans="1:9" ht="15.6">
       <c r="A185" s="17"/>
       <c r="B185" s="17" t="s">
         <v>21</v>
@@ -15804,7 +15804,7 @@
       </c>
       <c r="I185" s="17"/>
     </row>
-    <row r="186" spans="1:9" ht="15.75">
+    <row r="186" spans="1:9" ht="15.6">
       <c r="A186" s="17"/>
       <c r="B186" s="17" t="s">
         <v>21</v>
@@ -15827,7 +15827,7 @@
       </c>
       <c r="I186" s="17"/>
     </row>
-    <row r="187" spans="1:9" ht="15.75">
+    <row r="187" spans="1:9" ht="15.6">
       <c r="A187" s="17"/>
       <c r="B187" s="17" t="s">
         <v>21</v>
@@ -15850,7 +15850,7 @@
       </c>
       <c r="I187" s="17"/>
     </row>
-    <row r="188" spans="1:9" ht="15.75">
+    <row r="188" spans="1:9" ht="15.6">
       <c r="A188" s="17" t="b">
         <v>0</v>
       </c>
@@ -15869,7 +15869,7 @@
       <c r="H188" s="17"/>
       <c r="I188" s="17"/>
     </row>
-    <row r="189" spans="1:9" ht="15.75">
+    <row r="189" spans="1:9" ht="15.6">
       <c r="A189" s="17"/>
       <c r="B189" s="17" t="s">
         <v>21</v>
@@ -15890,7 +15890,7 @@
       <c r="H189" s="17"/>
       <c r="I189" s="17"/>
     </row>
-    <row r="190" spans="1:9" ht="15.75">
+    <row r="190" spans="1:9" ht="15.6">
       <c r="A190" s="17"/>
       <c r="B190" s="17" t="s">
         <v>21</v>
@@ -15913,7 +15913,7 @@
       </c>
       <c r="I190" s="17"/>
     </row>
-    <row r="191" spans="1:9" ht="15.75">
+    <row r="191" spans="1:9" ht="15.6">
       <c r="A191" s="17" t="b">
         <v>0</v>
       </c>
@@ -15932,7 +15932,7 @@
       <c r="H191" s="17"/>
       <c r="I191" s="17"/>
     </row>
-    <row r="192" spans="1:9" ht="15.75">
+    <row r="192" spans="1:9" ht="15.6">
       <c r="A192" s="17"/>
       <c r="B192" s="17" t="s">
         <v>21</v>
@@ -15955,7 +15955,7 @@
       </c>
       <c r="I192" s="17"/>
     </row>
-    <row r="193" spans="1:9" ht="15.75">
+    <row r="193" spans="1:9" ht="15.6">
       <c r="A193" s="17"/>
       <c r="B193" s="17" t="s">
         <v>21</v>
@@ -15980,7 +15980,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.75">
+    <row r="194" spans="1:9" ht="15.6">
       <c r="A194" s="17"/>
       <c r="B194" s="17" t="s">
         <v>21</v>
@@ -16001,7 +16001,7 @@
       <c r="H194" s="17"/>
       <c r="I194" s="17"/>
     </row>
-    <row r="195" spans="1:9" ht="15.75">
+    <row r="195" spans="1:9" ht="15.6">
       <c r="A195" s="17"/>
       <c r="B195" s="17" t="s">
         <v>21</v>
@@ -16026,7 +16026,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.75">
+    <row r="196" spans="1:9" ht="15.6">
       <c r="A196" s="17"/>
       <c r="B196" s="17" t="s">
         <v>21</v>
@@ -16051,7 +16051,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.75">
+    <row r="197" spans="1:9" ht="15.6">
       <c r="A197" s="17" t="b">
         <v>0</v>
       </c>
@@ -16070,7 +16070,7 @@
       <c r="H197" s="17"/>
       <c r="I197" s="17"/>
     </row>
-    <row r="198" spans="1:9" ht="15.75">
+    <row r="198" spans="1:9" ht="15.6">
       <c r="A198" s="17"/>
       <c r="B198" s="17" t="s">
         <v>21</v>
@@ -16095,7 +16095,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.75">
+    <row r="199" spans="1:9" ht="15.6">
       <c r="A199" s="17"/>
       <c r="B199" s="17" t="s">
         <v>21</v>
@@ -16118,7 +16118,7 @@
       </c>
       <c r="I199" s="17"/>
     </row>
-    <row r="200" spans="1:9" ht="15.75">
+    <row r="200" spans="1:9" ht="15.6">
       <c r="A200" s="17"/>
       <c r="B200" s="17" t="s">
         <v>21</v>
@@ -16141,7 +16141,7 @@
       </c>
       <c r="I200" s="17"/>
     </row>
-    <row r="201" spans="1:9" ht="15.75">
+    <row r="201" spans="1:9" ht="15.6">
       <c r="A201" s="17"/>
       <c r="B201" s="17" t="s">
         <v>21</v>
@@ -16164,7 +16164,7 @@
       </c>
       <c r="I201" s="17"/>
     </row>
-    <row r="202" spans="1:9" ht="15.75">
+    <row r="202" spans="1:9" ht="15.6">
       <c r="A202" s="17"/>
       <c r="B202" s="17" t="s">
         <v>21</v>
@@ -16187,7 +16187,7 @@
       </c>
       <c r="I202" s="17"/>
     </row>
-    <row r="203" spans="1:9" ht="15.75">
+    <row r="203" spans="1:9" ht="15.6">
       <c r="A203" s="17"/>
       <c r="B203" s="17" t="s">
         <v>21</v>
@@ -16210,7 +16210,7 @@
       </c>
       <c r="I203" s="17"/>
     </row>
-    <row r="204" spans="1:9" ht="15.75">
+    <row r="204" spans="1:9" ht="15.6">
       <c r="A204" s="17"/>
       <c r="B204" s="17" t="s">
         <v>21</v>
@@ -16233,7 +16233,7 @@
       </c>
       <c r="I204" s="17"/>
     </row>
-    <row r="205" spans="1:9" ht="15.75">
+    <row r="205" spans="1:9" ht="15.6">
       <c r="A205" s="17"/>
       <c r="B205" s="17" t="s">
         <v>21</v>
@@ -16256,7 +16256,7 @@
       </c>
       <c r="I205" s="17"/>
     </row>
-    <row r="206" spans="1:9" ht="15.75">
+    <row r="206" spans="1:9" ht="15.6">
       <c r="A206" s="17"/>
       <c r="B206" s="17" t="s">
         <v>21</v>
@@ -16279,7 +16279,7 @@
       </c>
       <c r="I206" s="17"/>
     </row>
-    <row r="207" spans="1:9" ht="15.75">
+    <row r="207" spans="1:9" ht="15.6">
       <c r="A207" s="17" t="b">
         <v>0</v>
       </c>
@@ -16298,7 +16298,7 @@
       <c r="H207" s="17"/>
       <c r="I207" s="17"/>
     </row>
-    <row r="208" spans="1:9" ht="15.75">
+    <row r="208" spans="1:9" ht="15.6">
       <c r="A208" s="17"/>
       <c r="B208" s="17" t="s">
         <v>21</v>
@@ -16323,7 +16323,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.75">
+    <row r="209" spans="1:9" ht="15.6">
       <c r="A209" s="17"/>
       <c r="B209" s="17" t="s">
         <v>21</v>
@@ -16346,7 +16346,7 @@
       </c>
       <c r="I209" s="17"/>
     </row>
-    <row r="210" spans="1:9" ht="15.75">
+    <row r="210" spans="1:9" ht="15.6">
       <c r="A210" s="17"/>
       <c r="B210" s="17" t="s">
         <v>21</v>
@@ -16369,7 +16369,7 @@
       </c>
       <c r="I210" s="17"/>
     </row>
-    <row r="211" spans="1:9" ht="15.75">
+    <row r="211" spans="1:9" ht="15.6">
       <c r="A211" s="17"/>
       <c r="B211" s="17" t="s">
         <v>21</v>
@@ -16392,7 +16392,7 @@
       </c>
       <c r="I211" s="17"/>
     </row>
-    <row r="212" spans="1:9" ht="15.75">
+    <row r="212" spans="1:9" ht="15.6">
       <c r="A212" s="17"/>
       <c r="B212" s="17" t="s">
         <v>21</v>
@@ -16415,7 +16415,7 @@
       </c>
       <c r="I212" s="17"/>
     </row>
-    <row r="213" spans="1:9" ht="15.75">
+    <row r="213" spans="1:9" ht="15.6">
       <c r="A213" s="17"/>
       <c r="B213" s="17" t="s">
         <v>21</v>
@@ -16438,7 +16438,7 @@
       </c>
       <c r="I213" s="17"/>
     </row>
-    <row r="214" spans="1:9" ht="15.75">
+    <row r="214" spans="1:9" ht="15.6">
       <c r="A214" s="17"/>
       <c r="B214" s="17" t="s">
         <v>21</v>
@@ -16461,7 +16461,7 @@
       </c>
       <c r="I214" s="17"/>
     </row>
-    <row r="215" spans="1:9" ht="15.75">
+    <row r="215" spans="1:9" ht="15.6">
       <c r="A215" s="17"/>
       <c r="B215" s="17" t="s">
         <v>21</v>
@@ -16484,7 +16484,7 @@
       </c>
       <c r="I215" s="17"/>
     </row>
-    <row r="216" spans="1:9" ht="15.75">
+    <row r="216" spans="1:9" ht="15.6">
       <c r="A216" s="17"/>
       <c r="B216" s="17" t="s">
         <v>21</v>
@@ -16507,7 +16507,7 @@
       </c>
       <c r="I216" s="17"/>
     </row>
-    <row r="217" spans="1:9" ht="15.75">
+    <row r="217" spans="1:9" ht="15.6">
       <c r="A217" s="17" t="b">
         <v>0</v>
       </c>
@@ -16526,7 +16526,7 @@
       <c r="H217" s="17"/>
       <c r="I217" s="17"/>
     </row>
-    <row r="218" spans="1:9" ht="15.75">
+    <row r="218" spans="1:9" ht="15.6">
       <c r="A218" s="17"/>
       <c r="B218" s="17" t="s">
         <v>21</v>
@@ -16547,7 +16547,7 @@
       <c r="H218" s="17"/>
       <c r="I218" s="17"/>
     </row>
-    <row r="219" spans="1:9" ht="15.75">
+    <row r="219" spans="1:9" ht="15.6">
       <c r="A219" s="17"/>
       <c r="B219" s="17" t="s">
         <v>21</v>
@@ -16570,7 +16570,7 @@
       </c>
       <c r="I219" s="17"/>
     </row>
-    <row r="220" spans="1:9" ht="15.75">
+    <row r="220" spans="1:9" ht="15.6">
       <c r="A220" s="17"/>
       <c r="B220" s="17" t="s">
         <v>21</v>
@@ -16593,7 +16593,7 @@
       </c>
       <c r="I220" s="17"/>
     </row>
-    <row r="221" spans="1:9" ht="15.75">
+    <row r="221" spans="1:9" ht="15.6">
       <c r="A221" s="17"/>
       <c r="B221" s="17" t="s">
         <v>21</v>
@@ -16616,7 +16616,7 @@
       </c>
       <c r="I221" s="17"/>
     </row>
-    <row r="222" spans="1:9" ht="15.75">
+    <row r="222" spans="1:9" ht="15.6">
       <c r="A222" s="17"/>
       <c r="B222" s="17" t="s">
         <v>21</v>
@@ -16639,7 +16639,7 @@
       </c>
       <c r="I222" s="17"/>
     </row>
-    <row r="223" spans="1:9" ht="15.75">
+    <row r="223" spans="1:9" ht="15.6">
       <c r="A223" s="17"/>
       <c r="B223" s="17" t="s">
         <v>21</v>
@@ -16662,7 +16662,7 @@
       </c>
       <c r="I223" s="17"/>
     </row>
-    <row r="224" spans="1:9" ht="15.75">
+    <row r="224" spans="1:9" ht="15.6">
       <c r="A224" s="17"/>
       <c r="B224" s="17" t="s">
         <v>21</v>
@@ -16685,7 +16685,7 @@
       </c>
       <c r="I224" s="17"/>
     </row>
-    <row r="225" spans="1:9" ht="15.75">
+    <row r="225" spans="1:9" ht="15.6">
       <c r="A225" s="17"/>
       <c r="B225" s="17" t="s">
         <v>21</v>
@@ -16708,7 +16708,7 @@
       </c>
       <c r="I225" s="17"/>
     </row>
-    <row r="226" spans="1:9" ht="15.75">
+    <row r="226" spans="1:9" ht="15.6">
       <c r="A226" s="17"/>
       <c r="B226" s="17" t="s">
         <v>21</v>
@@ -16731,7 +16731,7 @@
       </c>
       <c r="I226" s="17"/>
     </row>
-    <row r="227" spans="1:9" ht="15.75">
+    <row r="227" spans="1:9" ht="15.6">
       <c r="A227" s="17"/>
       <c r="B227" s="17" t="s">
         <v>21</v>
@@ -16754,7 +16754,7 @@
       </c>
       <c r="I227" s="17"/>
     </row>
-    <row r="228" spans="1:9" ht="15.75">
+    <row r="228" spans="1:9" ht="15.6">
       <c r="A228" s="17"/>
       <c r="B228" s="17" t="s">
         <v>21</v>
@@ -16777,7 +16777,7 @@
       </c>
       <c r="I228" s="17"/>
     </row>
-    <row r="229" spans="1:9" ht="15.75">
+    <row r="229" spans="1:9" ht="15.6">
       <c r="A229" s="17"/>
       <c r="B229" s="17" t="s">
         <v>21</v>
@@ -16800,7 +16800,7 @@
       </c>
       <c r="I229" s="17"/>
     </row>
-    <row r="230" spans="1:9" ht="15.75">
+    <row r="230" spans="1:9" ht="15.6">
       <c r="A230" s="17"/>
       <c r="B230" s="17" t="s">
         <v>21</v>
@@ -16823,7 +16823,7 @@
       </c>
       <c r="I230" s="17"/>
     </row>
-    <row r="231" spans="1:9" ht="15.75">
+    <row r="231" spans="1:9" ht="15.6">
       <c r="A231" s="17"/>
       <c r="B231" s="17" t="s">
         <v>21</v>
@@ -16846,7 +16846,7 @@
       </c>
       <c r="I231" s="17"/>
     </row>
-    <row r="232" spans="1:9" ht="15.75">
+    <row r="232" spans="1:9" ht="15.6">
       <c r="A232" s="17"/>
       <c r="B232" s="17" t="s">
         <v>21</v>
@@ -16869,7 +16869,7 @@
       </c>
       <c r="I232" s="17"/>
     </row>
-    <row r="233" spans="1:9" ht="15.75">
+    <row r="233" spans="1:9" ht="15.6">
       <c r="A233" s="17"/>
       <c r="B233" s="17" t="s">
         <v>21</v>
@@ -16892,7 +16892,7 @@
       </c>
       <c r="I233" s="17"/>
     </row>
-    <row r="234" spans="1:9" ht="15.75">
+    <row r="234" spans="1:9" ht="15.6">
       <c r="A234" s="17" t="b">
         <v>0</v>
       </c>
@@ -16911,7 +16911,7 @@
       <c r="H234" s="17"/>
       <c r="I234" s="17"/>
     </row>
-    <row r="235" spans="1:9" ht="15.75">
+    <row r="235" spans="1:9" ht="15.6">
       <c r="A235" s="17"/>
       <c r="B235" s="17" t="s">
         <v>21</v>
@@ -16932,7 +16932,7 @@
       <c r="H235" s="17"/>
       <c r="I235" s="17"/>
     </row>
-    <row r="236" spans="1:9" ht="15.75">
+    <row r="236" spans="1:9" ht="15.6">
       <c r="A236" s="17"/>
       <c r="B236" s="17" t="s">
         <v>21</v>
@@ -16955,7 +16955,7 @@
       </c>
       <c r="I236" s="17"/>
     </row>
-    <row r="237" spans="1:9" ht="15.75">
+    <row r="237" spans="1:9" ht="15.6">
       <c r="A237" s="17"/>
       <c r="B237" s="17" t="s">
         <v>21</v>
@@ -16978,7 +16978,7 @@
       </c>
       <c r="I237" s="17"/>
     </row>
-    <row r="238" spans="1:9" ht="15.75">
+    <row r="238" spans="1:9" ht="15.6">
       <c r="A238" s="17"/>
       <c r="B238" s="17" t="s">
         <v>21</v>
@@ -17001,7 +17001,7 @@
       </c>
       <c r="I238" s="17"/>
     </row>
-    <row r="239" spans="1:9" ht="15.75">
+    <row r="239" spans="1:9" ht="15.6">
       <c r="A239" s="17"/>
       <c r="B239" s="17" t="s">
         <v>21</v>
@@ -17024,7 +17024,7 @@
       </c>
       <c r="I239" s="17"/>
     </row>
-    <row r="240" spans="1:9" ht="15.75">
+    <row r="240" spans="1:9" ht="15.6">
       <c r="A240" s="17"/>
       <c r="B240" s="17" t="s">
         <v>21</v>
@@ -17047,7 +17047,7 @@
       </c>
       <c r="I240" s="17"/>
     </row>
-    <row r="241" spans="1:9" ht="15.75">
+    <row r="241" spans="1:9" ht="15.6">
       <c r="A241" s="17"/>
       <c r="B241" s="17" t="s">
         <v>21</v>
@@ -17070,7 +17070,7 @@
       </c>
       <c r="I241" s="17"/>
     </row>
-    <row r="242" spans="1:9" ht="15.75">
+    <row r="242" spans="1:9" ht="15.6">
       <c r="A242" s="17"/>
       <c r="B242" s="17" t="s">
         <v>21</v>
@@ -17093,7 +17093,7 @@
       </c>
       <c r="I242" s="17"/>
     </row>
-    <row r="243" spans="1:9" ht="15.75">
+    <row r="243" spans="1:9" ht="15.6">
       <c r="A243" s="17"/>
       <c r="B243" s="17" t="s">
         <v>21</v>
@@ -17116,7 +17116,7 @@
       </c>
       <c r="I243" s="17"/>
     </row>
-    <row r="244" spans="1:9" ht="15.75">
+    <row r="244" spans="1:9" ht="15.6">
       <c r="A244" s="17"/>
       <c r="B244" s="17" t="s">
         <v>21</v>
@@ -17139,7 +17139,7 @@
       </c>
       <c r="I244" s="17"/>
     </row>
-    <row r="245" spans="1:9" ht="15.75">
+    <row r="245" spans="1:9" ht="15.6">
       <c r="A245" s="17"/>
       <c r="B245" s="17" t="s">
         <v>21</v>
@@ -17162,7 +17162,7 @@
       </c>
       <c r="I245" s="17"/>
     </row>
-    <row r="246" spans="1:9" ht="15.75">
+    <row r="246" spans="1:9" ht="15.6">
       <c r="A246" s="17"/>
       <c r="B246" s="17" t="s">
         <v>21</v>
@@ -17185,7 +17185,7 @@
       </c>
       <c r="I246" s="17"/>
     </row>
-    <row r="247" spans="1:9" ht="15.75">
+    <row r="247" spans="1:9" ht="15.6">
       <c r="A247" s="17"/>
       <c r="B247" s="17" t="s">
         <v>21</v>
@@ -17208,7 +17208,7 @@
       </c>
       <c r="I247" s="17"/>
     </row>
-    <row r="248" spans="1:9" ht="15.75">
+    <row r="248" spans="1:9" ht="15.6">
       <c r="A248" s="17"/>
       <c r="B248" s="17" t="s">
         <v>21</v>
@@ -17231,7 +17231,7 @@
       </c>
       <c r="I248" s="17"/>
     </row>
-    <row r="249" spans="1:9" ht="15.75">
+    <row r="249" spans="1:9" ht="15.6">
       <c r="A249" s="17"/>
       <c r="B249" s="17" t="s">
         <v>21</v>
@@ -17254,7 +17254,7 @@
       </c>
       <c r="I249" s="17"/>
     </row>
-    <row r="250" spans="1:9" ht="15.75">
+    <row r="250" spans="1:9" ht="15.6">
       <c r="A250" s="17"/>
       <c r="B250" s="17" t="s">
         <v>21</v>
@@ -17277,7 +17277,7 @@
       </c>
       <c r="I250" s="17"/>
     </row>
-    <row r="251" spans="1:9" ht="15.75">
+    <row r="251" spans="1:9" ht="15.6">
       <c r="A251" s="17" t="b">
         <v>0</v>
       </c>
@@ -17296,7 +17296,7 @@
       <c r="H251" s="17"/>
       <c r="I251" s="17"/>
     </row>
-    <row r="252" spans="1:9" ht="15.75">
+    <row r="252" spans="1:9" ht="15.6">
       <c r="A252" s="17"/>
       <c r="B252" s="17" t="s">
         <v>21</v>
@@ -17321,7 +17321,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15.75">
+    <row r="253" spans="1:9" ht="15.6">
       <c r="A253" s="17"/>
       <c r="B253" s="17" t="s">
         <v>21</v>
@@ -17344,7 +17344,7 @@
       </c>
       <c r="I253" s="17"/>
     </row>
-    <row r="254" spans="1:9" ht="15.75">
+    <row r="254" spans="1:9" ht="15.6">
       <c r="A254" s="17"/>
       <c r="B254" s="17" t="s">
         <v>21</v>
@@ -17367,7 +17367,7 @@
       </c>
       <c r="I254" s="17"/>
     </row>
-    <row r="255" spans="1:9" ht="15.75">
+    <row r="255" spans="1:9" ht="15.6">
       <c r="A255" s="17"/>
       <c r="B255" s="17" t="s">
         <v>21</v>
@@ -17390,7 +17390,7 @@
       </c>
       <c r="I255" s="17"/>
     </row>
-    <row r="256" spans="1:9" ht="15.75">
+    <row r="256" spans="1:9" ht="15.6">
       <c r="A256" s="17"/>
       <c r="B256" s="17" t="s">
         <v>21</v>
@@ -17413,7 +17413,7 @@
       </c>
       <c r="I256" s="17"/>
     </row>
-    <row r="257" spans="1:9" ht="15.75">
+    <row r="257" spans="1:9" ht="15.6">
       <c r="A257" s="17" t="b">
         <v>0</v>
       </c>
@@ -17432,7 +17432,7 @@
       <c r="H257" s="17"/>
       <c r="I257" s="17"/>
     </row>
-    <row r="258" spans="1:9" ht="15.75">
+    <row r="258" spans="1:9" ht="15.6">
       <c r="A258" s="17"/>
       <c r="B258" s="17" t="s">
         <v>21</v>
@@ -17457,7 +17457,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15.75">
+    <row r="259" spans="1:9" ht="15.6">
       <c r="A259" s="17"/>
       <c r="B259" s="17" t="s">
         <v>21</v>
@@ -17480,7 +17480,7 @@
       </c>
       <c r="I259" s="17"/>
     </row>
-    <row r="260" spans="1:9" ht="15.75">
+    <row r="260" spans="1:9" ht="15.6">
       <c r="A260" s="17" t="b">
         <v>0</v>
       </c>
@@ -17499,7 +17499,7 @@
       <c r="H260" s="17"/>
       <c r="I260" s="17"/>
     </row>
-    <row r="261" spans="1:9" ht="15.75">
+    <row r="261" spans="1:9" ht="15.6">
       <c r="A261" s="17" t="b">
         <v>0</v>
       </c>
@@ -17518,7 +17518,7 @@
       <c r="H261" s="17"/>
       <c r="I261" s="17"/>
     </row>
-    <row r="262" spans="1:9" ht="15.75">
+    <row r="262" spans="1:9" ht="15.6">
       <c r="A262" s="17" t="b">
         <v>0</v>
       </c>
@@ -17537,7 +17537,7 @@
       <c r="H262" s="17"/>
       <c r="I262" s="17"/>
     </row>
-    <row r="263" spans="1:9" ht="15.75">
+    <row r="263" spans="1:9" ht="15.6">
       <c r="A263" s="17"/>
       <c r="B263" s="17" t="s">
         <v>21</v>
@@ -17558,7 +17558,7 @@
       <c r="H263" s="17"/>
       <c r="I263" s="17"/>
     </row>
-    <row r="264" spans="1:9" ht="15.75">
+    <row r="264" spans="1:9" ht="15.6">
       <c r="A264" s="17"/>
       <c r="B264" s="17" t="s">
         <v>21</v>
@@ -17581,7 +17581,7 @@
       </c>
       <c r="I264" s="17"/>
     </row>
-    <row r="265" spans="1:9" ht="15.75">
+    <row r="265" spans="1:9" ht="15.6">
       <c r="A265" s="17"/>
       <c r="B265" s="17" t="s">
         <v>21</v>
@@ -17604,7 +17604,7 @@
       </c>
       <c r="I265" s="17"/>
     </row>
-    <row r="266" spans="1:9" ht="15.75">
+    <row r="266" spans="1:9" ht="15.6">
       <c r="A266" s="17"/>
       <c r="B266" s="17" t="s">
         <v>21</v>
@@ -17627,7 +17627,7 @@
       </c>
       <c r="I266" s="17"/>
     </row>
-    <row r="267" spans="1:9" ht="15.75">
+    <row r="267" spans="1:9" ht="15.6">
       <c r="A267" s="17"/>
       <c r="B267" s="17" t="s">
         <v>21</v>
@@ -17650,7 +17650,7 @@
       </c>
       <c r="I267" s="17"/>
     </row>
-    <row r="268" spans="1:9" ht="15.75">
+    <row r="268" spans="1:9" ht="15.6">
       <c r="A268" s="17"/>
       <c r="B268" s="17" t="s">
         <v>21</v>
@@ -17673,7 +17673,7 @@
       </c>
       <c r="I268" s="17"/>
     </row>
-    <row r="269" spans="1:9" ht="15.75">
+    <row r="269" spans="1:9" ht="15.6">
       <c r="A269" s="17"/>
       <c r="B269" s="17" t="s">
         <v>21</v>
@@ -17696,7 +17696,7 @@
       </c>
       <c r="I269" s="17"/>
     </row>
-    <row r="270" spans="1:9" ht="15.75">
+    <row r="270" spans="1:9" ht="15.6">
       <c r="A270" s="17"/>
       <c r="B270" s="17" t="s">
         <v>21</v>
@@ -17719,7 +17719,7 @@
       </c>
       <c r="I270" s="17"/>
     </row>
-    <row r="271" spans="1:9" ht="15.75">
+    <row r="271" spans="1:9" ht="15.6">
       <c r="A271" s="17"/>
       <c r="B271" s="17" t="s">
         <v>21</v>
@@ -17742,7 +17742,7 @@
       </c>
       <c r="I271" s="17"/>
     </row>
-    <row r="272" spans="1:9" ht="15.75">
+    <row r="272" spans="1:9" ht="15.6">
       <c r="A272" s="17"/>
       <c r="B272" s="17" t="s">
         <v>21</v>
@@ -17765,7 +17765,7 @@
       </c>
       <c r="I272" s="17"/>
     </row>
-    <row r="273" spans="1:9" ht="15.75">
+    <row r="273" spans="1:9" ht="15.6">
       <c r="A273" s="17"/>
       <c r="B273" s="17" t="s">
         <v>21</v>
@@ -17788,7 +17788,7 @@
       </c>
       <c r="I273" s="17"/>
     </row>
-    <row r="274" spans="1:9" ht="15.75">
+    <row r="274" spans="1:9" ht="15.6">
       <c r="A274" s="17" t="b">
         <v>0</v>
       </c>
@@ -17807,7 +17807,7 @@
       <c r="H274" s="17"/>
       <c r="I274" s="17"/>
     </row>
-    <row r="275" spans="1:9" ht="15.75">
+    <row r="275" spans="1:9" ht="15.6">
       <c r="A275" s="17"/>
       <c r="B275" s="17" t="s">
         <v>21</v>
@@ -17830,7 +17830,7 @@
       </c>
       <c r="I275" s="17"/>
     </row>
-    <row r="276" spans="1:9" ht="15.75">
+    <row r="276" spans="1:9" ht="15.6">
       <c r="A276" s="17" t="b">
         <v>0</v>
       </c>
@@ -17849,7 +17849,7 @@
       <c r="H276" s="17"/>
       <c r="I276" s="17"/>
     </row>
-    <row r="277" spans="1:9" ht="15.75">
+    <row r="277" spans="1:9" ht="15.6">
       <c r="A277" s="17"/>
       <c r="B277" s="17" t="s">
         <v>21</v>
@@ -17874,7 +17874,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15.75">
+    <row r="278" spans="1:9" ht="15.6">
       <c r="A278" s="17"/>
       <c r="B278" s="17" t="s">
         <v>21</v>
@@ -17897,7 +17897,7 @@
       </c>
       <c r="I278" s="17"/>
     </row>
-    <row r="279" spans="1:9" ht="15.75">
+    <row r="279" spans="1:9" ht="15.6">
       <c r="A279" s="17"/>
       <c r="B279" s="17" t="s">
         <v>21</v>
@@ -17920,7 +17920,7 @@
       </c>
       <c r="I279" s="17"/>
     </row>
-    <row r="280" spans="1:9" ht="15.75">
+    <row r="280" spans="1:9" ht="15.6">
       <c r="A280" s="17"/>
       <c r="B280" s="17" t="s">
         <v>21</v>
@@ -17943,7 +17943,7 @@
       </c>
       <c r="I280" s="17"/>
     </row>
-    <row r="281" spans="1:9" ht="15.75">
+    <row r="281" spans="1:9" ht="15.6">
       <c r="A281" s="17"/>
       <c r="B281" s="17" t="s">
         <v>21</v>
@@ -17966,7 +17966,7 @@
       </c>
       <c r="I281" s="17"/>
     </row>
-    <row r="282" spans="1:9" ht="15.75">
+    <row r="282" spans="1:9" ht="15.6">
       <c r="A282" s="17"/>
       <c r="B282" s="17" t="s">
         <v>21</v>
@@ -17989,7 +17989,7 @@
       </c>
       <c r="I282" s="17"/>
     </row>
-    <row r="283" spans="1:9" ht="15.75">
+    <row r="283" spans="1:9" ht="15.6">
       <c r="A283" s="17"/>
       <c r="B283" s="17" t="s">
         <v>21</v>
@@ -18012,7 +18012,7 @@
       </c>
       <c r="I283" s="17"/>
     </row>
-    <row r="284" spans="1:9" ht="15.75">
+    <row r="284" spans="1:9" ht="15.6">
       <c r="A284" s="17"/>
       <c r="B284" s="17" t="s">
         <v>21</v>
@@ -18035,7 +18035,7 @@
       </c>
       <c r="I284" s="17"/>
     </row>
-    <row r="285" spans="1:9" ht="15.75">
+    <row r="285" spans="1:9" ht="15.6">
       <c r="A285" s="17"/>
       <c r="B285" s="17" t="s">
         <v>21</v>
@@ -18058,7 +18058,7 @@
       </c>
       <c r="I285" s="17"/>
     </row>
-    <row r="286" spans="1:9" ht="15.75">
+    <row r="286" spans="1:9" ht="15.6">
       <c r="A286" s="17"/>
       <c r="B286" s="17" t="s">
         <v>21</v>
@@ -18081,7 +18081,7 @@
       </c>
       <c r="I286" s="17"/>
     </row>
-    <row r="287" spans="1:9" ht="15.75">
+    <row r="287" spans="1:9" ht="15.6">
       <c r="A287" s="17"/>
       <c r="B287" s="17" t="s">
         <v>21</v>
@@ -18104,7 +18104,7 @@
       </c>
       <c r="I287" s="17"/>
     </row>
-    <row r="288" spans="1:9" ht="15.75">
+    <row r="288" spans="1:9" ht="15.6">
       <c r="A288" s="17" t="b">
         <v>0</v>
       </c>
@@ -18123,7 +18123,7 @@
       <c r="H288" s="17"/>
       <c r="I288" s="17"/>
     </row>
-    <row r="289" spans="1:9" ht="15.75">
+    <row r="289" spans="1:9" ht="15.6">
       <c r="A289" s="17"/>
       <c r="B289" s="17" t="s">
         <v>21</v>
@@ -18146,7 +18146,7 @@
       </c>
       <c r="I289" s="17"/>
     </row>
-    <row r="290" spans="1:9" ht="15.75">
+    <row r="290" spans="1:9" ht="15.6">
       <c r="A290" s="17" t="b">
         <v>0</v>
       </c>
@@ -18165,7 +18165,7 @@
       <c r="H290" s="17"/>
       <c r="I290" s="17"/>
     </row>
-    <row r="291" spans="1:9" ht="15.75">
+    <row r="291" spans="1:9" ht="15.6">
       <c r="A291" s="17"/>
       <c r="B291" s="17" t="s">
         <v>21</v>
@@ -18186,7 +18186,7 @@
       <c r="H291" s="17"/>
       <c r="I291" s="17"/>
     </row>
-    <row r="292" spans="1:9" ht="15.75">
+    <row r="292" spans="1:9" ht="15.6">
       <c r="A292" s="17" t="b">
         <v>0</v>
       </c>
@@ -18205,7 +18205,7 @@
       <c r="H292" s="17"/>
       <c r="I292" s="17"/>
     </row>
-    <row r="293" spans="1:9" ht="15.75">
+    <row r="293" spans="1:9" ht="15.6">
       <c r="A293" s="17"/>
       <c r="B293" s="17" t="s">
         <v>21</v>
@@ -18226,7 +18226,7 @@
       <c r="H293" s="17"/>
       <c r="I293" s="17"/>
     </row>
-    <row r="294" spans="1:9" ht="15.75">
+    <row r="294" spans="1:9" ht="15.6">
       <c r="A294" s="17" t="b">
         <v>0</v>
       </c>
@@ -18245,7 +18245,7 @@
       <c r="H294" s="17"/>
       <c r="I294" s="17"/>
     </row>
-    <row r="295" spans="1:9" ht="15.75">
+    <row r="295" spans="1:9" ht="15.6">
       <c r="A295" s="17"/>
       <c r="B295" s="17" t="s">
         <v>21</v>
@@ -18266,7 +18266,7 @@
       <c r="H295" s="17"/>
       <c r="I295" s="17"/>
     </row>
-    <row r="296" spans="1:9" ht="15.75">
+    <row r="296" spans="1:9" ht="15.6">
       <c r="A296" s="17" t="b">
         <v>0</v>
       </c>
@@ -18285,7 +18285,7 @@
       <c r="H296" s="17"/>
       <c r="I296" s="17"/>
     </row>
-    <row r="297" spans="1:9" ht="15.75">
+    <row r="297" spans="1:9" ht="15.6">
       <c r="A297" s="17"/>
       <c r="B297" s="17" t="s">
         <v>21</v>
@@ -18308,7 +18308,7 @@
       </c>
       <c r="I297" s="17"/>
     </row>
-    <row r="298" spans="1:9" ht="15.75">
+    <row r="298" spans="1:9" ht="15.6">
       <c r="A298" s="17" t="b">
         <v>0</v>
       </c>
@@ -18327,7 +18327,7 @@
       <c r="H298" s="17"/>
       <c r="I298" s="17"/>
     </row>
-    <row r="299" spans="1:9" ht="15.75">
+    <row r="299" spans="1:9" ht="15.6">
       <c r="A299" s="17"/>
       <c r="B299" s="17" t="s">
         <v>21</v>
@@ -18352,7 +18352,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15.75">
+    <row r="300" spans="1:9" ht="15.6">
       <c r="A300" s="17"/>
       <c r="B300" s="17" t="s">
         <v>21</v>
@@ -18375,7 +18375,7 @@
       </c>
       <c r="I300" s="17"/>
     </row>
-    <row r="301" spans="1:9" ht="15.75">
+    <row r="301" spans="1:9" ht="15.6">
       <c r="A301" s="17"/>
       <c r="B301" s="17" t="s">
         <v>21</v>
@@ -18398,7 +18398,7 @@
       </c>
       <c r="I301" s="17"/>
     </row>
-    <row r="302" spans="1:9" ht="15.75">
+    <row r="302" spans="1:9" ht="15.6">
       <c r="A302" s="17"/>
       <c r="B302" s="17" t="s">
         <v>21</v>
@@ -18421,7 +18421,7 @@
       </c>
       <c r="I302" s="17"/>
     </row>
-    <row r="303" spans="1:9" ht="15.75">
+    <row r="303" spans="1:9" ht="15.6">
       <c r="A303" s="17"/>
       <c r="B303" s="17" t="s">
         <v>21</v>
@@ -18444,7 +18444,7 @@
       </c>
       <c r="I303" s="17"/>
     </row>
-    <row r="304" spans="1:9" ht="15.75">
+    <row r="304" spans="1:9" ht="15.6">
       <c r="A304" s="17"/>
       <c r="B304" s="17" t="s">
         <v>21</v>
@@ -18467,7 +18467,7 @@
       </c>
       <c r="I304" s="17"/>
     </row>
-    <row r="305" spans="1:9" ht="15.75">
+    <row r="305" spans="1:9" ht="15.6">
       <c r="A305" s="17"/>
       <c r="B305" s="17" t="s">
         <v>21</v>
@@ -18490,7 +18490,7 @@
       </c>
       <c r="I305" s="17"/>
     </row>
-    <row r="306" spans="1:9" ht="15.75">
+    <row r="306" spans="1:9" ht="15.6">
       <c r="A306" s="17"/>
       <c r="B306" s="17" t="s">
         <v>21</v>
@@ -18513,7 +18513,7 @@
       </c>
       <c r="I306" s="17"/>
     </row>
-    <row r="307" spans="1:9" ht="15.75">
+    <row r="307" spans="1:9" ht="15.6">
       <c r="A307" s="17"/>
       <c r="B307" s="17" t="s">
         <v>21</v>
@@ -18536,7 +18536,7 @@
       </c>
       <c r="I307" s="17"/>
     </row>
-    <row r="308" spans="1:9" ht="15.75">
+    <row r="308" spans="1:9" ht="15.6">
       <c r="A308" s="17" t="b">
         <v>0</v>
       </c>
@@ -18555,7 +18555,7 @@
       <c r="H308" s="17"/>
       <c r="I308" s="17"/>
     </row>
-    <row r="309" spans="1:9" ht="15.75">
+    <row r="309" spans="1:9" ht="15.6">
       <c r="A309" s="17"/>
       <c r="B309" s="17" t="s">
         <v>21</v>
@@ -18578,7 +18578,7 @@
       </c>
       <c r="I309" s="17"/>
     </row>
-    <row r="310" spans="1:9" ht="15.75">
+    <row r="310" spans="1:9" ht="15.6">
       <c r="A310" s="17"/>
       <c r="B310" s="17" t="s">
         <v>21</v>
@@ -18601,7 +18601,7 @@
       </c>
       <c r="I310" s="17"/>
     </row>
-    <row r="311" spans="1:9" ht="15.75">
+    <row r="311" spans="1:9" ht="15.6">
       <c r="A311" s="17"/>
       <c r="B311" s="17" t="s">
         <v>21</v>
@@ -18624,7 +18624,7 @@
       </c>
       <c r="I311" s="17"/>
     </row>
-    <row r="312" spans="1:9" ht="15.75">
+    <row r="312" spans="1:9" ht="15.6">
       <c r="A312" s="17"/>
       <c r="B312" s="17" t="s">
         <v>21</v>
@@ -18647,7 +18647,7 @@
       </c>
       <c r="I312" s="17"/>
     </row>
-    <row r="313" spans="1:9" ht="15.75">
+    <row r="313" spans="1:9" ht="15.6">
       <c r="A313" s="17" t="b">
         <v>0</v>
       </c>
@@ -18666,7 +18666,7 @@
       <c r="H313" s="17"/>
       <c r="I313" s="17"/>
     </row>
-    <row r="314" spans="1:9" ht="15.75">
+    <row r="314" spans="1:9" ht="15.6">
       <c r="A314" s="17"/>
       <c r="B314" s="17" t="s">
         <v>21</v>
@@ -18689,7 +18689,7 @@
       </c>
       <c r="I314" s="17"/>
     </row>
-    <row r="315" spans="1:9" ht="15.75">
+    <row r="315" spans="1:9" ht="15.6">
       <c r="A315" s="17"/>
       <c r="B315" s="17" t="s">
         <v>21</v>
@@ -18712,7 +18712,7 @@
       </c>
       <c r="I315" s="17"/>
     </row>
-    <row r="316" spans="1:9" ht="15.75">
+    <row r="316" spans="1:9" ht="15.6">
       <c r="A316" s="17"/>
       <c r="B316" s="17" t="s">
         <v>21</v>
@@ -18737,7 +18737,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15.75">
+    <row r="317" spans="1:9" ht="15.6">
       <c r="A317" s="17" t="b">
         <v>0</v>
       </c>
@@ -18756,7 +18756,7 @@
       <c r="H317" s="17"/>
       <c r="I317" s="17"/>
     </row>
-    <row r="318" spans="1:9" ht="15.75">
+    <row r="318" spans="1:9" ht="15.6">
       <c r="A318" s="17"/>
       <c r="B318" s="17" t="s">
         <v>21</v>
@@ -18781,7 +18781,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15.75">
+    <row r="319" spans="1:9" ht="15.6">
       <c r="A319" s="17"/>
       <c r="B319" s="17" t="s">
         <v>21</v>
@@ -18804,7 +18804,7 @@
       </c>
       <c r="I319" s="17"/>
     </row>
-    <row r="320" spans="1:9" ht="15.75">
+    <row r="320" spans="1:9" ht="15.6">
       <c r="A320" s="17" t="b">
         <v>0</v>
       </c>
@@ -18823,7 +18823,7 @@
       <c r="H320" s="17"/>
       <c r="I320" s="17"/>
     </row>
-    <row r="321" spans="1:9" ht="15.75">
+    <row r="321" spans="1:9" ht="15.6">
       <c r="A321" s="17"/>
       <c r="B321" s="17" t="s">
         <v>21</v>
@@ -18844,7 +18844,7 @@
       <c r="H321" s="17"/>
       <c r="I321" s="17"/>
     </row>
-    <row r="322" spans="1:9" ht="15.75">
+    <row r="322" spans="1:9" ht="15.6">
       <c r="A322" s="17"/>
       <c r="B322" s="17" t="s">
         <v>21</v>
@@ -18865,7 +18865,7 @@
       <c r="H322" s="17"/>
       <c r="I322" s="17"/>
     </row>
-    <row r="323" spans="1:9" ht="15.75">
+    <row r="323" spans="1:9" ht="15.6">
       <c r="A323" s="17"/>
       <c r="B323" s="17" t="s">
         <v>21</v>
@@ -18888,7 +18888,7 @@
       </c>
       <c r="I323" s="17"/>
     </row>
-    <row r="324" spans="1:9" ht="15.75">
+    <row r="324" spans="1:9" ht="15.6">
       <c r="A324" s="17" t="b">
         <v>0</v>
       </c>
@@ -18907,7 +18907,7 @@
       <c r="H324" s="17"/>
       <c r="I324" s="17"/>
     </row>
-    <row r="325" spans="1:9" ht="15.75">
+    <row r="325" spans="1:9" ht="15.6">
       <c r="A325" s="17" t="b">
         <v>0</v>
       </c>
@@ -18926,7 +18926,7 @@
       <c r="H325" s="17"/>
       <c r="I325" s="17"/>
     </row>
-    <row r="326" spans="1:9" ht="15.75">
+    <row r="326" spans="1:9" ht="15.6">
       <c r="A326" s="17"/>
       <c r="B326" s="17" t="s">
         <v>21</v>
@@ -18951,7 +18951,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15.75">
+    <row r="327" spans="1:9" ht="15.6">
       <c r="A327" s="17"/>
       <c r="B327" s="17" t="s">
         <v>21</v>
@@ -19308,7 +19308,7 @@
       <c r="O343" s="1"/>
       <c r="P343" s="1"/>
     </row>
-    <row r="344" spans="1:16" ht="15.75">
+    <row r="344" spans="1:16" ht="15.6">
       <c r="A344" s="17"/>
       <c r="B344" t="s">
         <v>21</v>
@@ -19671,7 +19671,7 @@
       <c r="J361"/>
       <c r="K361"/>
     </row>
-    <row r="362" spans="1:18" s="1" customFormat="1" ht="15.75">
+    <row r="362" spans="1:18" s="1" customFormat="1" ht="15.6">
       <c r="A362" s="17"/>
       <c r="B362" t="s">
         <v>22</v>
@@ -19799,14 +19799,14 @@
       <selection activeCell="A17" sqref="A17:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="17" max="17" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">

</xml_diff>